<commit_message>
Updated the course spreadsheet
Lots of TODO …
</commit_message>
<xml_diff>
--- a/fl_course_outline_weeks.xlsx
+++ b/fl_course_outline_weeks.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27022"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27127"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14880" tabRatio="500"/>
+    <workbookView xWindow="4820" yWindow="200" windowWidth="32780" windowHeight="26860" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="365">
   <si>
     <t>Week</t>
   </si>
@@ -354,9 +354,6 @@
     <t>summarise content and preview week 3</t>
   </si>
   <si>
-    <t>Week 3: data structures and algorithms</t>
-  </si>
-  <si>
     <t>goal: explore a wider range of data structures and data processing</t>
   </si>
   <si>
@@ -762,9 +759,6 @@
     <t>5.12</t>
   </si>
   <si>
-    <t>5.13</t>
-  </si>
-  <si>
     <t>Video: welcome to week 5</t>
   </si>
   <si>
@@ -999,21 +993,12 @@
     <t>ditto - get some experience with evaluation</t>
   </si>
   <si>
-    <t>Video: Beginner's guide to monads</t>
-  </si>
-  <si>
-    <t>simple intro to complex subject - monads are a theoretical concept underlying sequence and effects in Haskell</t>
-  </si>
-  <si>
     <t>get an intuitive grasp of 'what Monads are for'</t>
   </si>
   <si>
     <t>monads are the essence of Haskell interaction with the real-world</t>
   </si>
   <si>
-    <t>Article: We already know about monads</t>
-  </si>
-  <si>
     <t>show where we have covered monadic operations throughout the course, in various weeks</t>
   </si>
   <si>
@@ -1096,13 +1081,52 @@
   </si>
   <si>
     <t>Video: welcome to week 4</t>
+  </si>
+  <si>
+    <t>in progress</t>
+  </si>
+  <si>
+    <t>todo</t>
+  </si>
+  <si>
+    <t>Week 3: Data Structures. Computations and Types</t>
+  </si>
+  <si>
+    <t>Video:  We already know about monads</t>
+  </si>
+  <si>
+    <t>6.13</t>
+  </si>
+  <si>
+    <t>Article: Example: The Maybe Monad</t>
+  </si>
+  <si>
+    <t>Article: Monad Theory</t>
+  </si>
+  <si>
+    <t>intro to complex subject - monads are a theoretical concept underlying sequence and effects in Haskell</t>
+  </si>
+  <si>
+    <t>A practical example demonstrating how to create and use a monad</t>
+  </si>
+  <si>
+    <t>WHO?</t>
+  </si>
+  <si>
+    <t>JW</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>J</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1154,8 +1178,28 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1171,6 +1215,28 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1244,7 +1310,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="150">
+  <cellStyleXfs count="286">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1395,8 +1461,144 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1444,8 +1646,32 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="151" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="150" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="150">
+  <cellStyles count="286">
+    <cellStyle name="Bad" xfId="150" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1520,6 +1746,73 @@
     <cellStyle name="Followed Hyperlink" xfId="145" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="147" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="149" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="153" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="155" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="157" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="159" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="161" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="163" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="165" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="167" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="169" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="171" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="173" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="175" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="177" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="179" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="181" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="183" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="185" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="187" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="189" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="191" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="193" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="195" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="197" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="199" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="201" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="203" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="205" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="207" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="209" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="211" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="213" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="215" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="217" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="219" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="221" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="223" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="225" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="227" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="229" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="231" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="233" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="235" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="237" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="239" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="241" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="243" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="245" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="247" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="249" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="251" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="253" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="255" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="257" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="259" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="261" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="263" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="265" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="267" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="269" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="271" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="273" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="275" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="277" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="279" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="281" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="283" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="285" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="55" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -1595,6 +1888,74 @@
     <cellStyle name="Hyperlink" xfId="144" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="146" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="148" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="152" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="154" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="156" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="158" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="160" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="162" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="164" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="166" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="168" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="170" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="172" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="174" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="176" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="178" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="180" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="182" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="184" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="186" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="188" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="190" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="192" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="194" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="196" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="198" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="200" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="202" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="204" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="206" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="208" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="210" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="212" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="214" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="216" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="218" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="220" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="222" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="224" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="226" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="228" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="230" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="232" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="234" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="236" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="238" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="240" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="242" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="244" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="246" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="248" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="250" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="252" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="254" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="256" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="258" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="260" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="262" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="264" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="266" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="268" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="270" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="272" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="274" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="276" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="278" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="280" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="282" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="284" builtinId="8" hidden="1"/>
+    <cellStyle name="Neutral" xfId="151" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1862,7 +2223,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1870,27 +2231,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J999"/>
+  <dimension ref="A1:K1004"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A73" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="I13" sqref="I13"/>
+      <selection pane="bottomLeft" activeCell="K90" sqref="K90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="43.6640625" customWidth="1"/>
+    <col min="1" max="1" width="26.5" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
     <col min="3" max="3" width="7.6640625" customWidth="1"/>
     <col min="4" max="4" width="33.6640625" customWidth="1"/>
     <col min="5" max="5" width="38.6640625" customWidth="1"/>
-    <col min="6" max="6" width="39.83203125" customWidth="1"/>
-    <col min="7" max="7" width="33.6640625" customWidth="1"/>
-    <col min="8" max="8" width="42.5" customWidth="1"/>
+    <col min="6" max="6" width="39.83203125" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="33.6640625" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="42.5" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="89" customHeight="1">
+    <row r="1" spans="1:11" ht="89" customHeight="1">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -1921,8 +2282,11 @@
       <c r="J1" s="12" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="49" customHeight="1">
+      <c r="K1" s="12" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="49" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -1932,7 +2296,7 @@
       <c r="C2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="25" t="s">
         <v>14</v>
       </c>
       <c r="E2" s="3" t="s">
@@ -1945,8 +2309,14 @@
         <v>43</v>
       </c>
       <c r="H2" s="3"/>
-    </row>
-    <row r="3" spans="1:10" ht="15.75" customHeight="1">
+      <c r="I2" s="22" t="s">
+        <v>353</v>
+      </c>
+      <c r="K2" s="16" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="15.75" customHeight="1">
       <c r="A3" s="11" t="s">
         <v>56</v>
       </c>
@@ -1954,7 +2324,7 @@
       <c r="C3" s="6">
         <v>1.2</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="25" t="s">
         <v>16</v>
       </c>
       <c r="E3" s="3" t="s">
@@ -1967,11 +2337,17 @@
         <v>43</v>
       </c>
       <c r="H3" s="3"/>
+      <c r="I3" s="22" t="s">
+        <v>353</v>
+      </c>
       <c r="J3" s="16" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="15.75" customHeight="1">
+        <v>343</v>
+      </c>
+      <c r="K3" s="16" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15.75" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -1993,13 +2369,16 @@
       </c>
       <c r="H4" s="3"/>
       <c r="I4" s="17" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="J4" s="16" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="15.75" customHeight="1">
+        <v>343</v>
+      </c>
+      <c r="K4" s="16" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="15.75" customHeight="1">
       <c r="A5" s="18" t="s">
         <v>12</v>
       </c>
@@ -2021,13 +2400,16 @@
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="17" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="J5" s="16" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="15.75" customHeight="1">
+        <v>344</v>
+      </c>
+      <c r="K5" s="16" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="15.75" customHeight="1">
       <c r="A6" s="19"/>
       <c r="B6" s="5"/>
       <c r="C6" s="7">
@@ -2047,13 +2429,16 @@
       </c>
       <c r="H6" s="3"/>
       <c r="I6" s="17" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="J6" s="16" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="15.75" customHeight="1">
+        <v>344</v>
+      </c>
+      <c r="K6" s="16" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="15.75" customHeight="1">
       <c r="A7" s="20"/>
       <c r="B7" s="5" t="s">
         <v>19</v>
@@ -2074,11 +2459,17 @@
         <v>43</v>
       </c>
       <c r="H7" s="3"/>
+      <c r="I7" s="22" t="s">
+        <v>353</v>
+      </c>
       <c r="J7" s="16" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="15.75" customHeight="1">
+        <v>343</v>
+      </c>
+      <c r="K7" s="16" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15.75" customHeight="1">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="8" t="s">
@@ -2098,13 +2489,16 @@
       </c>
       <c r="H8" s="3"/>
       <c r="I8" s="17" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="J8" s="16" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="15.75" customHeight="1">
+        <v>343</v>
+      </c>
+      <c r="K8" s="16" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="15.75" customHeight="1">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="8" t="s">
@@ -2124,13 +2518,16 @@
       </c>
       <c r="H9" s="3"/>
       <c r="I9" s="17" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="J9" s="16" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="15.75" customHeight="1">
+        <v>344</v>
+      </c>
+      <c r="K9" s="16" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="15.75" customHeight="1">
       <c r="A10" s="3"/>
       <c r="B10" s="5"/>
       <c r="C10" s="8" t="s">
@@ -2150,13 +2547,16 @@
       </c>
       <c r="H10" s="3"/>
       <c r="I10" s="17" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="J10" s="16" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="15.75" customHeight="1">
+        <v>344</v>
+      </c>
+      <c r="K10" s="16" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="15.75" customHeight="1">
       <c r="A11" s="3"/>
       <c r="B11" s="3" t="s">
         <v>22</v>
@@ -2177,14 +2577,17 @@
         <v>53</v>
       </c>
       <c r="H11" s="3"/>
-      <c r="I11" s="17" t="s">
-        <v>354</v>
+      <c r="I11" s="23" t="s">
+        <v>352</v>
       </c>
       <c r="J11" s="16" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="15.75" customHeight="1">
+        <v>345</v>
+      </c>
+      <c r="K11" s="16" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="15.75" customHeight="1">
       <c r="A12" s="3"/>
       <c r="B12" s="5"/>
       <c r="C12" s="8" t="s">
@@ -2203,11 +2606,17 @@
         <v>54</v>
       </c>
       <c r="H12" s="3"/>
+      <c r="I12" s="21" t="s">
+        <v>352</v>
+      </c>
       <c r="J12" s="16" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="15.75" customHeight="1">
+        <v>346</v>
+      </c>
+      <c r="K12" s="16" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="15.75" customHeight="1">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="8" t="s">
@@ -2226,11 +2635,14 @@
         <v>45</v>
       </c>
       <c r="H13" s="3"/>
-      <c r="I13" s="17" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="15.75" customHeight="1">
+      <c r="I13" s="21" t="s">
+        <v>352</v>
+      </c>
+      <c r="K13" s="16" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="15.75" customHeight="1">
       <c r="A14" s="3"/>
       <c r="B14" s="5"/>
       <c r="C14" s="3"/>
@@ -2240,7 +2652,7 @@
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
     </row>
-    <row r="15" spans="1:10" ht="15.75" customHeight="1">
+    <row r="15" spans="1:11" ht="15.75" customHeight="1">
       <c r="A15" s="3"/>
       <c r="B15" s="5"/>
       <c r="C15" s="9"/>
@@ -2250,7 +2662,7 @@
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
     </row>
-    <row r="16" spans="1:10" ht="15.75" customHeight="1">
+    <row r="16" spans="1:11" ht="15.75" customHeight="1">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="9"/>
@@ -2260,7 +2672,7 @@
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
     </row>
-    <row r="17" spans="1:10" ht="15.75" customHeight="1">
+    <row r="17" spans="1:11" ht="15.75" customHeight="1">
       <c r="A17" s="3"/>
       <c r="B17" s="5"/>
       <c r="C17" s="3"/>
@@ -2270,7 +2682,7 @@
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
     </row>
-    <row r="18" spans="1:10" ht="15.75" customHeight="1">
+    <row r="18" spans="1:11" ht="15.75" customHeight="1">
       <c r="A18" s="11" t="s">
         <v>57</v>
       </c>
@@ -2294,10 +2706,13 @@
       </c>
       <c r="H18" s="3"/>
       <c r="I18" s="17" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="15.75" customHeight="1">
+        <v>349</v>
+      </c>
+      <c r="K18" s="16" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="15.75" customHeight="1">
       <c r="A19" s="3" t="s">
         <v>58</v>
       </c>
@@ -2319,13 +2734,16 @@
       </c>
       <c r="H19" s="3"/>
       <c r="I19" s="17" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="J19" s="16" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="15.75" customHeight="1">
+        <v>343</v>
+      </c>
+      <c r="K19" s="16" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="15.75" customHeight="1">
       <c r="A20" s="3" t="s">
         <v>59</v>
       </c>
@@ -2347,13 +2765,16 @@
       </c>
       <c r="H20" s="3"/>
       <c r="I20" s="17" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="J20" s="16" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="15.75" customHeight="1">
+        <v>343</v>
+      </c>
+      <c r="K20" s="16" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="15.75" customHeight="1">
       <c r="A21" s="3"/>
       <c r="B21" s="5"/>
       <c r="C21" s="8" t="s">
@@ -2373,13 +2794,16 @@
       </c>
       <c r="H21" s="3"/>
       <c r="I21" s="17" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="J21" s="16" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="15.75" customHeight="1">
+        <v>344</v>
+      </c>
+      <c r="K21" s="16" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="15.75" customHeight="1">
       <c r="A22" s="3"/>
       <c r="B22" s="5"/>
       <c r="C22" s="8" t="s">
@@ -2399,13 +2823,16 @@
       </c>
       <c r="H22" s="3"/>
       <c r="I22" s="17" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="J22" s="16" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="15.75" customHeight="1">
+        <v>344</v>
+      </c>
+      <c r="K22" s="16" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="15.75" customHeight="1">
       <c r="A23" s="3"/>
       <c r="B23" s="5" t="s">
         <v>88</v>
@@ -2413,7 +2840,7 @@
       <c r="C23" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="26" t="s">
         <v>90</v>
       </c>
       <c r="E23" s="3" t="s">
@@ -2422,11 +2849,17 @@
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
+      <c r="I23" s="22" t="s">
+        <v>353</v>
+      </c>
       <c r="J23" s="16" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="15.75" customHeight="1">
+        <v>343</v>
+      </c>
+      <c r="K23" s="16" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="15.75" customHeight="1">
       <c r="A24" s="3"/>
       <c r="B24" s="5"/>
       <c r="C24" s="8" t="s">
@@ -2442,13 +2875,16 @@
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
       <c r="I24" s="17" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="J24" s="16" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="15.75" customHeight="1">
+        <v>344</v>
+      </c>
+      <c r="K24" s="16" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="15.75" customHeight="1">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="8" t="s">
@@ -2463,11 +2899,17 @@
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
+      <c r="I25" s="22" t="s">
+        <v>353</v>
+      </c>
       <c r="J25" s="16" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="15.75" customHeight="1">
+        <v>343</v>
+      </c>
+      <c r="K25" s="16" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="15.75" customHeight="1">
       <c r="A26" s="5"/>
       <c r="B26" s="5" t="s">
         <v>96</v>
@@ -2484,32 +2926,44 @@
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
+      <c r="I26" s="22" t="s">
+        <v>353</v>
+      </c>
       <c r="J26" s="16" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="15.75" customHeight="1">
+        <v>344</v>
+      </c>
+      <c r="K26" s="16" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="15.75" customHeight="1">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D27" s="26" t="s">
         <v>101</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>102</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
+      <c r="I27" s="22" t="s">
+        <v>353</v>
+      </c>
       <c r="J27" s="16" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="15.75" customHeight="1">
+        <v>343</v>
+      </c>
+      <c r="K27" s="16" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="15.75" customHeight="1">
       <c r="C28" s="8" t="s">
         <v>70</v>
       </c>
@@ -2519,11 +2973,17 @@
       <c r="E28" s="13" t="s">
         <v>104</v>
       </c>
+      <c r="I28" s="22" t="s">
+        <v>353</v>
+      </c>
       <c r="J28" s="16" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="15.75" customHeight="1">
+        <v>347</v>
+      </c>
+      <c r="K28" s="16" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="15.75" customHeight="1">
       <c r="C29" s="8" t="s">
         <v>99</v>
       </c>
@@ -2536,11 +2996,17 @@
       <c r="F29" s="14" t="s">
         <v>106</v>
       </c>
+      <c r="I29" s="22" t="s">
+        <v>353</v>
+      </c>
       <c r="J29" s="16" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="15.75" customHeight="1">
+        <v>344</v>
+      </c>
+      <c r="K29" s="16" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="15.75" customHeight="1">
       <c r="C30" s="8" t="s">
         <v>100</v>
       </c>
@@ -2554,27 +3020,30 @@
         <v>44</v>
       </c>
       <c r="I30" s="17" t="s">
+        <v>349</v>
+      </c>
+      <c r="K30" s="16" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="15.75" customHeight="1">
+      <c r="C31" s="8"/>
+    </row>
+    <row r="32" spans="1:11" ht="15.75" customHeight="1">
+      <c r="C32" s="1"/>
+    </row>
+    <row r="33" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A33" s="11" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" ht="15.75" customHeight="1">
-      <c r="C31" s="8"/>
-    </row>
-    <row r="32" spans="1:10" ht="15.75" customHeight="1">
-      <c r="C32" s="1"/>
-    </row>
-    <row r="33" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A33" s="11" t="s">
-        <v>109</v>
-      </c>
       <c r="B33" t="s">
+        <v>111</v>
+      </c>
+      <c r="C33" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="C33" s="8" t="s">
-        <v>113</v>
-      </c>
       <c r="D33" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E33" t="s">
         <v>72</v>
@@ -2583,288 +3052,354 @@
         <v>44</v>
       </c>
       <c r="G33" t="s">
+        <v>164</v>
+      </c>
+      <c r="I33" s="17" t="s">
+        <v>349</v>
+      </c>
+      <c r="K33" s="28" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A34" t="s">
+        <v>109</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="D34" t="s">
+        <v>126</v>
+      </c>
+      <c r="E34" t="s">
+        <v>127</v>
+      </c>
+      <c r="F34" t="s">
+        <v>155</v>
+      </c>
+      <c r="G34" t="s">
         <v>165</v>
       </c>
-      <c r="I33" s="17" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A34" t="s">
+      <c r="I34" s="22" t="s">
+        <v>353</v>
+      </c>
+      <c r="J34" s="16" t="s">
+        <v>344</v>
+      </c>
+      <c r="K34" s="28" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A35" t="s">
         <v>110</v>
       </c>
-      <c r="C34" s="8" t="s">
+      <c r="C35" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="D34" t="s">
-        <v>127</v>
-      </c>
-      <c r="E34" t="s">
+      <c r="D35" t="s">
         <v>128</v>
       </c>
-      <c r="F34" t="s">
+      <c r="E35" t="s">
+        <v>129</v>
+      </c>
+      <c r="F35" t="s">
         <v>156</v>
       </c>
-      <c r="G34" t="s">
+      <c r="G35" t="s">
         <v>166</v>
       </c>
-      <c r="J34" s="16" t="s">
+      <c r="I35" s="17" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A35" t="s">
-        <v>111</v>
-      </c>
-      <c r="C35" s="8" t="s">
+      <c r="J35" s="16" t="s">
+        <v>343</v>
+      </c>
+      <c r="K35" s="28" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="15.75" customHeight="1">
+      <c r="C36" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="D35" t="s">
-        <v>129</v>
-      </c>
-      <c r="E35" t="s">
+      <c r="D36" t="s">
         <v>130</v>
       </c>
-      <c r="F35" t="s">
-        <v>157</v>
-      </c>
-      <c r="G35" t="s">
+      <c r="E36" t="s">
+        <v>131</v>
+      </c>
+      <c r="F36" t="s">
+        <v>154</v>
+      </c>
+      <c r="G36" t="s">
         <v>167</v>
       </c>
-      <c r="I35" s="17" t="s">
-        <v>354</v>
-      </c>
-      <c r="J35" s="16" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" ht="15.75" customHeight="1">
-      <c r="C36" s="8" t="s">
+      <c r="I36" s="22" t="s">
+        <v>353</v>
+      </c>
+      <c r="J36" s="16" t="s">
+        <v>344</v>
+      </c>
+      <c r="K36" s="28" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="15.75" customHeight="1">
+      <c r="C37" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="D36" t="s">
-        <v>131</v>
-      </c>
-      <c r="E36" t="s">
+      <c r="D37" s="27" t="s">
         <v>132</v>
       </c>
-      <c r="F36" t="s">
-        <v>155</v>
-      </c>
-      <c r="G36" t="s">
+      <c r="E37" t="s">
+        <v>133</v>
+      </c>
+      <c r="F37" t="s">
+        <v>153</v>
+      </c>
+      <c r="G37" t="s">
         <v>168</v>
       </c>
-      <c r="J36" s="16" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" ht="15.75" customHeight="1">
-      <c r="C37" s="8" t="s">
+      <c r="I37" s="22" t="s">
+        <v>353</v>
+      </c>
+      <c r="J37" s="16" t="s">
+        <v>343</v>
+      </c>
+      <c r="K37" s="28" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="15.75" customHeight="1">
+      <c r="C38" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="D37" t="s">
-        <v>133</v>
-      </c>
-      <c r="E37" t="s">
+      <c r="D38" t="s">
         <v>134</v>
       </c>
-      <c r="F37" t="s">
-        <v>154</v>
-      </c>
-      <c r="G37" t="s">
-        <v>169</v>
-      </c>
-      <c r="J37" s="16" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" ht="15.75" customHeight="1">
-      <c r="C38" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="D38" t="s">
+      <c r="E38" t="s">
         <v>135</v>
       </c>
-      <c r="E38" t="s">
-        <v>136</v>
-      </c>
       <c r="F38" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G38" s="3" t="s">
         <v>55</v>
       </c>
+      <c r="I38" s="22" t="s">
+        <v>353</v>
+      </c>
       <c r="J38" s="16" t="s">
+        <v>344</v>
+      </c>
+      <c r="K38" s="28" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="15.75" customHeight="1">
+      <c r="B39" t="s">
+        <v>136</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="D39" s="27" t="s">
+        <v>137</v>
+      </c>
+      <c r="E39" t="s">
+        <v>138</v>
+      </c>
+      <c r="F39" t="s">
+        <v>139</v>
+      </c>
+      <c r="G39" t="s">
+        <v>169</v>
+      </c>
+      <c r="I39" s="22" t="s">
+        <v>353</v>
+      </c>
+      <c r="J39" s="16" t="s">
+        <v>343</v>
+      </c>
+      <c r="K39" s="28" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="15.75" customHeight="1">
+      <c r="C40" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="D40" t="s">
+        <v>140</v>
+      </c>
+      <c r="E40" t="s">
+        <v>141</v>
+      </c>
+      <c r="F40" t="s">
+        <v>151</v>
+      </c>
+      <c r="G40" t="s">
+        <v>170</v>
+      </c>
+      <c r="I40" s="17" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" ht="15.75" customHeight="1">
-      <c r="B39" t="s">
-        <v>137</v>
-      </c>
-      <c r="C39" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="D39" t="s">
-        <v>138</v>
-      </c>
-      <c r="E39" t="s">
-        <v>139</v>
-      </c>
-      <c r="F39" t="s">
-        <v>140</v>
-      </c>
-      <c r="G39" t="s">
-        <v>170</v>
-      </c>
-      <c r="J39" s="16" t="s">
+      <c r="J40" s="16" t="s">
+        <v>347</v>
+      </c>
+      <c r="K40" s="28" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="15.75" customHeight="1">
+      <c r="C41" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="D41" s="27" t="s">
+        <v>142</v>
+      </c>
+      <c r="E41" t="s">
+        <v>143</v>
+      </c>
+      <c r="F41" t="s">
+        <v>150</v>
+      </c>
+      <c r="G41" t="s">
+        <v>171</v>
+      </c>
+      <c r="I41" s="22" t="s">
+        <v>353</v>
+      </c>
+      <c r="J41" s="16" t="s">
+        <v>343</v>
+      </c>
+      <c r="K41" s="28" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="15.75" customHeight="1">
+      <c r="C42" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="D42" t="s">
+        <v>144</v>
+      </c>
+      <c r="E42" t="s">
+        <v>145</v>
+      </c>
+      <c r="F42" t="s">
+        <v>149</v>
+      </c>
+      <c r="G42" t="s">
+        <v>172</v>
+      </c>
+      <c r="I42" s="22" t="s">
+        <v>353</v>
+      </c>
+      <c r="J42" s="16" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" ht="15.75" customHeight="1">
-      <c r="C40" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="D40" t="s">
-        <v>141</v>
-      </c>
-      <c r="E40" t="s">
-        <v>142</v>
-      </c>
-      <c r="F40" t="s">
-        <v>152</v>
-      </c>
-      <c r="G40" t="s">
-        <v>171</v>
-      </c>
-      <c r="I40" s="17" t="s">
-        <v>354</v>
-      </c>
-      <c r="J40" s="16" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" ht="15.75" customHeight="1">
-      <c r="C41" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="D41" t="s">
-        <v>143</v>
-      </c>
-      <c r="E41" t="s">
-        <v>144</v>
-      </c>
-      <c r="F41" t="s">
-        <v>151</v>
-      </c>
-      <c r="G41" t="s">
-        <v>172</v>
-      </c>
-      <c r="J41" s="16" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" ht="15.75" customHeight="1">
-      <c r="C42" s="8" t="s">
+      <c r="K42" s="28" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="15.75" customHeight="1">
+      <c r="B43" t="s">
+        <v>157</v>
+      </c>
+      <c r="C43" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="D42" t="s">
-        <v>145</v>
-      </c>
-      <c r="E42" t="s">
-        <v>146</v>
-      </c>
-      <c r="F42" t="s">
-        <v>150</v>
-      </c>
-      <c r="G42" t="s">
-        <v>173</v>
-      </c>
-      <c r="J42" s="16" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" ht="15.75" customHeight="1">
-      <c r="B43" t="s">
+      <c r="D43" s="27" t="s">
         <v>158</v>
       </c>
-      <c r="C43" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="D43" t="s">
+      <c r="E43" s="13" t="s">
         <v>159</v>
-      </c>
-      <c r="E43" s="13" t="s">
-        <v>160</v>
       </c>
       <c r="F43" t="s">
         <v>44</v>
       </c>
       <c r="G43" t="s">
-        <v>174</v>
+        <v>173</v>
+      </c>
+      <c r="I43" s="22" t="s">
+        <v>353</v>
       </c>
       <c r="J43" s="16" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" ht="15.75" customHeight="1">
+        <v>345</v>
+      </c>
+      <c r="K43" s="28" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="15.75" customHeight="1">
       <c r="C44" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="D44" t="s">
+        <v>160</v>
+      </c>
+      <c r="E44" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="F44" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="G44" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="I44" s="22" t="s">
+        <v>353</v>
+      </c>
+      <c r="J44" s="16" t="s">
+        <v>345</v>
+      </c>
+      <c r="K44" s="28" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="15.75" customHeight="1">
+      <c r="C45" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="D44" t="s">
-        <v>161</v>
-      </c>
-      <c r="E44" s="14" t="s">
-        <v>162</v>
-      </c>
-      <c r="F44" s="14" t="s">
-        <v>163</v>
-      </c>
-      <c r="G44" s="14" t="s">
-        <v>164</v>
-      </c>
-      <c r="J44" s="16" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" ht="15.75" customHeight="1">
-      <c r="C45" s="8" t="s">
-        <v>125</v>
-      </c>
       <c r="D45" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E45" s="13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F45" t="s">
         <v>44</v>
       </c>
       <c r="G45" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I45" s="17" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" ht="15.75" customHeight="1">
+        <v>349</v>
+      </c>
+      <c r="K45" s="28" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" ht="15.75" customHeight="1">
       <c r="C46" s="1"/>
     </row>
-    <row r="47" spans="1:10" ht="12">
+    <row r="47" spans="1:11" ht="12">
       <c r="C47" s="1"/>
     </row>
-    <row r="48" spans="1:10" ht="12">
+    <row r="48" spans="1:11" ht="25">
       <c r="A48" s="11" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B48" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D48" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="E48" t="s">
         <v>72</v>
@@ -2873,239 +3408,305 @@
         <v>44</v>
       </c>
       <c r="G48" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" ht="12">
+        <v>164</v>
+      </c>
+      <c r="I48" s="21" t="s">
+        <v>352</v>
+      </c>
+      <c r="K48" s="29" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" ht="15">
       <c r="A49" t="s">
+        <v>185</v>
+      </c>
+      <c r="C49" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="D49" t="s">
+        <v>201</v>
+      </c>
+      <c r="E49" t="s">
+        <v>202</v>
+      </c>
+      <c r="F49" t="s">
+        <v>203</v>
+      </c>
+      <c r="G49" t="s">
+        <v>204</v>
+      </c>
+      <c r="I49" s="22" t="s">
+        <v>353</v>
+      </c>
+      <c r="J49" s="16" t="s">
+        <v>343</v>
+      </c>
+      <c r="K49" s="29" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" ht="15">
+      <c r="A50" t="s">
         <v>186</v>
       </c>
-      <c r="C49" s="8" t="s">
+      <c r="C50" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D50" t="s">
+        <v>205</v>
+      </c>
+      <c r="E50" t="s">
+        <v>206</v>
+      </c>
+      <c r="F50" t="s">
+        <v>203</v>
+      </c>
+      <c r="G50" t="s">
+        <v>207</v>
+      </c>
+      <c r="I50" s="22" t="s">
+        <v>353</v>
+      </c>
+      <c r="J50" s="16" t="s">
+        <v>343</v>
+      </c>
+      <c r="K50" s="29" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" ht="15">
+      <c r="C51" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="D51" s="27" t="s">
+        <v>208</v>
+      </c>
+      <c r="E51" t="s">
+        <v>209</v>
+      </c>
+      <c r="F51" t="s">
+        <v>210</v>
+      </c>
+      <c r="G51" t="s">
+        <v>211</v>
+      </c>
+      <c r="I51" s="22" t="s">
+        <v>353</v>
+      </c>
+      <c r="J51" s="16" t="s">
+        <v>343</v>
+      </c>
+      <c r="K51" s="29" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" ht="15">
+      <c r="C52" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="D52" t="s">
+        <v>212</v>
+      </c>
+      <c r="E52" t="s">
+        <v>213</v>
+      </c>
+      <c r="F52" t="s">
+        <v>214</v>
+      </c>
+      <c r="G52" t="s">
+        <v>215</v>
+      </c>
+      <c r="I52" s="22" t="s">
+        <v>353</v>
+      </c>
+      <c r="J52" t="s">
+        <v>344</v>
+      </c>
+      <c r="K52" s="29" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" ht="15">
+      <c r="B53" t="s">
+        <v>191</v>
+      </c>
+      <c r="C53" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="D53" t="s">
+        <v>187</v>
+      </c>
+      <c r="E53" t="s">
         <v>188</v>
       </c>
-      <c r="E49" t="s">
+      <c r="F53" t="s">
         <v>189</v>
       </c>
-      <c r="F49" t="s">
+      <c r="G53" t="s">
         <v>190</v>
       </c>
-      <c r="G49" t="s">
-        <v>191</v>
-      </c>
-      <c r="J49" s="16" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" ht="12">
-      <c r="A50" t="s">
-        <v>187</v>
-      </c>
-      <c r="C50" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="D50" t="s">
+      <c r="I53" s="17" t="s">
+        <v>349</v>
+      </c>
+      <c r="J53" s="16" t="s">
+        <v>343</v>
+      </c>
+      <c r="K53" s="29" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" ht="15">
+      <c r="C54" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="D54" s="27" t="s">
+        <v>192</v>
+      </c>
+      <c r="E54" t="s">
         <v>193</v>
       </c>
-      <c r="E50" t="s">
+      <c r="F54" t="s">
         <v>194</v>
       </c>
-      <c r="F50" t="s">
+      <c r="G54" t="s">
         <v>195</v>
       </c>
-      <c r="G50" t="s">
+      <c r="I54" s="22" t="s">
+        <v>353</v>
+      </c>
+      <c r="J54" s="16" t="s">
+        <v>343</v>
+      </c>
+      <c r="K54" s="29" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" ht="15">
+      <c r="C55" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="D55" t="s">
         <v>196</v>
       </c>
-      <c r="J50" s="16" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" ht="12">
-      <c r="C51" s="8" t="s">
-        <v>178</v>
-      </c>
-      <c r="D51" t="s">
+      <c r="E55" t="s">
         <v>197</v>
       </c>
-      <c r="E51" t="s">
+      <c r="F55" t="s">
         <v>198</v>
       </c>
-      <c r="F51" t="s">
+      <c r="G55" t="s">
         <v>199</v>
       </c>
-      <c r="G51" t="s">
-        <v>200</v>
-      </c>
-      <c r="J51" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" ht="12">
-      <c r="B52" t="s">
-        <v>201</v>
-      </c>
-      <c r="C52" s="8" t="s">
-        <v>179</v>
-      </c>
-      <c r="D52" t="s">
-        <v>202</v>
-      </c>
-      <c r="E52" t="s">
-        <v>203</v>
-      </c>
-      <c r="F52" t="s">
-        <v>204</v>
-      </c>
-      <c r="G52" t="s">
-        <v>205</v>
-      </c>
-      <c r="J52" s="16" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" ht="12">
-      <c r="C53" s="8" t="s">
-        <v>180</v>
-      </c>
-      <c r="D53" t="s">
-        <v>206</v>
-      </c>
-      <c r="E53" t="s">
-        <v>207</v>
-      </c>
-      <c r="F53" t="s">
-        <v>204</v>
-      </c>
-      <c r="G53" t="s">
-        <v>208</v>
-      </c>
-      <c r="J53" s="16" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" ht="12">
-      <c r="C54" s="8" t="s">
-        <v>181</v>
-      </c>
-      <c r="D54" t="s">
-        <v>209</v>
-      </c>
-      <c r="E54" t="s">
-        <v>210</v>
-      </c>
-      <c r="F54" t="s">
-        <v>211</v>
-      </c>
-      <c r="G54" t="s">
-        <v>212</v>
-      </c>
-      <c r="J54" s="16" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" ht="12">
-      <c r="C55" s="8" t="s">
+      <c r="I55" s="22" t="s">
+        <v>353</v>
+      </c>
+      <c r="J55" t="s">
+        <v>344</v>
+      </c>
+      <c r="K55" s="29" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" ht="15">
+      <c r="B56" t="s">
+        <v>216</v>
+      </c>
+      <c r="C56" s="8" t="s">
         <v>182</v>
       </c>
-      <c r="D55" t="s">
-        <v>213</v>
-      </c>
-      <c r="E55" t="s">
-        <v>214</v>
-      </c>
-      <c r="F55" t="s">
-        <v>215</v>
-      </c>
-      <c r="G55" t="s">
-        <v>216</v>
-      </c>
-      <c r="J55" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" ht="12">
-      <c r="B56" t="s">
+      <c r="D56" s="27" t="s">
         <v>217</v>
       </c>
-      <c r="C56" s="8" t="s">
+      <c r="E56" t="s">
+        <v>218</v>
+      </c>
+      <c r="F56" t="s">
+        <v>219</v>
+      </c>
+      <c r="G56" t="s">
+        <v>220</v>
+      </c>
+      <c r="I56" s="22" t="s">
+        <v>353</v>
+      </c>
+      <c r="J56" s="16" t="s">
+        <v>343</v>
+      </c>
+      <c r="K56" s="29" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" ht="15">
+      <c r="C57" s="8" t="s">
         <v>183</v>
       </c>
-      <c r="D56" t="s">
-        <v>218</v>
-      </c>
-      <c r="E56" t="s">
-        <v>219</v>
-      </c>
-      <c r="F56" t="s">
-        <v>220</v>
-      </c>
-      <c r="G56" t="s">
+      <c r="D57" t="s">
         <v>221</v>
       </c>
-      <c r="J56" s="16" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" ht="12">
-      <c r="C57" s="8" t="s">
-        <v>184</v>
-      </c>
-      <c r="D57" t="s">
+      <c r="E57" t="s">
+        <v>225</v>
+      </c>
+      <c r="F57" t="s">
+        <v>226</v>
+      </c>
+      <c r="G57" t="s">
+        <v>227</v>
+      </c>
+      <c r="I57" s="22" t="s">
+        <v>353</v>
+      </c>
+      <c r="J57" t="s">
+        <v>344</v>
+      </c>
+      <c r="K57" s="29" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" ht="15">
+      <c r="C58" s="8" t="s">
         <v>222</v>
       </c>
-      <c r="E57" t="s">
-        <v>226</v>
-      </c>
-      <c r="F57" t="s">
-        <v>227</v>
-      </c>
-      <c r="G57" t="s">
-        <v>228</v>
-      </c>
-      <c r="J57" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" ht="12">
-      <c r="C58" s="8" t="s">
+      <c r="D58" t="s">
         <v>223</v>
       </c>
-      <c r="D58" t="s">
+      <c r="E58" t="s">
         <v>224</v>
-      </c>
-      <c r="E58" t="s">
-        <v>225</v>
       </c>
       <c r="F58" t="s">
         <v>44</v>
       </c>
       <c r="G58" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" ht="12">
+        <v>164</v>
+      </c>
+      <c r="I58" s="21" t="s">
+        <v>352</v>
+      </c>
+      <c r="K58" s="29" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" ht="12">
       <c r="C59" s="1"/>
     </row>
-    <row r="60" spans="1:10" ht="12">
+    <row r="60" spans="1:11" ht="12">
       <c r="C60" s="1"/>
     </row>
-    <row r="61" spans="1:10" ht="12">
+    <row r="61" spans="1:11" ht="12">
       <c r="C61" s="1"/>
     </row>
-    <row r="62" spans="1:10" ht="12">
+    <row r="62" spans="1:11" ht="25">
       <c r="A62" s="15" t="s">
+        <v>228</v>
+      </c>
+      <c r="B62" s="24" t="s">
         <v>229</v>
       </c>
-      <c r="B62" t="s">
-        <v>230</v>
-      </c>
       <c r="C62" s="8" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D62" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="E62" t="s">
         <v>72</v>
@@ -3114,252 +3715,322 @@
         <v>44</v>
       </c>
       <c r="G62" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" ht="12">
-      <c r="A63" t="s">
+        <v>164</v>
+      </c>
+      <c r="I62" s="21" t="s">
+        <v>352</v>
+      </c>
+      <c r="K62" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" ht="37">
+      <c r="A63" s="24" t="s">
+        <v>230</v>
+      </c>
+      <c r="C63" s="8" t="s">
+        <v>233</v>
+      </c>
+      <c r="D63" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="E63" t="s">
+        <v>246</v>
+      </c>
+      <c r="F63" t="s">
+        <v>247</v>
+      </c>
+      <c r="I63" s="22" t="s">
+        <v>353</v>
+      </c>
+      <c r="J63" s="16" t="s">
+        <v>343</v>
+      </c>
+      <c r="K63" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" ht="37">
+      <c r="A64" s="24" t="s">
         <v>231</v>
       </c>
-      <c r="C63" s="8" t="s">
+      <c r="C64" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="D63" t="s">
-        <v>247</v>
-      </c>
-      <c r="E63" t="s">
+      <c r="D64" t="s">
         <v>248</v>
       </c>
-      <c r="F63" t="s">
+      <c r="E64" t="s">
         <v>249</v>
       </c>
-      <c r="J63" s="16" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" ht="12">
-      <c r="A64" t="s">
-        <v>232</v>
-      </c>
-      <c r="C64" s="8" t="s">
+      <c r="F64" t="s">
+        <v>250</v>
+      </c>
+      <c r="I64" s="22" t="s">
+        <v>353</v>
+      </c>
+      <c r="J64" t="s">
+        <v>347</v>
+      </c>
+      <c r="K64" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" ht="15">
+      <c r="C65" s="8" t="s">
         <v>235</v>
       </c>
-      <c r="D64" t="s">
+      <c r="D65" t="s">
+        <v>251</v>
+      </c>
+      <c r="E65" t="s">
+        <v>252</v>
+      </c>
+      <c r="F65" t="s">
+        <v>253</v>
+      </c>
+      <c r="I65" s="22" t="s">
+        <v>353</v>
+      </c>
+      <c r="J65" t="s">
+        <v>344</v>
+      </c>
+      <c r="K65" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" ht="15">
+      <c r="B66" t="s">
+        <v>256</v>
+      </c>
+      <c r="C66" s="8" t="s">
+        <v>236</v>
+      </c>
+      <c r="D66" t="s">
+        <v>254</v>
+      </c>
+      <c r="E66" t="s">
+        <v>255</v>
+      </c>
+      <c r="F66" t="s">
+        <v>257</v>
+      </c>
+      <c r="G66" t="s">
+        <v>258</v>
+      </c>
+      <c r="I66" s="22" t="s">
+        <v>353</v>
+      </c>
+      <c r="J66" t="s">
+        <v>346</v>
+      </c>
+      <c r="K66" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" ht="15">
+      <c r="C67" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="D67" s="27" t="s">
+        <v>259</v>
+      </c>
+      <c r="E67" t="s">
+        <v>260</v>
+      </c>
+      <c r="F67" t="s">
+        <v>261</v>
+      </c>
+      <c r="G67" t="s">
+        <v>262</v>
+      </c>
+      <c r="I67" s="22" t="s">
+        <v>353</v>
+      </c>
+      <c r="J67" t="s">
+        <v>343</v>
+      </c>
+      <c r="K67" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" ht="15">
+      <c r="C68" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="D68" t="s">
+        <v>263</v>
+      </c>
+      <c r="E68" t="s">
+        <v>264</v>
+      </c>
+      <c r="F68" t="s">
         <v>250</v>
       </c>
-      <c r="E64" t="s">
-        <v>251</v>
-      </c>
-      <c r="F64" t="s">
-        <v>252</v>
-      </c>
-      <c r="J64" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" ht="12">
-      <c r="C65" s="8" t="s">
-        <v>236</v>
-      </c>
-      <c r="D65" t="s">
-        <v>253</v>
-      </c>
-      <c r="E65" t="s">
-        <v>254</v>
-      </c>
-      <c r="F65" t="s">
-        <v>255</v>
-      </c>
-      <c r="J65" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" ht="12">
-      <c r="B66" t="s">
-        <v>258</v>
-      </c>
-      <c r="C66" s="8" t="s">
-        <v>237</v>
-      </c>
-      <c r="D66" t="s">
-        <v>256</v>
-      </c>
-      <c r="E66" t="s">
-        <v>257</v>
-      </c>
-      <c r="F66" t="s">
-        <v>259</v>
-      </c>
-      <c r="G66" t="s">
-        <v>260</v>
-      </c>
-      <c r="J66" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" ht="12">
-      <c r="C67" s="8" t="s">
-        <v>238</v>
-      </c>
-      <c r="D67" t="s">
-        <v>261</v>
-      </c>
-      <c r="E67" t="s">
-        <v>262</v>
-      </c>
-      <c r="F67" t="s">
-        <v>263</v>
-      </c>
-      <c r="G67" t="s">
-        <v>264</v>
-      </c>
-      <c r="J67" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" ht="12">
-      <c r="C68" s="8" t="s">
+      <c r="G68" t="s">
+        <v>265</v>
+      </c>
+      <c r="I68" s="22" t="s">
+        <v>353</v>
+      </c>
+      <c r="J68" t="s">
+        <v>343</v>
+      </c>
+      <c r="K68" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" ht="15">
+      <c r="C69" s="8" t="s">
         <v>239</v>
       </c>
-      <c r="D68" t="s">
-        <v>265</v>
-      </c>
-      <c r="E68" t="s">
+      <c r="D69" s="27" t="s">
         <v>266</v>
       </c>
-      <c r="F68" t="s">
-        <v>252</v>
-      </c>
-      <c r="G68" t="s">
+      <c r="E69" t="s">
         <v>267</v>
       </c>
-      <c r="J68" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" ht="12">
-      <c r="C69" s="8" t="s">
+      <c r="F69" t="s">
+        <v>268</v>
+      </c>
+      <c r="G69" t="s">
+        <v>269</v>
+      </c>
+      <c r="I69" s="22" t="s">
+        <v>353</v>
+      </c>
+      <c r="J69" t="s">
+        <v>343</v>
+      </c>
+      <c r="K69" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" ht="15">
+      <c r="C70" s="8" t="s">
         <v>240</v>
       </c>
-      <c r="D69" t="s">
-        <v>268</v>
-      </c>
-      <c r="E69" t="s">
-        <v>269</v>
-      </c>
-      <c r="F69" t="s">
+      <c r="D70" t="s">
         <v>270</v>
       </c>
-      <c r="G69" t="s">
+      <c r="E70" t="s">
+        <v>272</v>
+      </c>
+      <c r="F70" t="s">
         <v>271</v>
       </c>
-      <c r="J69" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" ht="12">
-      <c r="C70" s="8" t="s">
+      <c r="G70" t="s">
+        <v>273</v>
+      </c>
+      <c r="I70" s="22" t="s">
+        <v>353</v>
+      </c>
+      <c r="J70" t="s">
+        <v>344</v>
+      </c>
+      <c r="K70" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" ht="15">
+      <c r="B71" t="s">
+        <v>274</v>
+      </c>
+      <c r="C71" s="8" t="s">
         <v>241</v>
       </c>
-      <c r="D70" t="s">
-        <v>272</v>
-      </c>
-      <c r="E70" t="s">
-        <v>274</v>
-      </c>
-      <c r="F70" t="s">
-        <v>273</v>
-      </c>
-      <c r="G70" t="s">
+      <c r="D71" t="s">
         <v>275</v>
       </c>
-      <c r="J70" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10" ht="12">
-      <c r="B71" t="s">
+      <c r="E71" t="s">
         <v>276</v>
       </c>
-      <c r="C71" s="8" t="s">
+      <c r="F71" t="s">
+        <v>277</v>
+      </c>
+      <c r="G71" t="s">
+        <v>278</v>
+      </c>
+      <c r="I71" s="22" t="s">
+        <v>353</v>
+      </c>
+      <c r="J71" t="s">
+        <v>345</v>
+      </c>
+      <c r="K71" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" ht="15">
+      <c r="C72" s="8" t="s">
         <v>242</v>
       </c>
-      <c r="D71" t="s">
-        <v>277</v>
-      </c>
-      <c r="E71" t="s">
-        <v>278</v>
-      </c>
-      <c r="F71" t="s">
+      <c r="D72" s="27" t="s">
         <v>279</v>
       </c>
-      <c r="G71" t="s">
+      <c r="E72" t="s">
         <v>280</v>
       </c>
-      <c r="J71" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10" ht="12">
-      <c r="C72" s="8" t="s">
+      <c r="F72" t="s">
+        <v>281</v>
+      </c>
+      <c r="G72" t="s">
+        <v>282</v>
+      </c>
+      <c r="I72" s="22" t="s">
+        <v>353</v>
+      </c>
+      <c r="J72" t="s">
+        <v>345</v>
+      </c>
+      <c r="K72" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" ht="15">
+      <c r="C73" s="8" t="s">
         <v>243</v>
       </c>
-      <c r="D72" t="s">
-        <v>281</v>
-      </c>
-      <c r="E72" t="s">
-        <v>282</v>
-      </c>
-      <c r="F72" t="s">
+      <c r="D73" t="s">
         <v>283</v>
       </c>
-      <c r="G72" t="s">
+      <c r="E73" t="s">
         <v>284</v>
-      </c>
-      <c r="J72" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10" ht="12">
-      <c r="C73" s="8" t="s">
-        <v>244</v>
-      </c>
-      <c r="D73" t="s">
-        <v>285</v>
-      </c>
-      <c r="E73" t="s">
-        <v>286</v>
       </c>
       <c r="F73" t="s">
         <v>44</v>
       </c>
       <c r="G73" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10" ht="12">
-      <c r="C74" s="8" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10" ht="12">
+        <v>164</v>
+      </c>
+      <c r="I73" s="21" t="s">
+        <v>352</v>
+      </c>
+      <c r="K73" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" ht="12">
+      <c r="C74" s="8"/>
+    </row>
+    <row r="75" spans="1:11" ht="12">
       <c r="C75" s="1"/>
     </row>
-    <row r="76" spans="1:10" ht="12">
+    <row r="76" spans="1:11" ht="12">
       <c r="C76" s="1"/>
     </row>
-    <row r="77" spans="1:10" ht="12">
+    <row r="77" spans="1:11" ht="15">
       <c r="A77" s="15" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B77" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C77" s="8" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D77" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="E77" t="s">
         <v>72</v>
@@ -3368,263 +4039,349 @@
         <v>44</v>
       </c>
       <c r="G77" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="78" spans="1:10" ht="12">
-      <c r="A78" t="s">
-        <v>288</v>
+        <v>164</v>
+      </c>
+      <c r="I77" s="21" t="s">
+        <v>352</v>
+      </c>
+      <c r="K77" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" ht="25">
+      <c r="A78" s="24" t="s">
+        <v>286</v>
       </c>
       <c r="C78" s="8" t="s">
+        <v>289</v>
+      </c>
+      <c r="D78" s="27" t="s">
+        <v>302</v>
+      </c>
+      <c r="E78" t="s">
+        <v>303</v>
+      </c>
+      <c r="F78" t="s">
+        <v>304</v>
+      </c>
+      <c r="G78" t="s">
+        <v>305</v>
+      </c>
+      <c r="I78" s="22" t="s">
+        <v>353</v>
+      </c>
+      <c r="J78" t="s">
+        <v>343</v>
+      </c>
+      <c r="K78" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" ht="25">
+      <c r="A79" s="24" t="s">
+        <v>287</v>
+      </c>
+      <c r="C79" s="8" t="s">
+        <v>290</v>
+      </c>
+      <c r="D79" t="s">
+        <v>306</v>
+      </c>
+      <c r="E79" t="s">
+        <v>307</v>
+      </c>
+      <c r="F79" t="s">
+        <v>308</v>
+      </c>
+      <c r="G79" t="s">
+        <v>309</v>
+      </c>
+      <c r="I79" s="17" t="s">
+        <v>349</v>
+      </c>
+      <c r="J79" t="s">
+        <v>347</v>
+      </c>
+      <c r="K79" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" ht="15">
+      <c r="B80" t="s">
+        <v>310</v>
+      </c>
+      <c r="C80" s="8" t="s">
         <v>291</v>
       </c>
-      <c r="D78" t="s">
-        <v>304</v>
-      </c>
-      <c r="E78" t="s">
-        <v>305</v>
-      </c>
-      <c r="F78" t="s">
-        <v>306</v>
-      </c>
-      <c r="G78" t="s">
-        <v>307</v>
-      </c>
-      <c r="J78" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="79" spans="1:10" ht="12">
-      <c r="A79" t="s">
-        <v>289</v>
-      </c>
-      <c r="C79" s="8" t="s">
+      <c r="D80" t="s">
+        <v>314</v>
+      </c>
+      <c r="E80" t="s">
+        <v>311</v>
+      </c>
+      <c r="F80" t="s">
+        <v>312</v>
+      </c>
+      <c r="G80" t="s">
+        <v>313</v>
+      </c>
+      <c r="I80" s="17" t="s">
+        <v>349</v>
+      </c>
+      <c r="J80" t="s">
+        <v>343</v>
+      </c>
+      <c r="K80" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="81" spans="2:11" ht="15">
+      <c r="C81" s="8" t="s">
         <v>292</v>
       </c>
-      <c r="D79" t="s">
-        <v>308</v>
-      </c>
-      <c r="E79" t="s">
+      <c r="D81" s="27" t="s">
+        <v>315</v>
+      </c>
+      <c r="E81" t="s">
+        <v>316</v>
+      </c>
+      <c r="F81" t="s">
+        <v>317</v>
+      </c>
+      <c r="G81" t="s">
         <v>309</v>
       </c>
-      <c r="F79" t="s">
-        <v>310</v>
-      </c>
-      <c r="G79" t="s">
-        <v>311</v>
-      </c>
-      <c r="J79" t="s">
+      <c r="I81" s="22" t="s">
+        <v>353</v>
+      </c>
+      <c r="J81" t="s">
+        <v>343</v>
+      </c>
+      <c r="K81" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="82" spans="2:11" ht="15">
+      <c r="C82" s="8" t="s">
+        <v>293</v>
+      </c>
+      <c r="D82" t="s">
+        <v>318</v>
+      </c>
+      <c r="E82" t="s">
+        <v>319</v>
+      </c>
+      <c r="F82" t="s">
+        <v>320</v>
+      </c>
+      <c r="G82" t="s">
+        <v>321</v>
+      </c>
+      <c r="I82" s="22" t="s">
+        <v>353</v>
+      </c>
+      <c r="J82" t="s">
+        <v>344</v>
+      </c>
+      <c r="K82" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="83" spans="2:11" ht="15">
+      <c r="B83" t="s">
+        <v>350</v>
+      </c>
+      <c r="C83" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="D83" s="27" t="s">
+        <v>355</v>
+      </c>
+      <c r="E83" t="s">
+        <v>324</v>
+      </c>
+      <c r="F83" t="s">
+        <v>322</v>
+      </c>
+      <c r="G83" t="s">
+        <v>323</v>
+      </c>
+      <c r="I83" s="22" t="s">
+        <v>353</v>
+      </c>
+      <c r="J83" t="s">
+        <v>343</v>
+      </c>
+      <c r="K83" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="84" spans="2:11" ht="15">
+      <c r="C84" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="D84" t="s">
+        <v>358</v>
+      </c>
+      <c r="E84" t="s">
+        <v>359</v>
+      </c>
+      <c r="F84" t="s">
+        <v>325</v>
+      </c>
+      <c r="G84" t="s">
+        <v>326</v>
+      </c>
+      <c r="I84" s="21" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="80" spans="1:10" ht="12">
-      <c r="B80" t="s">
-        <v>312</v>
-      </c>
-      <c r="C80" s="8" t="s">
-        <v>293</v>
-      </c>
-      <c r="D80" t="s">
-        <v>316</v>
-      </c>
-      <c r="E80" t="s">
-        <v>313</v>
-      </c>
-      <c r="F80" t="s">
-        <v>314</v>
-      </c>
-      <c r="G80" t="s">
-        <v>315</v>
-      </c>
-      <c r="J80" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="81" spans="2:10" ht="12">
-      <c r="C81" s="8" t="s">
-        <v>294</v>
-      </c>
-      <c r="D81" t="s">
-        <v>317</v>
-      </c>
-      <c r="E81" t="s">
-        <v>318</v>
-      </c>
-      <c r="F81" t="s">
-        <v>319</v>
-      </c>
-      <c r="G81" t="s">
-        <v>311</v>
-      </c>
-      <c r="J81" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="82" spans="2:10" ht="12">
-      <c r="C82" s="8" t="s">
-        <v>295</v>
-      </c>
-      <c r="D82" t="s">
-        <v>320</v>
-      </c>
-      <c r="E82" t="s">
-        <v>321</v>
-      </c>
-      <c r="F82" t="s">
-        <v>322</v>
-      </c>
-      <c r="G82" t="s">
-        <v>323</v>
-      </c>
-      <c r="J82" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="83" spans="2:10" ht="12">
-      <c r="B83" t="s">
-        <v>355</v>
-      </c>
-      <c r="C83" s="8" t="s">
+      <c r="J84" t="s">
+        <v>345</v>
+      </c>
+      <c r="K84" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="85" spans="2:11" ht="15">
+      <c r="C85" s="8" t="s">
         <v>296</v>
       </c>
-      <c r="D83" t="s">
-        <v>324</v>
-      </c>
-      <c r="E83" t="s">
-        <v>325</v>
-      </c>
-      <c r="F83" t="s">
-        <v>326</v>
-      </c>
-      <c r="G83" t="s">
+      <c r="D85" t="s">
+        <v>357</v>
+      </c>
+      <c r="E85" t="s">
+        <v>360</v>
+      </c>
+      <c r="I85" s="21" t="s">
+        <v>352</v>
+      </c>
+      <c r="K85" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="86" spans="2:11" ht="15">
+      <c r="C86" s="8" t="s">
+        <v>297</v>
+      </c>
+      <c r="D86" t="s">
         <v>327</v>
       </c>
-      <c r="J83" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="84" spans="2:10" ht="12">
-      <c r="C84" s="8" t="s">
-        <v>297</v>
-      </c>
-      <c r="D84" t="s">
+      <c r="E86" t="s">
         <v>328</v>
       </c>
-      <c r="E84" t="s">
+      <c r="F86" t="s">
         <v>329</v>
       </c>
-      <c r="F84" t="s">
+      <c r="G86" t="s">
         <v>330</v>
       </c>
-      <c r="G84" t="s">
+      <c r="I86" s="22" t="s">
+        <v>353</v>
+      </c>
+      <c r="J86" t="s">
+        <v>346</v>
+      </c>
+      <c r="K86" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="87" spans="2:11" ht="15">
+      <c r="B87" t="s">
+        <v>340</v>
+      </c>
+      <c r="C87" s="8" t="s">
+        <v>298</v>
+      </c>
+      <c r="D87" s="27" t="s">
         <v>331</v>
       </c>
-      <c r="J84" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="85" spans="2:10" ht="12">
-      <c r="C85" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="D85" t="s">
+      <c r="E87" t="s">
         <v>332</v>
       </c>
-      <c r="E85" t="s">
+      <c r="F87" t="s">
         <v>333</v>
       </c>
-      <c r="F85" t="s">
+      <c r="G87" t="s">
         <v>334</v>
       </c>
-      <c r="G85" t="s">
+      <c r="I87" s="22" t="s">
+        <v>353</v>
+      </c>
+      <c r="J87" t="s">
+        <v>345</v>
+      </c>
+      <c r="K87" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="88" spans="2:11" ht="15">
+      <c r="C88" s="8" t="s">
+        <v>299</v>
+      </c>
+      <c r="D88" t="s">
         <v>335</v>
       </c>
-      <c r="J85" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="86" spans="2:10" ht="12">
-      <c r="B86" t="s">
-        <v>345</v>
-      </c>
-      <c r="C86" s="8" t="s">
-        <v>299</v>
-      </c>
-      <c r="D86" t="s">
+      <c r="E88" t="s">
         <v>336</v>
       </c>
-      <c r="E86" t="s">
+      <c r="F88" t="s">
         <v>337</v>
       </c>
-      <c r="F86" t="s">
+      <c r="G88" t="s">
+        <v>342</v>
+      </c>
+      <c r="I88" s="22" t="s">
+        <v>353</v>
+      </c>
+      <c r="J88" t="s">
+        <v>346</v>
+      </c>
+      <c r="K88" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="89" spans="2:11" ht="15">
+      <c r="C89" s="8" t="s">
+        <v>356</v>
+      </c>
+      <c r="D89" t="s">
+        <v>339</v>
+      </c>
+      <c r="E89" t="s">
+        <v>341</v>
+      </c>
+      <c r="F89" t="s">
+        <v>44</v>
+      </c>
+      <c r="G89" t="s">
         <v>338</v>
       </c>
-      <c r="G86" t="s">
-        <v>339</v>
-      </c>
-      <c r="J86" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="87" spans="2:10" ht="12">
-      <c r="C87" s="8" t="s">
-        <v>300</v>
-      </c>
-      <c r="D87" t="s">
-        <v>340</v>
-      </c>
-      <c r="E87" t="s">
-        <v>341</v>
-      </c>
-      <c r="F87" t="s">
-        <v>342</v>
-      </c>
-      <c r="G87" t="s">
-        <v>347</v>
-      </c>
-      <c r="J87" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="88" spans="2:10" ht="12">
-      <c r="C88" s="8" t="s">
-        <v>301</v>
-      </c>
-      <c r="D88" t="s">
-        <v>344</v>
-      </c>
-      <c r="E88" t="s">
-        <v>346</v>
-      </c>
-      <c r="F88" t="s">
-        <v>44</v>
-      </c>
-      <c r="G88" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="89" spans="2:10" ht="12">
-      <c r="C89" s="1"/>
-    </row>
-    <row r="90" spans="2:10" ht="12">
+      <c r="I89" s="21" t="s">
+        <v>352</v>
+      </c>
+      <c r="K89" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="90" spans="2:11" ht="12">
       <c r="C90" s="1"/>
     </row>
-    <row r="91" spans="2:10" ht="12">
+    <row r="91" spans="2:11" ht="12">
       <c r="C91" s="1"/>
     </row>
-    <row r="92" spans="2:10" ht="12">
+    <row r="92" spans="2:11" ht="12">
       <c r="C92" s="1"/>
     </row>
-    <row r="93" spans="2:10" ht="12">
+    <row r="93" spans="2:11" ht="12">
       <c r="C93" s="1"/>
     </row>
-    <row r="94" spans="2:10" ht="12">
+    <row r="94" spans="2:11" ht="12">
       <c r="C94" s="1"/>
     </row>
-    <row r="95" spans="2:10" ht="12">
+    <row r="95" spans="2:11" ht="12">
       <c r="C95" s="1"/>
     </row>
-    <row r="96" spans="2:10" ht="12">
+    <row r="96" spans="2:11" ht="12">
       <c r="C96" s="1"/>
     </row>
     <row r="97" spans="3:3" ht="12">
@@ -6336,6 +7093,13 @@
     <row r="999" spans="3:3" ht="12">
       <c r="C999" s="1"/>
     </row>
+    <row r="1000" spans="3:3" ht="12">
+      <c r="C1000" s="1"/>
+    </row>
+    <row r="1001" spans="3:3" ht="12"/>
+    <row r="1002" spans="3:3" ht="12"/>
+    <row r="1003" spans="3:3" ht="12"/>
+    <row r="1004" spans="3:3" ht="12"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A5:A7"/>

</xml_diff>

<commit_message>
More work on the course
Added pictures, updated the article sources from the site and added a
quiz for Week 3
</commit_message>
<xml_diff>
--- a/fl_course_outline_weeks.xlsx
+++ b/fl_course_outline_weeks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27127"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4820" yWindow="200" windowWidth="32780" windowHeight="26860" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="42440" windowHeight="26400" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="367">
   <si>
     <t>Week</t>
   </si>
@@ -78,9 +78,6 @@
     <t>Video: the basic elements of Haskell</t>
   </si>
   <si>
-    <t>Tutorial: try it for yourself</t>
-  </si>
-  <si>
     <t>Quiz: what do you know about Haskell?</t>
   </si>
   <si>
@@ -405,9 +402,6 @@
     <t>Video: welcome to week 3</t>
   </si>
   <si>
-    <t>Tutorial: Filtering lists</t>
-  </si>
-  <si>
     <t>filter takes a function argument, and applies it to elements of list - key concept</t>
   </si>
   <si>
@@ -417,9 +411,6 @@
     <t>the shape of recursion on lists, base case and inductive step, etc</t>
   </si>
   <si>
-    <t>Tutorial: Mapping lists</t>
-  </si>
-  <si>
     <t>map for transforming lists, folds, sum of squares?</t>
   </si>
   <si>
@@ -1120,6 +1111,21 @@
   </si>
   <si>
     <t>J</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>Tutorial 1.1: The Basics: Expressions, Functions and Equations</t>
+  </si>
+  <si>
+    <t>Tutorial 1.2: The Essentials: Functions and Lists</t>
+  </si>
+  <si>
+    <t>Tutorial 3.1: Lists and Recursion</t>
+  </si>
+  <si>
+    <t>Tutorial 3.2: More Computations on Lists</t>
   </si>
 </sst>
 </file>
@@ -1199,7 +1205,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1236,6 +1242,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1310,7 +1322,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="286">
+  <cellStyleXfs count="304">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1597,8 +1609,26 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1637,15 +1667,6 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="55" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="151" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1669,8 +1690,43 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="286">
+  <cellStyles count="304">
     <cellStyle name="Bad" xfId="150" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -1813,6 +1869,15 @@
     <cellStyle name="Followed Hyperlink" xfId="281" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="283" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="285" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="287" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="289" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="291" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="293" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="295" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="297" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="299" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="301" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="303" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="55" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -1955,6 +2020,15 @@
     <cellStyle name="Hyperlink" xfId="280" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="282" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="284" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="286" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="288" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="290" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="292" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="294" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="296" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="298" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="300" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="302" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="151" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -2223,7 +2297,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2231,12 +2305,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K1004"/>
+  <dimension ref="A1:L1004"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A73" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="K90" sqref="K90"/>
+      <selection pane="bottomLeft" activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -2244,8 +2318,8 @@
     <col min="1" max="1" width="26.5" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
     <col min="3" max="3" width="7.6640625" customWidth="1"/>
-    <col min="4" max="4" width="33.6640625" customWidth="1"/>
-    <col min="5" max="5" width="38.6640625" customWidth="1"/>
+    <col min="4" max="4" width="52" customWidth="1"/>
+    <col min="5" max="5" width="38.6640625" style="33" customWidth="1"/>
     <col min="6" max="6" width="39.83203125" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="33.6640625" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="42.5" hidden="1" customWidth="1"/>
@@ -2264,7 +2338,7 @@
       <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="32" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="10" t="s">
@@ -2277,13 +2351,13 @@
         <v>7</v>
       </c>
       <c r="I1" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="J1" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="J1" s="12" t="s">
-        <v>79</v>
-      </c>
       <c r="K1" s="12" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="49" customHeight="1">
@@ -2296,55 +2370,55 @@
       <c r="C2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>32</v>
+      <c r="E2" s="31" t="s">
+        <v>31</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H2" s="3"/>
-      <c r="I2" s="22" t="s">
-        <v>353</v>
+      <c r="I2" s="19" t="s">
+        <v>350</v>
       </c>
       <c r="K2" s="16" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.75" customHeight="1">
       <c r="A3" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="6">
         <v>1.2</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>33</v>
+      <c r="E3" s="31" t="s">
+        <v>32</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H3" s="3"/>
-      <c r="I3" s="22" t="s">
-        <v>353</v>
+      <c r="I3" s="19" t="s">
+        <v>350</v>
       </c>
       <c r="J3" s="16" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="K3" s="16" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15.75" customHeight="1">
@@ -2358,288 +2432,288 @@
       <c r="D4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>34</v>
+      <c r="E4" s="31" t="s">
+        <v>33</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H4" s="3"/>
       <c r="I4" s="17" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="J4" s="16" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="K4" s="16" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="28" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="6">
         <v>1.4</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>35</v>
+      <c r="D5" s="31" t="s">
+        <v>363</v>
+      </c>
+      <c r="E5" s="38" t="s">
+        <v>34</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="17" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="J5" s="16" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="K5" s="16" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A6" s="19"/>
+      <c r="A6" s="29"/>
       <c r="B6" s="5"/>
       <c r="C6" s="7">
         <v>1.5</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>36</v>
+        <v>17</v>
+      </c>
+      <c r="E6" s="31" t="s">
+        <v>35</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H6" s="3"/>
       <c r="I6" s="17" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="J6" s="16" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="K6" s="16" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A7" s="20"/>
+      <c r="A7" s="30"/>
       <c r="B7" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>37</v>
+      <c r="D7" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="31" t="s">
+        <v>36</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H7" s="3"/>
-      <c r="I7" s="22" t="s">
-        <v>353</v>
+      <c r="I7" s="19" t="s">
+        <v>350</v>
       </c>
       <c r="J7" s="16" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="K7" s="16" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15.75" customHeight="1">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>38</v>
+        <v>20</v>
+      </c>
+      <c r="E8" s="31" t="s">
+        <v>37</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H8" s="3"/>
       <c r="I8" s="17" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="J8" s="16" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="K8" s="16" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.75" customHeight="1">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>39</v>
+        <v>364</v>
+      </c>
+      <c r="E9" s="31" t="s">
+        <v>38</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H9" s="3"/>
       <c r="I9" s="17" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="J9" s="16" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="K9" s="16" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="15.75" customHeight="1">
       <c r="A10" s="3"/>
       <c r="B10" s="5"/>
       <c r="C10" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>36</v>
+        <v>17</v>
+      </c>
+      <c r="E10" s="31" t="s">
+        <v>35</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H10" s="3"/>
       <c r="I10" s="17" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="J10" s="16" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="K10" s="16" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="15.75" customHeight="1">
       <c r="A11" s="3"/>
       <c r="B11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>40</v>
+      <c r="E11" s="31" t="s">
+        <v>39</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H11" s="3"/>
-      <c r="I11" s="23" t="s">
-        <v>352</v>
+      <c r="I11" s="20" t="s">
+        <v>349</v>
       </c>
       <c r="J11" s="16" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="K11" s="16" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="15.75" customHeight="1">
       <c r="A12" s="3"/>
       <c r="B12" s="5"/>
       <c r="C12" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>41</v>
+        <v>23</v>
+      </c>
+      <c r="E12" s="31" t="s">
+        <v>40</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H12" s="3"/>
-      <c r="I12" s="21" t="s">
-        <v>352</v>
+      <c r="I12" s="18" t="s">
+        <v>349</v>
       </c>
       <c r="J12" s="16" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="K12" s="16" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="15.75" customHeight="1">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>42</v>
+        <v>24</v>
+      </c>
+      <c r="E13" s="31" t="s">
+        <v>41</v>
       </c>
       <c r="F13" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G13" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="G13" s="3" t="s">
-        <v>45</v>
-      </c>
       <c r="H13" s="3"/>
-      <c r="I13" s="21" t="s">
-        <v>352</v>
+      <c r="I13" s="18" t="s">
+        <v>349</v>
       </c>
       <c r="K13" s="16" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="15.75" customHeight="1">
@@ -2647,7 +2721,7 @@
       <c r="B14" s="5"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
+      <c r="E14" s="31"/>
       <c r="F14" s="5"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
@@ -2657,7 +2731,7 @@
       <c r="B15" s="5"/>
       <c r="C15" s="9"/>
       <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
+      <c r="E15" s="31"/>
       <c r="F15" s="5"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
@@ -2667,7 +2741,7 @@
       <c r="B16" s="3"/>
       <c r="C16" s="9"/>
       <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
+      <c r="E16" s="31"/>
       <c r="F16" s="5"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
@@ -2677,1690 +2751,1699 @@
       <c r="B17" s="5"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
+      <c r="E17" s="31"/>
       <c r="F17" s="5"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
     </row>
     <row r="18" spans="1:11" ht="15.75" customHeight="1">
       <c r="A18" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D18" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E18" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="E18" s="3" t="s">
-        <v>72</v>
-      </c>
       <c r="F18" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H18" s="3"/>
       <c r="I18" s="17" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="K18" s="16" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="15.75" customHeight="1">
       <c r="A19" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B19" s="5"/>
       <c r="C19" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D19" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E19" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="F19" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="F19" s="3" t="s">
-        <v>75</v>
-      </c>
       <c r="G19" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H19" s="3"/>
       <c r="I19" s="17" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="J19" s="16" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="K19" s="16" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="15.75" customHeight="1">
       <c r="A20" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B20" s="5"/>
       <c r="C20" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D20" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E20" s="31" t="s">
         <v>76</v>
       </c>
-      <c r="E20" s="3" t="s">
-        <v>77</v>
-      </c>
       <c r="F20" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G20" s="3" t="s">
         <v>83</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>84</v>
       </c>
       <c r="H20" s="3"/>
       <c r="I20" s="17" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="J20" s="16" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="K20" s="16" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="15.75" customHeight="1">
       <c r="A21" s="3"/>
       <c r="B21" s="5"/>
       <c r="C21" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D21" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E21" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="F21" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="F21" s="3" t="s">
-        <v>82</v>
-      </c>
       <c r="G21" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H21" s="3"/>
       <c r="I21" s="17" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="J21" s="16" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="K21" s="16" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="15.75" customHeight="1">
       <c r="A22" s="3"/>
       <c r="B22" s="5"/>
       <c r="C22" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D22" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E22" s="31" t="s">
         <v>85</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="F22" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="F22" s="3" t="s">
-        <v>87</v>
-      </c>
       <c r="G22" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H22" s="3"/>
       <c r="I22" s="17" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="J22" s="16" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="K22" s="16" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="15.75" customHeight="1">
       <c r="A23" s="3"/>
       <c r="B23" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="D23" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="D23" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="E23" s="31" t="s">
         <v>90</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>91</v>
       </c>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
-      <c r="I23" s="22" t="s">
-        <v>353</v>
+      <c r="I23" s="19" t="s">
+        <v>350</v>
       </c>
       <c r="J23" s="16" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="K23" s="16" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="15.75" customHeight="1">
       <c r="A24" s="3"/>
       <c r="B24" s="5"/>
       <c r="C24" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D24" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E24" s="31" t="s">
         <v>92</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>93</v>
       </c>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
       <c r="I24" s="17" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="J24" s="16" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="K24" s="16" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="15.75" customHeight="1">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D25" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="E25" s="34" t="s">
         <v>94</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>95</v>
       </c>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
-      <c r="I25" s="22" t="s">
-        <v>353</v>
+      <c r="I25" s="19" t="s">
+        <v>350</v>
       </c>
       <c r="J25" s="16" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="K25" s="16" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="15.75" customHeight="1">
       <c r="A26" s="5"/>
       <c r="B26" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="D26" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="C26" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="D26" s="5" t="s">
+      <c r="E26" s="34" t="s">
         <v>97</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>98</v>
       </c>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
-      <c r="I26" s="22" t="s">
-        <v>353</v>
+      <c r="I26" s="19" t="s">
+        <v>350</v>
       </c>
       <c r="J26" s="16" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="K26" s="16" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="15.75" customHeight="1">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="D27" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="D27" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="E27" s="34" t="s">
         <v>101</v>
       </c>
-      <c r="E27" s="5" t="s">
-        <v>102</v>
-      </c>
       <c r="F27" s="5" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
-      <c r="I27" s="22" t="s">
-        <v>353</v>
+      <c r="I27" s="19" t="s">
+        <v>350</v>
       </c>
       <c r="J27" s="16" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="K27" s="16" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="15.75" customHeight="1">
       <c r="C28" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D28" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="E28" s="35" t="s">
         <v>103</v>
       </c>
-      <c r="E28" s="13" t="s">
-        <v>104</v>
-      </c>
-      <c r="I28" s="22" t="s">
-        <v>353</v>
+      <c r="I28" s="19" t="s">
+        <v>350</v>
       </c>
       <c r="J28" s="16" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="K28" s="16" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="15.75" customHeight="1">
       <c r="C29" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D29" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="E29" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E29" s="35" t="s">
+        <v>104</v>
+      </c>
+      <c r="F29" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="F29" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="I29" s="22" t="s">
-        <v>353</v>
+      <c r="I29" s="19" t="s">
+        <v>350</v>
       </c>
       <c r="J29" s="16" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="K29" s="16" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="15.75" customHeight="1">
       <c r="C30" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D30" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="E30" s="35" t="s">
         <v>107</v>
       </c>
-      <c r="E30" s="13" t="s">
-        <v>108</v>
-      </c>
       <c r="F30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I30" s="17" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="K30" s="16" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="15.75" customHeight="1">
       <c r="C31" s="8"/>
-    </row>
-    <row r="32" spans="1:11" ht="15.75" customHeight="1">
-      <c r="C32" s="1"/>
-    </row>
-    <row r="33" spans="1:11" ht="15.75" customHeight="1">
+      <c r="E31" s="36"/>
+    </row>
+    <row r="33" spans="1:12" ht="15.75" customHeight="1">
       <c r="A33" s="11" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="B33" t="s">
+        <v>110</v>
+      </c>
+      <c r="C33" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="C33" s="8" t="s">
+      <c r="D33" t="s">
+        <v>124</v>
+      </c>
+      <c r="E33" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="F33" t="s">
+        <v>43</v>
+      </c>
+      <c r="G33" t="s">
+        <v>161</v>
+      </c>
+      <c r="I33" s="17" t="s">
+        <v>346</v>
+      </c>
+      <c r="K33" s="25" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A34" t="s">
+        <v>108</v>
+      </c>
+      <c r="C34" s="8" t="s">
         <v>112</v>
-      </c>
-      <c r="D33" t="s">
-        <v>125</v>
-      </c>
-      <c r="E33" t="s">
-        <v>72</v>
-      </c>
-      <c r="F33" t="s">
-        <v>44</v>
-      </c>
-      <c r="G33" t="s">
-        <v>164</v>
-      </c>
-      <c r="I33" s="17" t="s">
-        <v>349</v>
-      </c>
-      <c r="K33" s="28" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A34" t="s">
-        <v>109</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>113</v>
       </c>
       <c r="D34" t="s">
         <v>126</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E34" s="36" t="s">
         <v>127</v>
       </c>
       <c r="F34" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G34" t="s">
-        <v>165</v>
-      </c>
-      <c r="I34" s="22" t="s">
-        <v>353</v>
+        <v>163</v>
+      </c>
+      <c r="I34" s="17" t="s">
+        <v>346</v>
       </c>
       <c r="J34" s="16" t="s">
-        <v>344</v>
-      </c>
-      <c r="K34" s="28" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" ht="15.75" customHeight="1">
+        <v>340</v>
+      </c>
+      <c r="K34" s="25" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="15.75" customHeight="1">
       <c r="A35" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D35" t="s">
-        <v>128</v>
-      </c>
-      <c r="E35" t="s">
-        <v>129</v>
+        <v>365</v>
+      </c>
+      <c r="E35" s="36" t="s">
+        <v>125</v>
       </c>
       <c r="F35" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="G35" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="I35" s="17" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="J35" s="16" t="s">
-        <v>343</v>
-      </c>
-      <c r="K35" s="28" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" ht="15.75" customHeight="1">
+        <v>341</v>
+      </c>
+      <c r="K35" s="25" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="15.75" customHeight="1">
       <c r="C36" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D36" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="E36" s="36" t="s">
         <v>130</v>
       </c>
-      <c r="E36" t="s">
+      <c r="F36" t="s">
+        <v>150</v>
+      </c>
+      <c r="G36" t="s">
+        <v>165</v>
+      </c>
+      <c r="I36" s="19" t="s">
+        <v>350</v>
+      </c>
+      <c r="J36" s="16" t="s">
+        <v>340</v>
+      </c>
+      <c r="K36" s="25" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="15.75" customHeight="1">
+      <c r="C37" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="D37" t="s">
+        <v>366</v>
+      </c>
+      <c r="E37" s="36" t="s">
+        <v>128</v>
+      </c>
+      <c r="F37" t="s">
+        <v>151</v>
+      </c>
+      <c r="G37" t="s">
+        <v>164</v>
+      </c>
+      <c r="I37" s="17" t="s">
+        <v>346</v>
+      </c>
+      <c r="J37" s="16" t="s">
+        <v>341</v>
+      </c>
+      <c r="K37" s="25" t="s">
+        <v>360</v>
+      </c>
+      <c r="L37" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="15.75" customHeight="1">
+      <c r="C38" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="D38" s="39" t="s">
         <v>131</v>
       </c>
-      <c r="F36" t="s">
+      <c r="E38" s="36" t="s">
+        <v>132</v>
+      </c>
+      <c r="F38" t="s">
+        <v>149</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="I38" s="17" t="s">
+        <v>346</v>
+      </c>
+      <c r="J38" s="16" t="s">
+        <v>341</v>
+      </c>
+      <c r="K38" s="25" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="15.75" customHeight="1">
+      <c r="B39" t="s">
+        <v>133</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="D39" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="E39" s="36" t="s">
+        <v>135</v>
+      </c>
+      <c r="F39" t="s">
+        <v>136</v>
+      </c>
+      <c r="G39" t="s">
+        <v>166</v>
+      </c>
+      <c r="I39" s="19" t="s">
+        <v>350</v>
+      </c>
+      <c r="J39" s="16" t="s">
+        <v>340</v>
+      </c>
+      <c r="K39" s="25" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="15.75" customHeight="1">
+      <c r="C40" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="D40" t="s">
+        <v>137</v>
+      </c>
+      <c r="E40" s="36" t="s">
+        <v>138</v>
+      </c>
+      <c r="F40" t="s">
+        <v>148</v>
+      </c>
+      <c r="G40" t="s">
+        <v>167</v>
+      </c>
+      <c r="I40" s="17" t="s">
+        <v>346</v>
+      </c>
+      <c r="J40" s="16" t="s">
+        <v>344</v>
+      </c>
+      <c r="K40" s="25" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="15.75" customHeight="1">
+      <c r="C41" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="D41" s="24" t="s">
+        <v>139</v>
+      </c>
+      <c r="E41" s="36" t="s">
+        <v>140</v>
+      </c>
+      <c r="F41" t="s">
+        <v>147</v>
+      </c>
+      <c r="G41" t="s">
+        <v>168</v>
+      </c>
+      <c r="I41" s="19" t="s">
+        <v>350</v>
+      </c>
+      <c r="J41" s="16" t="s">
+        <v>340</v>
+      </c>
+      <c r="K41" s="25" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="15.75" customHeight="1">
+      <c r="C42" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="D42" t="s">
+        <v>141</v>
+      </c>
+      <c r="E42" s="36" t="s">
+        <v>142</v>
+      </c>
+      <c r="F42" t="s">
+        <v>146</v>
+      </c>
+      <c r="G42" t="s">
+        <v>169</v>
+      </c>
+      <c r="I42" s="19" t="s">
+        <v>350</v>
+      </c>
+      <c r="J42" s="16" t="s">
+        <v>345</v>
+      </c>
+      <c r="K42" s="25" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="15.75" customHeight="1">
+      <c r="B43" t="s">
         <v>154</v>
       </c>
-      <c r="G36" t="s">
-        <v>167</v>
-      </c>
-      <c r="I36" s="22" t="s">
-        <v>353</v>
-      </c>
-      <c r="J36" s="16" t="s">
-        <v>344</v>
-      </c>
-      <c r="K36" s="28" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" ht="15.75" customHeight="1">
-      <c r="C37" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="D37" s="27" t="s">
-        <v>132</v>
-      </c>
-      <c r="E37" t="s">
-        <v>133</v>
-      </c>
-      <c r="F37" t="s">
-        <v>153</v>
-      </c>
-      <c r="G37" t="s">
-        <v>168</v>
-      </c>
-      <c r="I37" s="22" t="s">
-        <v>353</v>
-      </c>
-      <c r="J37" s="16" t="s">
-        <v>343</v>
-      </c>
-      <c r="K37" s="28" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" ht="15.75" customHeight="1">
-      <c r="C38" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="D38" t="s">
-        <v>134</v>
-      </c>
-      <c r="E38" t="s">
-        <v>135</v>
-      </c>
-      <c r="F38" t="s">
-        <v>152</v>
-      </c>
-      <c r="G38" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="I38" s="22" t="s">
-        <v>353</v>
-      </c>
-      <c r="J38" s="16" t="s">
-        <v>344</v>
-      </c>
-      <c r="K38" s="28" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" ht="15.75" customHeight="1">
-      <c r="B39" t="s">
-        <v>136</v>
-      </c>
-      <c r="C39" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="D39" s="27" t="s">
-        <v>137</v>
-      </c>
-      <c r="E39" t="s">
-        <v>138</v>
-      </c>
-      <c r="F39" t="s">
-        <v>139</v>
-      </c>
-      <c r="G39" t="s">
-        <v>169</v>
-      </c>
-      <c r="I39" s="22" t="s">
-        <v>353</v>
-      </c>
-      <c r="J39" s="16" t="s">
-        <v>343</v>
-      </c>
-      <c r="K39" s="28" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" ht="15.75" customHeight="1">
-      <c r="C40" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="D40" t="s">
-        <v>140</v>
-      </c>
-      <c r="E40" t="s">
-        <v>141</v>
-      </c>
-      <c r="F40" t="s">
-        <v>151</v>
-      </c>
-      <c r="G40" t="s">
+      <c r="C43" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="D43" s="24" t="s">
+        <v>155</v>
+      </c>
+      <c r="E43" s="35" t="s">
+        <v>156</v>
+      </c>
+      <c r="F43" t="s">
+        <v>43</v>
+      </c>
+      <c r="G43" t="s">
         <v>170</v>
       </c>
-      <c r="I40" s="17" t="s">
+      <c r="I43" s="19" t="s">
+        <v>350</v>
+      </c>
+      <c r="J43" s="16" t="s">
+        <v>342</v>
+      </c>
+      <c r="K43" s="25" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="15.75" customHeight="1">
+      <c r="C44" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="D44" t="s">
+        <v>157</v>
+      </c>
+      <c r="E44" s="37" t="s">
+        <v>158</v>
+      </c>
+      <c r="F44" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="G44" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="I44" s="19" t="s">
+        <v>350</v>
+      </c>
+      <c r="J44" s="16" t="s">
+        <v>342</v>
+      </c>
+      <c r="K44" s="25" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="15.75" customHeight="1">
+      <c r="C45" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="D45" t="s">
+        <v>143</v>
+      </c>
+      <c r="E45" s="35" t="s">
+        <v>145</v>
+      </c>
+      <c r="F45" t="s">
+        <v>43</v>
+      </c>
+      <c r="G45" t="s">
+        <v>161</v>
+      </c>
+      <c r="I45" s="17" t="s">
+        <v>346</v>
+      </c>
+      <c r="K45" s="25" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="15.75" customHeight="1">
+      <c r="C46" s="1"/>
+      <c r="E46" s="36"/>
+    </row>
+    <row r="47" spans="1:12" ht="12">
+      <c r="C47" s="1"/>
+      <c r="E47" s="36"/>
+    </row>
+    <row r="48" spans="1:12" ht="25">
+      <c r="A48" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="B48" t="s">
+        <v>197</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="D48" t="s">
+        <v>348</v>
+      </c>
+      <c r="E48" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="F48" t="s">
+        <v>43</v>
+      </c>
+      <c r="G48" t="s">
+        <v>161</v>
+      </c>
+      <c r="I48" s="18" t="s">
         <v>349</v>
       </c>
-      <c r="J40" s="16" t="s">
-        <v>347</v>
-      </c>
-      <c r="K40" s="28" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" ht="15.75" customHeight="1">
-      <c r="C41" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="D41" s="27" t="s">
-        <v>142</v>
-      </c>
-      <c r="E41" t="s">
-        <v>143</v>
-      </c>
-      <c r="F41" t="s">
-        <v>150</v>
-      </c>
-      <c r="G41" t="s">
-        <v>171</v>
-      </c>
-      <c r="I41" s="22" t="s">
-        <v>353</v>
-      </c>
-      <c r="J41" s="16" t="s">
-        <v>343</v>
-      </c>
-      <c r="K41" s="28" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" ht="15.75" customHeight="1">
-      <c r="C42" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="D42" t="s">
-        <v>144</v>
-      </c>
-      <c r="E42" t="s">
-        <v>145</v>
-      </c>
-      <c r="F42" t="s">
-        <v>149</v>
-      </c>
-      <c r="G42" t="s">
-        <v>172</v>
-      </c>
-      <c r="I42" s="22" t="s">
-        <v>353</v>
-      </c>
-      <c r="J42" s="16" t="s">
-        <v>348</v>
-      </c>
-      <c r="K42" s="28" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" ht="15.75" customHeight="1">
-      <c r="B43" t="s">
-        <v>157</v>
-      </c>
-      <c r="C43" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="D43" s="27" t="s">
-        <v>158</v>
-      </c>
-      <c r="E43" s="13" t="s">
-        <v>159</v>
-      </c>
-      <c r="F43" t="s">
-        <v>44</v>
-      </c>
-      <c r="G43" t="s">
-        <v>173</v>
-      </c>
-      <c r="I43" s="22" t="s">
-        <v>353</v>
-      </c>
-      <c r="J43" s="16" t="s">
-        <v>345</v>
-      </c>
-      <c r="K43" s="28" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" ht="15.75" customHeight="1">
-      <c r="C44" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="D44" t="s">
-        <v>160</v>
-      </c>
-      <c r="E44" s="14" t="s">
-        <v>161</v>
-      </c>
-      <c r="F44" s="14" t="s">
-        <v>162</v>
-      </c>
-      <c r="G44" s="14" t="s">
-        <v>163</v>
-      </c>
-      <c r="I44" s="22" t="s">
-        <v>353</v>
-      </c>
-      <c r="J44" s="16" t="s">
-        <v>345</v>
-      </c>
-      <c r="K44" s="28" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" ht="15.75" customHeight="1">
-      <c r="C45" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="D45" t="s">
-        <v>146</v>
-      </c>
-      <c r="E45" s="13" t="s">
-        <v>148</v>
-      </c>
-      <c r="F45" t="s">
-        <v>44</v>
-      </c>
-      <c r="G45" t="s">
-        <v>164</v>
-      </c>
-      <c r="I45" s="17" t="s">
-        <v>349</v>
-      </c>
-      <c r="K45" s="28" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" ht="15.75" customHeight="1">
-      <c r="C46" s="1"/>
-    </row>
-    <row r="47" spans="1:11" ht="12">
-      <c r="C47" s="1"/>
-    </row>
-    <row r="48" spans="1:11" ht="25">
-      <c r="A48" s="11" t="s">
-        <v>184</v>
-      </c>
-      <c r="B48" t="s">
-        <v>200</v>
-      </c>
-      <c r="C48" s="8" t="s">
-        <v>174</v>
-      </c>
-      <c r="D48" t="s">
-        <v>351</v>
-      </c>
-      <c r="E48" t="s">
-        <v>72</v>
-      </c>
-      <c r="F48" t="s">
-        <v>44</v>
-      </c>
-      <c r="G48" t="s">
-        <v>164</v>
-      </c>
-      <c r="I48" s="21" t="s">
-        <v>352</v>
-      </c>
-      <c r="K48" s="29" t="s">
-        <v>364</v>
+      <c r="K48" s="26" t="s">
+        <v>361</v>
       </c>
     </row>
     <row r="49" spans="1:11" ht="15">
       <c r="A49" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D49" t="s">
+        <v>198</v>
+      </c>
+      <c r="E49" s="36" t="s">
+        <v>199</v>
+      </c>
+      <c r="F49" t="s">
+        <v>200</v>
+      </c>
+      <c r="G49" t="s">
         <v>201</v>
       </c>
-      <c r="E49" t="s">
+      <c r="I49" s="19" t="s">
+        <v>350</v>
+      </c>
+      <c r="J49" s="16" t="s">
+        <v>340</v>
+      </c>
+      <c r="K49" s="26" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" ht="25">
+      <c r="A50" t="s">
+        <v>183</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="D50" t="s">
         <v>202</v>
       </c>
-      <c r="F49" t="s">
+      <c r="E50" s="36" t="s">
         <v>203</v>
       </c>
-      <c r="G49" t="s">
+      <c r="F50" t="s">
+        <v>200</v>
+      </c>
+      <c r="G50" t="s">
         <v>204</v>
       </c>
-      <c r="I49" s="22" t="s">
-        <v>353</v>
-      </c>
-      <c r="J49" s="16" t="s">
-        <v>343</v>
-      </c>
-      <c r="K49" s="29" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" ht="15">
-      <c r="A50" t="s">
-        <v>186</v>
-      </c>
-      <c r="C50" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="D50" t="s">
-        <v>205</v>
-      </c>
-      <c r="E50" t="s">
-        <v>206</v>
-      </c>
-      <c r="F50" t="s">
-        <v>203</v>
-      </c>
-      <c r="G50" t="s">
-        <v>207</v>
-      </c>
-      <c r="I50" s="22" t="s">
-        <v>353</v>
+      <c r="I50" s="19" t="s">
+        <v>350</v>
       </c>
       <c r="J50" s="16" t="s">
-        <v>343</v>
-      </c>
-      <c r="K50" s="29" t="s">
-        <v>364</v>
+        <v>340</v>
+      </c>
+      <c r="K50" s="26" t="s">
+        <v>361</v>
       </c>
     </row>
     <row r="51" spans="1:11" ht="15">
       <c r="C51" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="D51" s="27" t="s">
+        <v>174</v>
+      </c>
+      <c r="D51" s="24" t="s">
+        <v>205</v>
+      </c>
+      <c r="E51" s="36" t="s">
+        <v>206</v>
+      </c>
+      <c r="F51" t="s">
+        <v>207</v>
+      </c>
+      <c r="G51" t="s">
         <v>208</v>
       </c>
-      <c r="E51" t="s">
-        <v>209</v>
-      </c>
-      <c r="F51" t="s">
-        <v>210</v>
-      </c>
-      <c r="G51" t="s">
-        <v>211</v>
-      </c>
-      <c r="I51" s="22" t="s">
-        <v>353</v>
+      <c r="I51" s="19" t="s">
+        <v>350</v>
       </c>
       <c r="J51" s="16" t="s">
-        <v>343</v>
-      </c>
-      <c r="K51" s="29" t="s">
-        <v>364</v>
+        <v>340</v>
+      </c>
+      <c r="K51" s="26" t="s">
+        <v>361</v>
       </c>
     </row>
     <row r="52" spans="1:11" ht="15">
       <c r="C52" s="8" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D52" t="s">
+        <v>209</v>
+      </c>
+      <c r="E52" s="36" t="s">
+        <v>210</v>
+      </c>
+      <c r="F52" t="s">
+        <v>211</v>
+      </c>
+      <c r="G52" t="s">
         <v>212</v>
       </c>
-      <c r="E52" t="s">
-        <v>213</v>
-      </c>
-      <c r="F52" t="s">
-        <v>214</v>
-      </c>
-      <c r="G52" t="s">
-        <v>215</v>
-      </c>
-      <c r="I52" s="22" t="s">
-        <v>353</v>
+      <c r="I52" s="19" t="s">
+        <v>350</v>
       </c>
       <c r="J52" t="s">
-        <v>344</v>
-      </c>
-      <c r="K52" s="29" t="s">
-        <v>364</v>
+        <v>341</v>
+      </c>
+      <c r="K52" s="26" t="s">
+        <v>361</v>
       </c>
     </row>
     <row r="53" spans="1:11" ht="15">
       <c r="B53" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D53" t="s">
+        <v>184</v>
+      </c>
+      <c r="E53" s="36" t="s">
+        <v>185</v>
+      </c>
+      <c r="F53" t="s">
+        <v>186</v>
+      </c>
+      <c r="G53" t="s">
         <v>187</v>
       </c>
-      <c r="E53" t="s">
-        <v>188</v>
-      </c>
-      <c r="F53" t="s">
-        <v>189</v>
-      </c>
-      <c r="G53" t="s">
-        <v>190</v>
-      </c>
       <c r="I53" s="17" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="J53" s="16" t="s">
-        <v>343</v>
-      </c>
-      <c r="K53" s="29" t="s">
-        <v>363</v>
+        <v>340</v>
+      </c>
+      <c r="K53" s="26" t="s">
+        <v>360</v>
       </c>
     </row>
     <row r="54" spans="1:11" ht="15">
       <c r="C54" s="8" t="s">
-        <v>180</v>
-      </c>
-      <c r="D54" s="27" t="s">
+        <v>177</v>
+      </c>
+      <c r="D54" s="24" t="s">
+        <v>189</v>
+      </c>
+      <c r="E54" s="36" t="s">
+        <v>190</v>
+      </c>
+      <c r="F54" t="s">
+        <v>191</v>
+      </c>
+      <c r="G54" t="s">
         <v>192</v>
       </c>
-      <c r="E54" t="s">
-        <v>193</v>
-      </c>
-      <c r="F54" t="s">
-        <v>194</v>
-      </c>
-      <c r="G54" t="s">
-        <v>195</v>
-      </c>
-      <c r="I54" s="22" t="s">
-        <v>353</v>
+      <c r="I54" s="19" t="s">
+        <v>350</v>
       </c>
       <c r="J54" s="16" t="s">
-        <v>343</v>
-      </c>
-      <c r="K54" s="29" t="s">
-        <v>363</v>
+        <v>340</v>
+      </c>
+      <c r="K54" s="26" t="s">
+        <v>360</v>
       </c>
     </row>
     <row r="55" spans="1:11" ht="15">
       <c r="C55" s="8" t="s">
-        <v>181</v>
-      </c>
-      <c r="D55" t="s">
+        <v>178</v>
+      </c>
+      <c r="D55" s="27" t="s">
+        <v>193</v>
+      </c>
+      <c r="E55" s="36" t="s">
+        <v>194</v>
+      </c>
+      <c r="F55" t="s">
+        <v>195</v>
+      </c>
+      <c r="G55" t="s">
         <v>196</v>
       </c>
-      <c r="E55" t="s">
-        <v>197</v>
-      </c>
-      <c r="F55" t="s">
-        <v>198</v>
-      </c>
-      <c r="G55" t="s">
-        <v>199</v>
-      </c>
-      <c r="I55" s="22" t="s">
-        <v>353</v>
+      <c r="I55" s="19" t="s">
+        <v>350</v>
       </c>
       <c r="J55" t="s">
-        <v>344</v>
-      </c>
-      <c r="K55" s="29" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" ht="15">
+        <v>341</v>
+      </c>
+      <c r="K55" s="26" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" ht="25">
       <c r="B56" t="s">
+        <v>213</v>
+      </c>
+      <c r="C56" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="D56" s="24" t="s">
+        <v>214</v>
+      </c>
+      <c r="E56" s="36" t="s">
+        <v>215</v>
+      </c>
+      <c r="F56" t="s">
         <v>216</v>
       </c>
-      <c r="C56" s="8" t="s">
-        <v>182</v>
-      </c>
-      <c r="D56" s="27" t="s">
+      <c r="G56" t="s">
         <v>217</v>
       </c>
-      <c r="E56" t="s">
+      <c r="I56" s="19" t="s">
+        <v>350</v>
+      </c>
+      <c r="J56" s="16" t="s">
+        <v>340</v>
+      </c>
+      <c r="K56" s="26" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" ht="25">
+      <c r="C57" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="D57" t="s">
         <v>218</v>
       </c>
-      <c r="F56" t="s">
-        <v>219</v>
-      </c>
-      <c r="G56" t="s">
-        <v>220</v>
-      </c>
-      <c r="I56" s="22" t="s">
-        <v>353</v>
-      </c>
-      <c r="J56" s="16" t="s">
-        <v>343</v>
-      </c>
-      <c r="K56" s="29" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" ht="15">
-      <c r="C57" s="8" t="s">
-        <v>183</v>
-      </c>
-      <c r="D57" t="s">
-        <v>221</v>
-      </c>
-      <c r="E57" t="s">
-        <v>225</v>
+      <c r="E57" s="36" t="s">
+        <v>222</v>
       </c>
       <c r="F57" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="G57" t="s">
-        <v>227</v>
-      </c>
-      <c r="I57" s="22" t="s">
-        <v>353</v>
+        <v>224</v>
+      </c>
+      <c r="I57" s="19" t="s">
+        <v>350</v>
       </c>
       <c r="J57" t="s">
-        <v>344</v>
-      </c>
-      <c r="K57" s="29" t="s">
-        <v>364</v>
+        <v>341</v>
+      </c>
+      <c r="K57" s="26" t="s">
+        <v>361</v>
       </c>
     </row>
     <row r="58" spans="1:11" ht="15">
       <c r="C58" s="8" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D58" t="s">
-        <v>223</v>
-      </c>
-      <c r="E58" t="s">
-        <v>224</v>
+        <v>220</v>
+      </c>
+      <c r="E58" s="36" t="s">
+        <v>221</v>
       </c>
       <c r="F58" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G58" t="s">
-        <v>164</v>
-      </c>
-      <c r="I58" s="21" t="s">
-        <v>352</v>
-      </c>
-      <c r="K58" s="29" t="s">
-        <v>363</v>
+        <v>161</v>
+      </c>
+      <c r="I58" s="18" t="s">
+        <v>349</v>
+      </c>
+      <c r="K58" s="26" t="s">
+        <v>360</v>
       </c>
     </row>
     <row r="59" spans="1:11" ht="12">
       <c r="C59" s="1"/>
+      <c r="E59" s="36"/>
     </row>
     <row r="60" spans="1:11" ht="12">
       <c r="C60" s="1"/>
+      <c r="E60" s="36"/>
     </row>
     <row r="61" spans="1:11" ht="12">
       <c r="C61" s="1"/>
+      <c r="E61" s="36"/>
     </row>
     <row r="62" spans="1:11" ht="25">
       <c r="A62" s="15" t="s">
+        <v>225</v>
+      </c>
+      <c r="B62" s="21" t="s">
+        <v>226</v>
+      </c>
+      <c r="C62" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="D62" t="s">
+        <v>241</v>
+      </c>
+      <c r="E62" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="F62" t="s">
+        <v>43</v>
+      </c>
+      <c r="G62" t="s">
+        <v>161</v>
+      </c>
+      <c r="I62" s="18" t="s">
+        <v>349</v>
+      </c>
+      <c r="K62" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" ht="37">
+      <c r="A63" s="21" t="s">
+        <v>227</v>
+      </c>
+      <c r="C63" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="D63" s="24" t="s">
+        <v>242</v>
+      </c>
+      <c r="E63" s="36" t="s">
+        <v>243</v>
+      </c>
+      <c r="F63" t="s">
+        <v>244</v>
+      </c>
+      <c r="I63" s="19" t="s">
+        <v>350</v>
+      </c>
+      <c r="J63" s="16" t="s">
+        <v>340</v>
+      </c>
+      <c r="K63" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" ht="37">
+      <c r="A64" s="21" t="s">
         <v>228</v>
       </c>
-      <c r="B62" s="24" t="s">
-        <v>229</v>
-      </c>
-      <c r="C62" s="8" t="s">
-        <v>232</v>
-      </c>
-      <c r="D62" t="s">
-        <v>244</v>
-      </c>
-      <c r="E62" t="s">
-        <v>72</v>
-      </c>
-      <c r="F62" t="s">
-        <v>44</v>
-      </c>
-      <c r="G62" t="s">
-        <v>164</v>
-      </c>
-      <c r="I62" s="21" t="s">
-        <v>352</v>
-      </c>
-      <c r="K62" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11" ht="37">
-      <c r="A63" s="24" t="s">
-        <v>230</v>
-      </c>
-      <c r="C63" s="8" t="s">
-        <v>233</v>
-      </c>
-      <c r="D63" s="27" t="s">
+      <c r="C64" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="D64" t="s">
         <v>245</v>
       </c>
-      <c r="E63" t="s">
+      <c r="E64" s="36" t="s">
         <v>246</v>
       </c>
-      <c r="F63" t="s">
+      <c r="F64" t="s">
         <v>247</v>
       </c>
-      <c r="I63" s="22" t="s">
-        <v>353</v>
-      </c>
-      <c r="J63" s="16" t="s">
-        <v>343</v>
-      </c>
-      <c r="K63" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11" ht="37">
-      <c r="A64" s="24" t="s">
-        <v>231</v>
-      </c>
-      <c r="C64" s="8" t="s">
-        <v>234</v>
-      </c>
-      <c r="D64" t="s">
-        <v>248</v>
-      </c>
-      <c r="E64" t="s">
-        <v>249</v>
-      </c>
-      <c r="F64" t="s">
-        <v>250</v>
-      </c>
-      <c r="I64" s="22" t="s">
-        <v>353</v>
+      <c r="I64" s="19" t="s">
+        <v>350</v>
       </c>
       <c r="J64" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="K64" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="65" spans="1:11" ht="15">
       <c r="C65" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="D65" t="s">
+        <v>248</v>
+      </c>
+      <c r="E65" s="36" t="s">
+        <v>249</v>
+      </c>
+      <c r="F65" t="s">
+        <v>250</v>
+      </c>
+      <c r="I65" s="19" t="s">
+        <v>350</v>
+      </c>
+      <c r="J65" t="s">
+        <v>341</v>
+      </c>
+      <c r="K65" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" ht="49">
+      <c r="B66" t="s">
+        <v>253</v>
+      </c>
+      <c r="C66" s="8" t="s">
+        <v>233</v>
+      </c>
+      <c r="D66" t="s">
+        <v>251</v>
+      </c>
+      <c r="E66" s="36" t="s">
+        <v>252</v>
+      </c>
+      <c r="F66" t="s">
+        <v>254</v>
+      </c>
+      <c r="G66" t="s">
+        <v>255</v>
+      </c>
+      <c r="I66" s="19" t="s">
+        <v>350</v>
+      </c>
+      <c r="J66" t="s">
+        <v>343</v>
+      </c>
+      <c r="K66" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" ht="25">
+      <c r="C67" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="D67" s="24" t="s">
+        <v>256</v>
+      </c>
+      <c r="E67" s="36" t="s">
+        <v>257</v>
+      </c>
+      <c r="F67" t="s">
+        <v>258</v>
+      </c>
+      <c r="G67" t="s">
+        <v>259</v>
+      </c>
+      <c r="I67" s="19" t="s">
+        <v>350</v>
+      </c>
+      <c r="J67" t="s">
+        <v>340</v>
+      </c>
+      <c r="K67" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" ht="37">
+      <c r="C68" s="8" t="s">
         <v>235</v>
       </c>
-      <c r="D65" t="s">
-        <v>251</v>
-      </c>
-      <c r="E65" t="s">
-        <v>252</v>
-      </c>
-      <c r="F65" t="s">
-        <v>253</v>
-      </c>
-      <c r="I65" s="22" t="s">
-        <v>353</v>
-      </c>
-      <c r="J65" t="s">
-        <v>344</v>
-      </c>
-      <c r="K65" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11" ht="15">
-      <c r="B66" t="s">
-        <v>256</v>
-      </c>
-      <c r="C66" s="8" t="s">
+      <c r="D68" s="27" t="s">
+        <v>260</v>
+      </c>
+      <c r="E68" s="36" t="s">
+        <v>261</v>
+      </c>
+      <c r="F68" t="s">
+        <v>247</v>
+      </c>
+      <c r="G68" t="s">
+        <v>262</v>
+      </c>
+      <c r="I68" s="19" t="s">
+        <v>350</v>
+      </c>
+      <c r="J68" t="s">
+        <v>340</v>
+      </c>
+      <c r="K68" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" ht="25">
+      <c r="C69" s="8" t="s">
         <v>236</v>
       </c>
-      <c r="D66" t="s">
-        <v>254</v>
-      </c>
-      <c r="E66" t="s">
-        <v>255</v>
-      </c>
-      <c r="F66" t="s">
-        <v>257</v>
-      </c>
-      <c r="G66" t="s">
-        <v>258</v>
-      </c>
-      <c r="I66" s="22" t="s">
-        <v>353</v>
-      </c>
-      <c r="J66" t="s">
-        <v>346</v>
-      </c>
-      <c r="K66" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" ht="15">
-      <c r="C67" s="8" t="s">
+      <c r="D69" s="24" t="s">
+        <v>263</v>
+      </c>
+      <c r="E69" s="36" t="s">
+        <v>264</v>
+      </c>
+      <c r="F69" t="s">
+        <v>265</v>
+      </c>
+      <c r="G69" t="s">
+        <v>266</v>
+      </c>
+      <c r="I69" s="19" t="s">
+        <v>350</v>
+      </c>
+      <c r="J69" t="s">
+        <v>340</v>
+      </c>
+      <c r="K69" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" ht="25">
+      <c r="C70" s="8" t="s">
         <v>237</v>
       </c>
-      <c r="D67" s="27" t="s">
-        <v>259</v>
-      </c>
-      <c r="E67" t="s">
-        <v>260</v>
-      </c>
-      <c r="F67" t="s">
-        <v>261</v>
-      </c>
-      <c r="G67" t="s">
-        <v>262</v>
-      </c>
-      <c r="I67" s="22" t="s">
-        <v>353</v>
-      </c>
-      <c r="J67" t="s">
-        <v>343</v>
-      </c>
-      <c r="K67" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11" ht="15">
-      <c r="C68" s="8" t="s">
+      <c r="D70" s="27" t="s">
+        <v>267</v>
+      </c>
+      <c r="E70" s="36" t="s">
+        <v>269</v>
+      </c>
+      <c r="F70" t="s">
+        <v>268</v>
+      </c>
+      <c r="G70" t="s">
+        <v>270</v>
+      </c>
+      <c r="I70" s="19" t="s">
+        <v>350</v>
+      </c>
+      <c r="J70" t="s">
+        <v>341</v>
+      </c>
+      <c r="K70" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" ht="25">
+      <c r="B71" t="s">
+        <v>271</v>
+      </c>
+      <c r="C71" s="8" t="s">
         <v>238</v>
       </c>
-      <c r="D68" t="s">
-        <v>263</v>
-      </c>
-      <c r="E68" t="s">
-        <v>264</v>
-      </c>
-      <c r="F68" t="s">
-        <v>250</v>
-      </c>
-      <c r="G68" t="s">
-        <v>265</v>
-      </c>
-      <c r="I68" s="22" t="s">
-        <v>353</v>
-      </c>
-      <c r="J68" t="s">
-        <v>343</v>
-      </c>
-      <c r="K68" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11" ht="15">
-      <c r="C69" s="8" t="s">
+      <c r="D71" s="27" t="s">
+        <v>272</v>
+      </c>
+      <c r="E71" s="36" t="s">
+        <v>273</v>
+      </c>
+      <c r="F71" t="s">
+        <v>274</v>
+      </c>
+      <c r="G71" t="s">
+        <v>275</v>
+      </c>
+      <c r="I71" s="19" t="s">
+        <v>350</v>
+      </c>
+      <c r="J71" t="s">
+        <v>342</v>
+      </c>
+      <c r="K71" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" ht="25">
+      <c r="C72" s="8" t="s">
         <v>239</v>
       </c>
-      <c r="D69" s="27" t="s">
-        <v>266</v>
-      </c>
-      <c r="E69" t="s">
-        <v>267</v>
-      </c>
-      <c r="F69" t="s">
-        <v>268</v>
-      </c>
-      <c r="G69" t="s">
-        <v>269</v>
-      </c>
-      <c r="I69" s="22" t="s">
-        <v>353</v>
-      </c>
-      <c r="J69" t="s">
-        <v>343</v>
-      </c>
-      <c r="K69" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="70" spans="1:11" ht="15">
-      <c r="C70" s="8" t="s">
-        <v>240</v>
-      </c>
-      <c r="D70" t="s">
-        <v>270</v>
-      </c>
-      <c r="E70" t="s">
-        <v>272</v>
-      </c>
-      <c r="F70" t="s">
-        <v>271</v>
-      </c>
-      <c r="G70" t="s">
-        <v>273</v>
-      </c>
-      <c r="I70" s="22" t="s">
-        <v>353</v>
-      </c>
-      <c r="J70" t="s">
-        <v>344</v>
-      </c>
-      <c r="K70" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="71" spans="1:11" ht="15">
-      <c r="B71" t="s">
-        <v>274</v>
-      </c>
-      <c r="C71" s="8" t="s">
-        <v>241</v>
-      </c>
-      <c r="D71" t="s">
-        <v>275</v>
-      </c>
-      <c r="E71" t="s">
+      <c r="D72" s="24" t="s">
         <v>276</v>
       </c>
-      <c r="F71" t="s">
+      <c r="E72" s="36" t="s">
         <v>277</v>
       </c>
-      <c r="G71" t="s">
+      <c r="F72" t="s">
         <v>278</v>
       </c>
-      <c r="I71" s="22" t="s">
-        <v>353</v>
-      </c>
-      <c r="J71" t="s">
-        <v>345</v>
-      </c>
-      <c r="K71" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11" ht="15">
-      <c r="C72" s="8" t="s">
-        <v>242</v>
-      </c>
-      <c r="D72" s="27" t="s">
+      <c r="G72" t="s">
         <v>279</v>
       </c>
-      <c r="E72" t="s">
-        <v>280</v>
-      </c>
-      <c r="F72" t="s">
-        <v>281</v>
-      </c>
-      <c r="G72" t="s">
-        <v>282</v>
-      </c>
-      <c r="I72" s="22" t="s">
-        <v>353</v>
+      <c r="I72" s="19" t="s">
+        <v>350</v>
       </c>
       <c r="J72" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="K72" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="73" spans="1:11" ht="15">
       <c r="C73" s="8" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="D73" t="s">
-        <v>283</v>
-      </c>
-      <c r="E73" t="s">
-        <v>284</v>
+        <v>280</v>
+      </c>
+      <c r="E73" s="36" t="s">
+        <v>281</v>
       </c>
       <c r="F73" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G73" t="s">
-        <v>164</v>
-      </c>
-      <c r="I73" s="21" t="s">
-        <v>352</v>
+        <v>161</v>
+      </c>
+      <c r="I73" s="18" t="s">
+        <v>349</v>
       </c>
       <c r="K73" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
     </row>
     <row r="74" spans="1:11" ht="12">
       <c r="C74" s="8"/>
+      <c r="E74" s="36"/>
     </row>
     <row r="75" spans="1:11" ht="12">
       <c r="C75" s="1"/>
+      <c r="E75" s="36"/>
     </row>
     <row r="76" spans="1:11" ht="12">
       <c r="C76" s="1"/>
+      <c r="E76" s="36"/>
     </row>
     <row r="77" spans="1:11" ht="15">
       <c r="A77" s="15" t="s">
+        <v>282</v>
+      </c>
+      <c r="B77" t="s">
+        <v>297</v>
+      </c>
+      <c r="C77" s="8" t="s">
         <v>285</v>
       </c>
-      <c r="B77" t="s">
+      <c r="D77" t="s">
+        <v>298</v>
+      </c>
+      <c r="E77" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="F77" t="s">
+        <v>43</v>
+      </c>
+      <c r="G77" t="s">
+        <v>161</v>
+      </c>
+      <c r="I77" s="18" t="s">
+        <v>349</v>
+      </c>
+      <c r="K77" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" ht="25">
+      <c r="A78" s="21" t="s">
+        <v>283</v>
+      </c>
+      <c r="C78" s="8" t="s">
+        <v>286</v>
+      </c>
+      <c r="D78" s="24" t="s">
+        <v>299</v>
+      </c>
+      <c r="E78" s="36" t="s">
         <v>300</v>
       </c>
-      <c r="C77" s="8" t="s">
+      <c r="F78" t="s">
+        <v>301</v>
+      </c>
+      <c r="G78" t="s">
+        <v>302</v>
+      </c>
+      <c r="I78" s="19" t="s">
+        <v>350</v>
+      </c>
+      <c r="J78" t="s">
+        <v>340</v>
+      </c>
+      <c r="K78" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" ht="25">
+      <c r="A79" s="21" t="s">
+        <v>284</v>
+      </c>
+      <c r="C79" s="8" t="s">
+        <v>287</v>
+      </c>
+      <c r="D79" t="s">
+        <v>303</v>
+      </c>
+      <c r="E79" s="36" t="s">
+        <v>304</v>
+      </c>
+      <c r="F79" t="s">
+        <v>305</v>
+      </c>
+      <c r="G79" t="s">
+        <v>306</v>
+      </c>
+      <c r="I79" s="17" t="s">
+        <v>346</v>
+      </c>
+      <c r="J79" t="s">
+        <v>344</v>
+      </c>
+      <c r="K79" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" ht="25">
+      <c r="B80" t="s">
+        <v>307</v>
+      </c>
+      <c r="C80" s="8" t="s">
         <v>288</v>
       </c>
-      <c r="D77" t="s">
-        <v>301</v>
-      </c>
-      <c r="E77" t="s">
-        <v>72</v>
-      </c>
-      <c r="F77" t="s">
-        <v>44</v>
-      </c>
-      <c r="G77" t="s">
-        <v>164</v>
-      </c>
-      <c r="I77" s="21" t="s">
-        <v>352</v>
-      </c>
-      <c r="K77" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="78" spans="1:11" ht="25">
-      <c r="A78" s="24" t="s">
-        <v>286</v>
-      </c>
-      <c r="C78" s="8" t="s">
+      <c r="D80" t="s">
+        <v>311</v>
+      </c>
+      <c r="E80" s="36" t="s">
+        <v>308</v>
+      </c>
+      <c r="F80" t="s">
+        <v>309</v>
+      </c>
+      <c r="G80" t="s">
+        <v>310</v>
+      </c>
+      <c r="I80" s="17" t="s">
+        <v>346</v>
+      </c>
+      <c r="J80" t="s">
+        <v>340</v>
+      </c>
+      <c r="K80" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="81" spans="2:11" ht="25">
+      <c r="C81" s="8" t="s">
         <v>289</v>
       </c>
-      <c r="D78" s="27" t="s">
-        <v>302</v>
-      </c>
-      <c r="E78" t="s">
-        <v>303</v>
-      </c>
-      <c r="F78" t="s">
-        <v>304</v>
-      </c>
-      <c r="G78" t="s">
-        <v>305</v>
-      </c>
-      <c r="I78" s="22" t="s">
-        <v>353</v>
-      </c>
-      <c r="J78" t="s">
-        <v>343</v>
-      </c>
-      <c r="K78" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="79" spans="1:11" ht="25">
-      <c r="A79" s="24" t="s">
-        <v>287</v>
-      </c>
-      <c r="C79" s="8" t="s">
-        <v>290</v>
-      </c>
-      <c r="D79" t="s">
+      <c r="D81" s="24" t="s">
+        <v>312</v>
+      </c>
+      <c r="E81" s="36" t="s">
+        <v>313</v>
+      </c>
+      <c r="F81" t="s">
+        <v>314</v>
+      </c>
+      <c r="G81" t="s">
         <v>306</v>
       </c>
-      <c r="E79" t="s">
-        <v>307</v>
-      </c>
-      <c r="F79" t="s">
-        <v>308</v>
-      </c>
-      <c r="G79" t="s">
-        <v>309</v>
-      </c>
-      <c r="I79" s="17" t="s">
-        <v>349</v>
-      </c>
-      <c r="J79" t="s">
-        <v>347</v>
-      </c>
-      <c r="K79" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="80" spans="1:11" ht="15">
-      <c r="B80" t="s">
-        <v>310</v>
-      </c>
-      <c r="C80" s="8" t="s">
-        <v>291</v>
-      </c>
-      <c r="D80" t="s">
-        <v>314</v>
-      </c>
-      <c r="E80" t="s">
-        <v>311</v>
-      </c>
-      <c r="F80" t="s">
-        <v>312</v>
-      </c>
-      <c r="G80" t="s">
-        <v>313</v>
-      </c>
-      <c r="I80" s="17" t="s">
-        <v>349</v>
-      </c>
-      <c r="J80" t="s">
-        <v>343</v>
-      </c>
-      <c r="K80" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="81" spans="2:11" ht="15">
-      <c r="C81" s="8" t="s">
-        <v>292</v>
-      </c>
-      <c r="D81" s="27" t="s">
-        <v>315</v>
-      </c>
-      <c r="E81" t="s">
-        <v>316</v>
-      </c>
-      <c r="F81" t="s">
-        <v>317</v>
-      </c>
-      <c r="G81" t="s">
-        <v>309</v>
-      </c>
-      <c r="I81" s="22" t="s">
-        <v>353</v>
+      <c r="I81" s="19" t="s">
+        <v>350</v>
       </c>
       <c r="J81" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="K81" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="82" spans="2:11" ht="15">
       <c r="C82" s="8" t="s">
+        <v>290</v>
+      </c>
+      <c r="D82" s="27" t="s">
+        <v>315</v>
+      </c>
+      <c r="E82" s="36" t="s">
+        <v>316</v>
+      </c>
+      <c r="F82" t="s">
+        <v>317</v>
+      </c>
+      <c r="G82" t="s">
+        <v>318</v>
+      </c>
+      <c r="I82" s="19" t="s">
+        <v>350</v>
+      </c>
+      <c r="J82" t="s">
+        <v>341</v>
+      </c>
+      <c r="K82" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="83" spans="2:11" ht="25">
+      <c r="B83" t="s">
+        <v>347</v>
+      </c>
+      <c r="C83" s="8" t="s">
+        <v>291</v>
+      </c>
+      <c r="D83" s="24" t="s">
+        <v>352</v>
+      </c>
+      <c r="E83" s="36" t="s">
+        <v>321</v>
+      </c>
+      <c r="F83" t="s">
+        <v>319</v>
+      </c>
+      <c r="G83" t="s">
+        <v>320</v>
+      </c>
+      <c r="I83" s="19" t="s">
+        <v>350</v>
+      </c>
+      <c r="J83" t="s">
+        <v>340</v>
+      </c>
+      <c r="K83" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="84" spans="2:11" ht="37">
+      <c r="C84" s="8" t="s">
+        <v>292</v>
+      </c>
+      <c r="D84" t="s">
+        <v>355</v>
+      </c>
+      <c r="E84" s="36" t="s">
+        <v>356</v>
+      </c>
+      <c r="F84" t="s">
+        <v>322</v>
+      </c>
+      <c r="G84" t="s">
+        <v>323</v>
+      </c>
+      <c r="I84" s="18" t="s">
+        <v>349</v>
+      </c>
+      <c r="J84" t="s">
+        <v>342</v>
+      </c>
+      <c r="K84" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="85" spans="2:11" ht="25">
+      <c r="C85" s="8" t="s">
         <v>293</v>
       </c>
-      <c r="D82" t="s">
-        <v>318</v>
-      </c>
-      <c r="E82" t="s">
-        <v>319</v>
-      </c>
-      <c r="F82" t="s">
-        <v>320</v>
-      </c>
-      <c r="G82" t="s">
-        <v>321</v>
-      </c>
-      <c r="I82" s="22" t="s">
+      <c r="D85" t="s">
+        <v>354</v>
+      </c>
+      <c r="E85" s="36" t="s">
+        <v>357</v>
+      </c>
+      <c r="I85" s="18" t="s">
+        <v>349</v>
+      </c>
+      <c r="K85" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="86" spans="2:11" ht="37">
+      <c r="C86" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="D86" s="27" t="s">
+        <v>324</v>
+      </c>
+      <c r="E86" s="36" t="s">
+        <v>325</v>
+      </c>
+      <c r="F86" t="s">
+        <v>326</v>
+      </c>
+      <c r="G86" t="s">
+        <v>327</v>
+      </c>
+      <c r="I86" s="19" t="s">
+        <v>350</v>
+      </c>
+      <c r="J86" t="s">
+        <v>343</v>
+      </c>
+      <c r="K86" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="87" spans="2:11" ht="25">
+      <c r="B87" t="s">
+        <v>337</v>
+      </c>
+      <c r="C87" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="D87" s="24" t="s">
+        <v>328</v>
+      </c>
+      <c r="E87" s="36" t="s">
+        <v>329</v>
+      </c>
+      <c r="F87" t="s">
+        <v>330</v>
+      </c>
+      <c r="G87" t="s">
+        <v>331</v>
+      </c>
+      <c r="I87" s="19" t="s">
+        <v>350</v>
+      </c>
+      <c r="J87" t="s">
+        <v>342</v>
+      </c>
+      <c r="K87" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="88" spans="2:11" ht="25">
+      <c r="C88" s="8" t="s">
+        <v>296</v>
+      </c>
+      <c r="D88" t="s">
+        <v>332</v>
+      </c>
+      <c r="E88" s="36" t="s">
+        <v>333</v>
+      </c>
+      <c r="F88" t="s">
+        <v>334</v>
+      </c>
+      <c r="G88" t="s">
+        <v>339</v>
+      </c>
+      <c r="I88" s="19" t="s">
+        <v>350</v>
+      </c>
+      <c r="J88" t="s">
+        <v>343</v>
+      </c>
+      <c r="K88" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="89" spans="2:11" ht="25">
+      <c r="C89" s="8" t="s">
         <v>353</v>
       </c>
-      <c r="J82" t="s">
-        <v>344</v>
-      </c>
-      <c r="K82" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="83" spans="2:11" ht="15">
-      <c r="B83" t="s">
-        <v>350</v>
-      </c>
-      <c r="C83" s="8" t="s">
-        <v>294</v>
-      </c>
-      <c r="D83" s="27" t="s">
-        <v>355</v>
-      </c>
-      <c r="E83" t="s">
-        <v>324</v>
-      </c>
-      <c r="F83" t="s">
-        <v>322</v>
-      </c>
-      <c r="G83" t="s">
-        <v>323</v>
-      </c>
-      <c r="I83" s="22" t="s">
-        <v>353</v>
-      </c>
-      <c r="J83" t="s">
-        <v>343</v>
-      </c>
-      <c r="K83" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="84" spans="2:11" ht="15">
-      <c r="C84" s="8" t="s">
-        <v>295</v>
-      </c>
-      <c r="D84" t="s">
-        <v>358</v>
-      </c>
-      <c r="E84" t="s">
+      <c r="D89" t="s">
+        <v>336</v>
+      </c>
+      <c r="E89" s="36" t="s">
+        <v>338</v>
+      </c>
+      <c r="F89" t="s">
+        <v>43</v>
+      </c>
+      <c r="G89" t="s">
+        <v>335</v>
+      </c>
+      <c r="I89" s="18" t="s">
+        <v>349</v>
+      </c>
+      <c r="K89" t="s">
         <v>359</v>
-      </c>
-      <c r="F84" t="s">
-        <v>325</v>
-      </c>
-      <c r="G84" t="s">
-        <v>326</v>
-      </c>
-      <c r="I84" s="21" t="s">
-        <v>352</v>
-      </c>
-      <c r="J84" t="s">
-        <v>345</v>
-      </c>
-      <c r="K84" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="85" spans="2:11" ht="15">
-      <c r="C85" s="8" t="s">
-        <v>296</v>
-      </c>
-      <c r="D85" t="s">
-        <v>357</v>
-      </c>
-      <c r="E85" t="s">
-        <v>360</v>
-      </c>
-      <c r="I85" s="21" t="s">
-        <v>352</v>
-      </c>
-      <c r="K85" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="86" spans="2:11" ht="15">
-      <c r="C86" s="8" t="s">
-        <v>297</v>
-      </c>
-      <c r="D86" t="s">
-        <v>327</v>
-      </c>
-      <c r="E86" t="s">
-        <v>328</v>
-      </c>
-      <c r="F86" t="s">
-        <v>329</v>
-      </c>
-      <c r="G86" t="s">
-        <v>330</v>
-      </c>
-      <c r="I86" s="22" t="s">
-        <v>353</v>
-      </c>
-      <c r="J86" t="s">
-        <v>346</v>
-      </c>
-      <c r="K86" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="87" spans="2:11" ht="15">
-      <c r="B87" t="s">
-        <v>340</v>
-      </c>
-      <c r="C87" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="D87" s="27" t="s">
-        <v>331</v>
-      </c>
-      <c r="E87" t="s">
-        <v>332</v>
-      </c>
-      <c r="F87" t="s">
-        <v>333</v>
-      </c>
-      <c r="G87" t="s">
-        <v>334</v>
-      </c>
-      <c r="I87" s="22" t="s">
-        <v>353</v>
-      </c>
-      <c r="J87" t="s">
-        <v>345</v>
-      </c>
-      <c r="K87" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="88" spans="2:11" ht="15">
-      <c r="C88" s="8" t="s">
-        <v>299</v>
-      </c>
-      <c r="D88" t="s">
-        <v>335</v>
-      </c>
-      <c r="E88" t="s">
-        <v>336</v>
-      </c>
-      <c r="F88" t="s">
-        <v>337</v>
-      </c>
-      <c r="G88" t="s">
-        <v>342</v>
-      </c>
-      <c r="I88" s="22" t="s">
-        <v>353</v>
-      </c>
-      <c r="J88" t="s">
-        <v>346</v>
-      </c>
-      <c r="K88" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="89" spans="2:11" ht="15">
-      <c r="C89" s="8" t="s">
-        <v>356</v>
-      </c>
-      <c r="D89" t="s">
-        <v>339</v>
-      </c>
-      <c r="E89" t="s">
-        <v>341</v>
-      </c>
-      <c r="F89" t="s">
-        <v>44</v>
-      </c>
-      <c r="G89" t="s">
-        <v>338</v>
-      </c>
-      <c r="I89" s="21" t="s">
-        <v>352</v>
-      </c>
-      <c r="K89" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="90" spans="2:11" ht="12">

</xml_diff>

<commit_message>
Added Parsec quiz and Monad Metaphor forum
</commit_message>
<xml_diff>
--- a/fl_course_outline_weeks.xlsx
+++ b/fl_course_outline_weeks.xlsx
@@ -1331,7 +1331,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="310">
+  <cellStyleXfs count="314">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1642,8 +1642,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1735,6 +1739,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1745,7 +1755,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="310">
+  <cellStyles count="314">
     <cellStyle name="Bad" xfId="150" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -1900,6 +1910,8 @@
     <cellStyle name="Followed Hyperlink" xfId="305" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="307" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="309" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="311" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="313" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="55" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -2054,6 +2066,8 @@
     <cellStyle name="Hyperlink" xfId="304" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="306" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="308" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="310" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="312" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="151" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -2330,13 +2344,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:L1004"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="D35" sqref="D35"/>
+      <selection pane="bottomLeft" activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -2386,7 +2399,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="49" hidden="1" customHeight="1">
+    <row r="2" spans="1:11" ht="49" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -2416,7 +2429,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15.75" customHeight="1">
+    <row r="3" spans="1:11" ht="29" customHeight="1">
       <c r="A3" s="11" t="s">
         <v>55</v>
       </c>
@@ -2427,7 +2440,7 @@
       <c r="D3" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="28" t="s">
+      <c r="E3" s="39" t="s">
         <v>32</v>
       </c>
       <c r="F3" s="3" t="s">
@@ -2479,7 +2492,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="41" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="3"/>
@@ -2510,7 +2523,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A6" s="40"/>
+      <c r="A6" s="42"/>
       <c r="B6" s="5"/>
       <c r="C6" s="7">
         <v>1.5</v>
@@ -2538,8 +2551,8 @@
         <v>359</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A7" s="41"/>
+    <row r="7" spans="1:11" ht="31" customHeight="1">
+      <c r="A7" s="43"/>
       <c r="B7" s="5" t="s">
         <v>18</v>
       </c>
@@ -2549,7 +2562,7 @@
       <c r="D7" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="28" t="s">
+      <c r="E7" s="39" t="s">
         <v>36</v>
       </c>
       <c r="F7" s="3" t="s">
@@ -2656,7 +2669,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15.75" hidden="1" customHeight="1">
+    <row r="11" spans="1:11" ht="15.75" customHeight="1">
       <c r="A11" s="3"/>
       <c r="B11" s="3" t="s">
         <v>21</v>
@@ -2687,7 +2700,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="15.75" hidden="1" customHeight="1">
+    <row r="12" spans="1:11" ht="15.75" customHeight="1">
       <c r="A12" s="3"/>
       <c r="B12" s="5"/>
       <c r="C12" s="8" t="s">
@@ -2716,7 +2729,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="15.75" hidden="1" customHeight="1">
+    <row r="13" spans="1:11" ht="15.75" customHeight="1">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="8" t="s">
@@ -2742,7 +2755,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="15.75" hidden="1" customHeight="1">
+    <row r="14" spans="1:11" ht="15.75" customHeight="1">
       <c r="A14" s="3"/>
       <c r="B14" s="5"/>
       <c r="C14" s="3"/>
@@ -2752,7 +2765,7 @@
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
     </row>
-    <row r="15" spans="1:11" ht="15.75" hidden="1" customHeight="1">
+    <row r="15" spans="1:11" ht="15.75" customHeight="1">
       <c r="A15" s="3"/>
       <c r="B15" s="5"/>
       <c r="C15" s="9"/>
@@ -2762,7 +2775,7 @@
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
     </row>
-    <row r="16" spans="1:11" ht="15.75" hidden="1" customHeight="1">
+    <row r="16" spans="1:11" ht="15.75" customHeight="1">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="9"/>
@@ -2772,7 +2785,7 @@
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
     </row>
-    <row r="17" spans="1:11" ht="15.75" hidden="1" customHeight="1">
+    <row r="17" spans="1:11" ht="15.75" customHeight="1">
       <c r="A17" s="3"/>
       <c r="B17" s="5"/>
       <c r="C17" s="3"/>
@@ -2782,7 +2795,7 @@
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
     </row>
-    <row r="18" spans="1:11" ht="15.75" hidden="1" customHeight="1">
+    <row r="18" spans="1:11" ht="15.75" customHeight="1">
       <c r="A18" s="11" t="s">
         <v>56</v>
       </c>
@@ -2812,7 +2825,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="15.75" hidden="1" customHeight="1">
+    <row r="19" spans="1:11" ht="15.75" customHeight="1">
       <c r="A19" s="3" t="s">
         <v>57</v>
       </c>
@@ -2843,7 +2856,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="15.75" hidden="1" customHeight="1">
+    <row r="20" spans="1:11" ht="15.75" customHeight="1">
       <c r="A20" s="3" t="s">
         <v>58</v>
       </c>
@@ -2874,7 +2887,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="15.75" hidden="1" customHeight="1">
+    <row r="21" spans="1:11" ht="15.75" customHeight="1">
       <c r="A21" s="3"/>
       <c r="B21" s="5"/>
       <c r="C21" s="8" t="s">
@@ -2903,7 +2916,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="15.75" hidden="1" customHeight="1">
+    <row r="22" spans="1:11" ht="15.75" customHeight="1">
       <c r="A22" s="3"/>
       <c r="B22" s="5"/>
       <c r="C22" s="8" t="s">
@@ -2932,7 +2945,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="15.75" hidden="1" customHeight="1">
+    <row r="23" spans="1:11" ht="15.75" customHeight="1">
       <c r="A23" s="3"/>
       <c r="B23" s="5" t="s">
         <v>87</v>
@@ -2959,7 +2972,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="15.75" hidden="1" customHeight="1">
+    <row r="24" spans="1:11" ht="15.75" customHeight="1">
       <c r="A24" s="3"/>
       <c r="B24" s="5"/>
       <c r="C24" s="8" t="s">
@@ -2984,7 +2997,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="15.75" hidden="1" customHeight="1">
+    <row r="25" spans="1:11" ht="15.75" customHeight="1">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="8" t="s">
@@ -3009,7 +3022,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="15.75" hidden="1" customHeight="1">
+    <row r="26" spans="1:11" ht="15.75" customHeight="1">
       <c r="A26" s="5"/>
       <c r="B26" s="5" t="s">
         <v>95</v>
@@ -3036,7 +3049,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="15.75" hidden="1" customHeight="1">
+    <row r="27" spans="1:11" ht="15.75" customHeight="1">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="8" t="s">
@@ -3063,7 +3076,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="15.75" hidden="1" customHeight="1">
+    <row r="28" spans="1:11" ht="15.75" customHeight="1">
       <c r="C28" s="8" t="s">
         <v>69</v>
       </c>
@@ -3083,7 +3096,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="15.75" hidden="1" customHeight="1">
+    <row r="29" spans="1:11" ht="15.75" customHeight="1">
       <c r="C29" s="8" t="s">
         <v>98</v>
       </c>
@@ -3106,7 +3119,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="15.75" hidden="1" customHeight="1">
+    <row r="30" spans="1:11" ht="15.75" customHeight="1">
       <c r="C30" s="8" t="s">
         <v>99</v>
       </c>
@@ -3126,11 +3139,10 @@
         <v>360</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="15.75" hidden="1" customHeight="1">
+    <row r="31" spans="1:11" ht="15.75" customHeight="1">
       <c r="C31" s="8"/>
       <c r="E31" s="33"/>
     </row>
-    <row r="32" spans="1:11" ht="15.75" hidden="1" customHeight="1"/>
     <row r="33" spans="1:12" ht="15.75" customHeight="1">
       <c r="A33" s="11" t="s">
         <v>350</v>
@@ -3299,7 +3311,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="15.75" hidden="1" customHeight="1">
+    <row r="39" spans="1:12" ht="15.75" customHeight="1">
       <c r="B39" t="s">
         <v>132</v>
       </c>
@@ -3328,7 +3340,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="15.75" hidden="1" customHeight="1">
+    <row r="40" spans="1:12" ht="15.75" customHeight="1">
       <c r="C40" s="8" t="s">
         <v>118</v>
       </c>
@@ -3354,7 +3366,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="15.75" hidden="1" customHeight="1">
+    <row r="41" spans="1:12" ht="15.75" customHeight="1">
       <c r="C41" s="8" t="s">
         <v>119</v>
       </c>
@@ -3380,7 +3392,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="15.75" hidden="1" customHeight="1">
+    <row r="42" spans="1:12" ht="15.75" customHeight="1">
       <c r="C42" s="8" t="s">
         <v>120</v>
       </c>
@@ -3406,7 +3418,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="15.75" hidden="1" customHeight="1">
+    <row r="43" spans="1:12" ht="15.75" customHeight="1">
       <c r="B43" t="s">
         <v>153</v>
       </c>
@@ -3435,7 +3447,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="15.75" hidden="1" customHeight="1">
+    <row r="44" spans="1:12" ht="15.75" customHeight="1">
       <c r="C44" s="8" t="s">
         <v>122</v>
       </c>
@@ -3461,7 +3473,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="15.75" hidden="1" customHeight="1">
+    <row r="45" spans="1:12" ht="15.75" customHeight="1">
       <c r="C45" s="8" t="s">
         <v>123</v>
       </c>
@@ -3484,15 +3496,15 @@
         <v>360</v>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="15.75" hidden="1" customHeight="1">
+    <row r="46" spans="1:12" ht="15.75" customHeight="1">
       <c r="C46" s="1"/>
       <c r="E46" s="33"/>
     </row>
-    <row r="47" spans="1:12" ht="12" hidden="1">
+    <row r="47" spans="1:12" ht="12">
       <c r="C47" s="1"/>
       <c r="E47" s="33"/>
     </row>
-    <row r="48" spans="1:12" ht="25" hidden="1">
+    <row r="48" spans="1:12" ht="25">
       <c r="A48" s="11" t="s">
         <v>180</v>
       </c>
@@ -3521,7 +3533,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="15" hidden="1">
+    <row r="49" spans="1:11" ht="15">
       <c r="A49" t="s">
         <v>181</v>
       </c>
@@ -3550,7 +3562,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="25" hidden="1">
+    <row r="50" spans="1:11" ht="25">
       <c r="A50" t="s">
         <v>182</v>
       </c>
@@ -3579,7 +3591,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="15" hidden="1">
+    <row r="51" spans="1:11" ht="15">
       <c r="C51" s="8" t="s">
         <v>173</v>
       </c>
@@ -3605,7 +3617,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="15" hidden="1">
+    <row r="52" spans="1:11" ht="15">
       <c r="C52" s="8" t="s">
         <v>174</v>
       </c>
@@ -3686,14 +3698,14 @@
         <v>359</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="15">
+    <row r="55" spans="1:11" ht="31" customHeight="1">
       <c r="C55" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="D55" s="27" t="s">
+      <c r="D55" s="36" t="s">
         <v>192</v>
       </c>
-      <c r="E55" s="33" t="s">
+      <c r="E55" s="40" t="s">
         <v>193</v>
       </c>
       <c r="F55" t="s">
@@ -3702,8 +3714,8 @@
       <c r="G55" t="s">
         <v>195</v>
       </c>
-      <c r="I55" s="19" t="s">
-        <v>349</v>
+      <c r="I55" s="17" t="s">
+        <v>345</v>
       </c>
       <c r="J55" t="s">
         <v>340</v>
@@ -3712,7 +3724,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="56" spans="1:11" ht="25" hidden="1">
+    <row r="56" spans="1:11" ht="25">
       <c r="B56" t="s">
         <v>212</v>
       </c>
@@ -3741,7 +3753,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="57" spans="1:11" ht="25" hidden="1">
+    <row r="57" spans="1:11" ht="25">
       <c r="C57" s="8" t="s">
         <v>179</v>
       </c>
@@ -3790,15 +3802,15 @@
         <v>359</v>
       </c>
     </row>
-    <row r="59" spans="1:11" ht="12" hidden="1">
+    <row r="59" spans="1:11" ht="12">
       <c r="C59" s="1"/>
       <c r="E59" s="33"/>
     </row>
-    <row r="60" spans="1:11" ht="12" hidden="1">
+    <row r="60" spans="1:11" ht="12">
       <c r="C60" s="1"/>
       <c r="E60" s="33"/>
     </row>
-    <row r="61" spans="1:11" ht="12" hidden="1">
+    <row r="61" spans="1:11" ht="12">
       <c r="C61" s="1"/>
       <c r="E61" s="33"/>
     </row>
@@ -3831,7 +3843,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="63" spans="1:11" ht="37" hidden="1">
+    <row r="63" spans="1:11" ht="37">
       <c r="A63" s="21" t="s">
         <v>226</v>
       </c>
@@ -3857,7 +3869,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="64" spans="1:11" ht="37" hidden="1">
+    <row r="64" spans="1:11" ht="37">
       <c r="A64" s="21" t="s">
         <v>227</v>
       </c>
@@ -3883,7 +3895,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="65" spans="1:11" ht="15" hidden="1">
+    <row r="65" spans="1:11" ht="15">
       <c r="C65" s="8" t="s">
         <v>231</v>
       </c>
@@ -3906,7 +3918,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="66" spans="1:11" ht="49" hidden="1">
+    <row r="66" spans="1:11" ht="49">
       <c r="B66" t="s">
         <v>252</v>
       </c>
@@ -3935,14 +3947,14 @@
         <v>360</v>
       </c>
     </row>
-    <row r="67" spans="1:11" ht="25">
+    <row r="67" spans="1:11" ht="24">
       <c r="C67" s="8" t="s">
         <v>233</v>
       </c>
       <c r="D67" s="38" t="s">
         <v>255</v>
       </c>
-      <c r="E67" s="33" t="s">
+      <c r="E67" s="40" t="s">
         <v>256</v>
       </c>
       <c r="F67" t="s">
@@ -3961,14 +3973,14 @@
         <v>359</v>
       </c>
     </row>
-    <row r="68" spans="1:11" ht="37">
+    <row r="68" spans="1:11" ht="36">
       <c r="C68" s="8" t="s">
         <v>234</v>
       </c>
       <c r="D68" s="27" t="s">
         <v>259</v>
       </c>
-      <c r="E68" s="33" t="s">
+      <c r="E68" s="40" t="s">
         <v>260</v>
       </c>
       <c r="F68" t="s">
@@ -3987,14 +3999,14 @@
         <v>359</v>
       </c>
     </row>
-    <row r="69" spans="1:11" ht="25">
+    <row r="69" spans="1:11" ht="24">
       <c r="C69" s="8" t="s">
         <v>235</v>
       </c>
       <c r="D69" s="38" t="s">
         <v>262</v>
       </c>
-      <c r="E69" s="33" t="s">
+      <c r="E69" s="40" t="s">
         <v>263</v>
       </c>
       <c r="F69" t="s">
@@ -4013,14 +4025,14 @@
         <v>359</v>
       </c>
     </row>
-    <row r="70" spans="1:11" ht="25">
+    <row r="70" spans="1:11" ht="24">
       <c r="C70" s="8" t="s">
         <v>236</v>
       </c>
       <c r="D70" s="27" t="s">
         <v>266</v>
       </c>
-      <c r="E70" s="33" t="s">
+      <c r="E70" s="40" t="s">
         <v>268</v>
       </c>
       <c r="F70" t="s">
@@ -4039,7 +4051,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="71" spans="1:11" ht="25">
+    <row r="71" spans="1:11" ht="24">
       <c r="B71" t="s">
         <v>270</v>
       </c>
@@ -4049,7 +4061,7 @@
       <c r="D71" s="27" t="s">
         <v>271</v>
       </c>
-      <c r="E71" s="33" t="s">
+      <c r="E71" s="40" t="s">
         <v>272</v>
       </c>
       <c r="F71" t="s">
@@ -4068,7 +4080,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="72" spans="1:11" ht="25" hidden="1">
+    <row r="72" spans="1:11" ht="25">
       <c r="C72" s="8" t="s">
         <v>238</v>
       </c>
@@ -4117,15 +4129,15 @@
         <v>359</v>
       </c>
     </row>
-    <row r="74" spans="1:11" ht="12" hidden="1">
+    <row r="74" spans="1:11" ht="12">
       <c r="C74" s="8"/>
       <c r="E74" s="33"/>
     </row>
-    <row r="75" spans="1:11" ht="12" hidden="1">
+    <row r="75" spans="1:11" ht="12">
       <c r="C75" s="1"/>
       <c r="E75" s="33"/>
     </row>
-    <row r="76" spans="1:11" ht="12" hidden="1">
+    <row r="76" spans="1:11" ht="12">
       <c r="C76" s="1"/>
       <c r="E76" s="33"/>
     </row>
@@ -4168,7 +4180,7 @@
       <c r="D78" s="38" t="s">
         <v>298</v>
       </c>
-      <c r="E78" s="33" t="s">
+      <c r="E78" s="40" t="s">
         <v>299</v>
       </c>
       <c r="F78" t="s">
@@ -4245,7 +4257,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="81" spans="2:11" ht="25" hidden="1">
+    <row r="81" spans="2:11" ht="25">
       <c r="C81" s="8" t="s">
         <v>288</v>
       </c>
@@ -4278,7 +4290,7 @@
       <c r="D82" s="27" t="s">
         <v>314</v>
       </c>
-      <c r="E82" s="33" t="s">
+      <c r="E82" s="40" t="s">
         <v>315</v>
       </c>
       <c r="F82" t="s">
@@ -4297,7 +4309,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="83" spans="2:11" ht="25" hidden="1">
+    <row r="83" spans="2:11" ht="25">
       <c r="B83" t="s">
         <v>346</v>
       </c>
@@ -4369,14 +4381,14 @@
         <v>359</v>
       </c>
     </row>
-    <row r="86" spans="2:11" ht="37">
+    <row r="86" spans="2:11" ht="36">
       <c r="C86" s="8" t="s">
         <v>293</v>
       </c>
-      <c r="D86" s="38" t="s">
+      <c r="D86" s="36" t="s">
         <v>323</v>
       </c>
-      <c r="E86" s="33" t="s">
+      <c r="E86" s="40" t="s">
         <v>324</v>
       </c>
       <c r="F86" t="s">
@@ -4385,8 +4397,8 @@
       <c r="G86" t="s">
         <v>326</v>
       </c>
-      <c r="I86" s="19" t="s">
-        <v>349</v>
+      <c r="I86" s="17" t="s">
+        <v>345</v>
       </c>
       <c r="J86" t="s">
         <v>342</v>
@@ -4395,7 +4407,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="87" spans="2:11" ht="25" hidden="1">
+    <row r="87" spans="2:11" ht="25">
       <c r="B87" t="s">
         <v>336</v>
       </c>
@@ -4424,7 +4436,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="88" spans="2:11" ht="25" hidden="1">
+    <row r="88" spans="2:11" ht="25">
       <c r="C88" s="8" t="s">
         <v>295</v>
       </c>
@@ -4450,7 +4462,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="89" spans="2:11" ht="25" hidden="1">
+    <row r="89" spans="2:11" ht="25">
       <c r="C89" s="8" t="s">
         <v>352</v>
       </c>
@@ -7211,13 +7223,7 @@
     <row r="1003" spans="3:3" ht="12"/>
     <row r="1004" spans="3:3" ht="12"/>
   </sheetData>
-  <autoFilter ref="A1:K89">
-    <filterColumn colId="10">
-      <filters>
-        <filter val="W"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:K89"/>
   <mergeCells count="1">
     <mergeCell ref="A5:A7"/>
   </mergeCells>

</xml_diff>

<commit_message>
Basic elements code, type checking quiz, who uses haskell article
</commit_message>
<xml_diff>
--- a/fl_course_outline_weeks.xlsx
+++ b/fl_course_outline_weeks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27127"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="27260" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="40540" windowHeight="25220" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1331,7 +1331,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="314">
+  <cellStyleXfs count="318">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1484,6 +1484,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1755,7 +1759,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="314">
+  <cellStyles count="318">
     <cellStyle name="Bad" xfId="150" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -1912,6 +1916,8 @@
     <cellStyle name="Followed Hyperlink" xfId="309" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="311" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="313" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="315" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="317" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="55" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -2068,6 +2074,8 @@
     <cellStyle name="Hyperlink" xfId="308" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="310" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="312" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="314" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="316" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="151" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -2336,7 +2344,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2349,7 +2357,7 @@
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="M2" sqref="M2"/>
+      <selection pane="bottomLeft" activeCell="I70" sqref="I70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -4029,7 +4037,7 @@
       <c r="C70" s="8" t="s">
         <v>236</v>
       </c>
-      <c r="D70" s="27" t="s">
+      <c r="D70" s="36" t="s">
         <v>266</v>
       </c>
       <c r="E70" s="40" t="s">
@@ -4041,8 +4049,8 @@
       <c r="G70" t="s">
         <v>269</v>
       </c>
-      <c r="I70" s="19" t="s">
-        <v>349</v>
+      <c r="I70" s="17" t="s">
+        <v>345</v>
       </c>
       <c r="J70" t="s">
         <v>340</v>
@@ -4058,7 +4066,7 @@
       <c r="C71" s="8" t="s">
         <v>237</v>
       </c>
-      <c r="D71" s="27" t="s">
+      <c r="D71" s="36" t="s">
         <v>271</v>
       </c>
       <c r="E71" s="40" t="s">
@@ -4070,8 +4078,8 @@
       <c r="G71" t="s">
         <v>274</v>
       </c>
-      <c r="I71" s="19" t="s">
-        <v>349</v>
+      <c r="I71" s="17" t="s">
+        <v>345</v>
       </c>
       <c r="J71" t="s">
         <v>341</v>

</xml_diff>

<commit_message>
Changed wk1-1 to Markdown
added contend for typeclasses video
</commit_message>
<xml_diff>
--- a/fl_course_outline_weeks.xlsx
+++ b/fl_course_outline_weeks.xlsx
@@ -1337,7 +1337,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="322">
+  <cellStyleXfs count="324">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1660,8 +1660,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1756,6 +1758,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1765,12 +1771,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="322">
+  <cellStyles count="324">
     <cellStyle name="Bad" xfId="150" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -1931,6 +1936,7 @@
     <cellStyle name="Followed Hyperlink" xfId="317" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="319" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="321" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="323" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="55" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -2091,6 +2097,7 @@
     <cellStyle name="Hyperlink" xfId="316" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="318" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="320" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="322" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="151" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -2359,7 +2366,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2373,7 +2380,7 @@
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="E78" sqref="E78"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -2453,7 +2460,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="29" customHeight="1">
+    <row r="3" spans="1:11" ht="29" hidden="1" customHeight="1">
       <c r="A3" s="11" t="s">
         <v>55</v>
       </c>
@@ -2461,7 +2468,7 @@
       <c r="C3" s="6">
         <v>1.2</v>
       </c>
-      <c r="D3" s="43" t="s">
+      <c r="D3" s="45" t="s">
         <v>16</v>
       </c>
       <c r="E3" s="38" t="s">
@@ -2474,8 +2481,8 @@
         <v>42</v>
       </c>
       <c r="H3" s="3"/>
-      <c r="I3" s="19" t="s">
-        <v>346</v>
+      <c r="I3" s="17" t="s">
+        <v>342</v>
       </c>
       <c r="J3" s="16" t="s">
         <v>336</v>
@@ -2516,7 +2523,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="15.75" hidden="1" customHeight="1">
-      <c r="A5" s="40" t="s">
+      <c r="A5" s="42" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="3"/>
@@ -2547,7 +2554,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="15.75" hidden="1" customHeight="1">
-      <c r="A6" s="41"/>
+      <c r="A6" s="43"/>
       <c r="B6" s="5"/>
       <c r="C6" s="7">
         <v>1.5</v>
@@ -2576,14 +2583,14 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="31" customHeight="1">
-      <c r="A7" s="42"/>
+      <c r="A7" s="44"/>
       <c r="B7" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="43" t="s">
+      <c r="D7" s="40" t="s">
         <v>19</v>
       </c>
       <c r="E7" s="38" t="s">
@@ -4002,7 +4009,7 @@
       <c r="C68" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="D68" s="44" t="s">
+      <c r="D68" s="41" t="s">
         <v>364</v>
       </c>
       <c r="E68" s="39" t="s">
@@ -4202,7 +4209,7 @@
       <c r="C78" s="8" t="s">
         <v>282</v>
       </c>
-      <c r="D78" s="44" t="s">
+      <c r="D78" s="41" t="s">
         <v>295</v>
       </c>
       <c r="E78" s="39" t="s">

</xml_diff>

<commit_message>
More vids and transcripts
</commit_message>
<xml_diff>
--- a/fl_course_outline_weeks.xlsx
+++ b/fl_course_outline_weeks.xlsx
@@ -1128,7 +1128,7 @@
     <t>Article Function types</t>
   </si>
   <si>
-    <t>Camtasia? Video: type checking</t>
+    <t>Video: type inference</t>
   </si>
 </sst>
 </file>
@@ -1208,7 +1208,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1251,12 +1251,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1337,7 +1331,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="324">
+  <cellStyleXfs count="332">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1662,8 +1656,16 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1751,17 +1753,16 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1771,11 +1772,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="324">
+  <cellStyles count="332">
     <cellStyle name="Bad" xfId="150" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -1937,6 +1935,10 @@
     <cellStyle name="Followed Hyperlink" xfId="319" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="321" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="323" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="325" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="327" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="329" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="331" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="55" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -2098,6 +2100,10 @@
     <cellStyle name="Hyperlink" xfId="318" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="320" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="322" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="324" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="326" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="328" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="330" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="151" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -2366,7 +2372,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2374,13 +2380,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:L1004"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomLeft" activeCell="I68" sqref="I68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -2430,7 +2435,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="49" hidden="1" customHeight="1">
+    <row r="2" spans="1:11" ht="49" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -2460,7 +2465,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="29" hidden="1" customHeight="1">
+    <row r="3" spans="1:11" ht="29" customHeight="1">
       <c r="A3" s="11" t="s">
         <v>55</v>
       </c>
@@ -2468,10 +2473,10 @@
       <c r="C3" s="6">
         <v>1.2</v>
       </c>
-      <c r="D3" s="45" t="s">
+      <c r="D3" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="38" t="s">
+      <c r="E3" s="37" t="s">
         <v>32</v>
       </c>
       <c r="F3" s="3" t="s">
@@ -2491,7 +2496,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15.75" hidden="1" customHeight="1">
+    <row r="4" spans="1:11" ht="15.75" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -2522,8 +2527,8 @@
         <v>356</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="15.75" hidden="1" customHeight="1">
-      <c r="A5" s="42" t="s">
+    <row r="5" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A5" s="41" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="3"/>
@@ -2553,8 +2558,8 @@
         <v>356</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15.75" hidden="1" customHeight="1">
-      <c r="A6" s="43"/>
+    <row r="6" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A6" s="42"/>
       <c r="B6" s="5"/>
       <c r="C6" s="7">
         <v>1.5</v>
@@ -2583,7 +2588,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="31" customHeight="1">
-      <c r="A7" s="44"/>
+      <c r="A7" s="43"/>
       <c r="B7" s="5" t="s">
         <v>18</v>
       </c>
@@ -2593,7 +2598,7 @@
       <c r="D7" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="38" t="s">
+      <c r="E7" s="37" t="s">
         <v>36</v>
       </c>
       <c r="F7" s="3" t="s">
@@ -2603,8 +2608,8 @@
         <v>42</v>
       </c>
       <c r="H7" s="3"/>
-      <c r="I7" s="19" t="s">
-        <v>346</v>
+      <c r="I7" s="17" t="s">
+        <v>342</v>
       </c>
       <c r="J7" s="16" t="s">
         <v>336</v>
@@ -2613,7 +2618,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15.75" hidden="1" customHeight="1">
+    <row r="8" spans="1:11" ht="15.75" customHeight="1">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="8" t="s">
@@ -2642,7 +2647,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15.75" hidden="1" customHeight="1">
+    <row r="9" spans="1:11" ht="15.75" customHeight="1">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="8" t="s">
@@ -2671,7 +2676,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15.75" hidden="1" customHeight="1">
+    <row r="10" spans="1:11" ht="15.75" customHeight="1">
       <c r="A10" s="3"/>
       <c r="B10" s="5"/>
       <c r="C10" s="8" t="s">
@@ -2700,7 +2705,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15.75" hidden="1" customHeight="1">
+    <row r="11" spans="1:11" ht="15.75" customHeight="1">
       <c r="A11" s="3"/>
       <c r="B11" s="3" t="s">
         <v>21</v>
@@ -2731,7 +2736,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="15.75" hidden="1" customHeight="1">
+    <row r="12" spans="1:11" ht="15.75" customHeight="1">
       <c r="A12" s="3"/>
       <c r="B12" s="5"/>
       <c r="C12" s="8" t="s">
@@ -2760,7 +2765,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="15.75" hidden="1" customHeight="1">
+    <row r="13" spans="1:11" ht="15.75" customHeight="1">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="8" t="s">
@@ -2786,7 +2791,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="15.75" hidden="1" customHeight="1">
+    <row r="14" spans="1:11" ht="15.75" customHeight="1">
       <c r="A14" s="3"/>
       <c r="B14" s="5"/>
       <c r="C14" s="3"/>
@@ -2796,7 +2801,7 @@
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
     </row>
-    <row r="15" spans="1:11" ht="15.75" hidden="1" customHeight="1">
+    <row r="15" spans="1:11" ht="15.75" customHeight="1">
       <c r="A15" s="3"/>
       <c r="B15" s="5"/>
       <c r="C15" s="9"/>
@@ -2806,7 +2811,7 @@
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
     </row>
-    <row r="16" spans="1:11" ht="15.75" hidden="1" customHeight="1">
+    <row r="16" spans="1:11" ht="15.75" customHeight="1">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="9"/>
@@ -2816,7 +2821,7 @@
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
     </row>
-    <row r="17" spans="1:11" ht="15.75" hidden="1" customHeight="1">
+    <row r="17" spans="1:11" ht="15.75" customHeight="1">
       <c r="A17" s="3"/>
       <c r="B17" s="5"/>
       <c r="C17" s="3"/>
@@ -2826,7 +2831,7 @@
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
     </row>
-    <row r="18" spans="1:11" ht="15.75" hidden="1" customHeight="1">
+    <row r="18" spans="1:11" ht="15.75" customHeight="1">
       <c r="A18" s="11" t="s">
         <v>56</v>
       </c>
@@ -2856,7 +2861,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="15.75" hidden="1" customHeight="1">
+    <row r="19" spans="1:11" ht="15.75" customHeight="1">
       <c r="A19" s="3" t="s">
         <v>57</v>
       </c>
@@ -2887,7 +2892,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="15.75" hidden="1" customHeight="1">
+    <row r="20" spans="1:11" ht="15.75" customHeight="1">
       <c r="A20" s="3" t="s">
         <v>58</v>
       </c>
@@ -2918,7 +2923,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="15.75" hidden="1" customHeight="1">
+    <row r="21" spans="1:11" ht="15.75" customHeight="1">
       <c r="A21" s="3"/>
       <c r="B21" s="5"/>
       <c r="C21" s="8" t="s">
@@ -2947,7 +2952,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="15.75" hidden="1" customHeight="1">
+    <row r="22" spans="1:11" ht="15.75" customHeight="1">
       <c r="A22" s="3"/>
       <c r="B22" s="5"/>
       <c r="C22" s="8" t="s">
@@ -2976,7 +2981,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="15.75" hidden="1" customHeight="1">
+    <row r="23" spans="1:11" ht="15.75" customHeight="1">
       <c r="A23" s="3"/>
       <c r="B23" s="5" t="s">
         <v>87</v>
@@ -3003,7 +3008,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="15.75" hidden="1" customHeight="1">
+    <row r="24" spans="1:11" ht="15.75" customHeight="1">
       <c r="A24" s="3"/>
       <c r="B24" s="5"/>
       <c r="C24" s="8" t="s">
@@ -3028,7 +3033,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="15.75" hidden="1" customHeight="1">
+    <row r="25" spans="1:11" ht="15.75" customHeight="1">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="8" t="s">
@@ -3053,7 +3058,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="15.75" hidden="1" customHeight="1">
+    <row r="26" spans="1:11" ht="15.75" customHeight="1">
       <c r="A26" s="5"/>
       <c r="B26" s="5" t="s">
         <v>95</v>
@@ -3080,7 +3085,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="15.75" hidden="1" customHeight="1">
+    <row r="27" spans="1:11" ht="15.75" customHeight="1">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="8" t="s">
@@ -3107,7 +3112,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="15.75" hidden="1" customHeight="1">
+    <row r="28" spans="1:11" ht="15.75" customHeight="1">
       <c r="C28" s="8" t="s">
         <v>69</v>
       </c>
@@ -3127,7 +3132,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="15.75" hidden="1" customHeight="1">
+    <row r="29" spans="1:11" ht="15.75" customHeight="1">
       <c r="C29" s="8" t="s">
         <v>98</v>
       </c>
@@ -3150,7 +3155,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="15.75" hidden="1" customHeight="1">
+    <row r="30" spans="1:11" ht="15.75" customHeight="1">
       <c r="C30" s="8" t="s">
         <v>99</v>
       </c>
@@ -3170,12 +3175,11 @@
         <v>357</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="15.75" hidden="1" customHeight="1">
+    <row r="31" spans="1:11" ht="15.75" customHeight="1">
       <c r="C31" s="8"/>
       <c r="E31" s="33"/>
     </row>
-    <row r="32" spans="1:11" ht="15.75" hidden="1" customHeight="1"/>
-    <row r="33" spans="1:12" ht="15.75" hidden="1" customHeight="1">
+    <row r="33" spans="1:12" ht="15.75" customHeight="1">
       <c r="A33" s="11" t="s">
         <v>347</v>
       </c>
@@ -3204,7 +3208,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="15.75" hidden="1" customHeight="1">
+    <row r="34" spans="1:12" ht="15.75" customHeight="1">
       <c r="A34" t="s">
         <v>108</v>
       </c>
@@ -3233,7 +3237,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="15.75" hidden="1" customHeight="1">
+    <row r="35" spans="1:12" ht="15.75" customHeight="1">
       <c r="A35" t="s">
         <v>109</v>
       </c>
@@ -3262,7 +3266,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="15.75" hidden="1" customHeight="1">
+    <row r="36" spans="1:12" ht="15.75" customHeight="1">
       <c r="C36" s="8" t="s">
         <v>115</v>
       </c>
@@ -3288,7 +3292,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="15.75" hidden="1" customHeight="1">
+    <row r="37" spans="1:12" ht="15.75" customHeight="1">
       <c r="C37" s="8" t="s">
         <v>114</v>
       </c>
@@ -3317,7 +3321,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="15.75" hidden="1" customHeight="1">
+    <row r="38" spans="1:12" ht="15.75" customHeight="1">
       <c r="C38" s="8" t="s">
         <v>116</v>
       </c>
@@ -3343,7 +3347,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="15.75" hidden="1" customHeight="1">
+    <row r="39" spans="1:12" ht="15.75" customHeight="1">
       <c r="B39" t="s">
         <v>132</v>
       </c>
@@ -3372,7 +3376,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="15.75" hidden="1" customHeight="1">
+    <row r="40" spans="1:12" ht="15.75" customHeight="1">
       <c r="C40" s="8" t="s">
         <v>118</v>
       </c>
@@ -3398,7 +3402,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="15.75" hidden="1" customHeight="1">
+    <row r="41" spans="1:12" ht="15.75" customHeight="1">
       <c r="C41" s="8" t="s">
         <v>119</v>
       </c>
@@ -3424,7 +3428,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="15.75" hidden="1" customHeight="1">
+    <row r="42" spans="1:12" ht="15.75" customHeight="1">
       <c r="C42" s="8" t="s">
         <v>120</v>
       </c>
@@ -3450,7 +3454,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="15.75" hidden="1" customHeight="1">
+    <row r="43" spans="1:12" ht="15.75" customHeight="1">
       <c r="B43" t="s">
         <v>153</v>
       </c>
@@ -3479,7 +3483,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="15.75" hidden="1" customHeight="1">
+    <row r="44" spans="1:12" ht="15.75" customHeight="1">
       <c r="C44" s="8" t="s">
         <v>122</v>
       </c>
@@ -3505,7 +3509,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="15.75" hidden="1" customHeight="1">
+    <row r="45" spans="1:12" ht="15.75" customHeight="1">
       <c r="C45" s="8" t="s">
         <v>123</v>
       </c>
@@ -3528,15 +3532,15 @@
         <v>357</v>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="15.75" hidden="1" customHeight="1">
+    <row r="46" spans="1:12" ht="15.75" customHeight="1">
       <c r="C46" s="1"/>
       <c r="E46" s="33"/>
     </row>
-    <row r="47" spans="1:12" ht="12" hidden="1">
+    <row r="47" spans="1:12" ht="12">
       <c r="C47" s="1"/>
       <c r="E47" s="33"/>
     </row>
-    <row r="48" spans="1:12" ht="25" hidden="1">
+    <row r="48" spans="1:12" ht="25">
       <c r="A48" s="11" t="s">
         <v>180</v>
       </c>
@@ -3565,7 +3569,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="15" hidden="1">
+    <row r="49" spans="1:11" ht="15">
       <c r="A49" t="s">
         <v>181</v>
       </c>
@@ -3594,7 +3598,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="25" hidden="1">
+    <row r="50" spans="1:11" ht="25">
       <c r="A50" t="s">
         <v>182</v>
       </c>
@@ -3623,7 +3627,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="15" hidden="1">
+    <row r="51" spans="1:11" ht="15">
       <c r="C51" s="8" t="s">
         <v>173</v>
       </c>
@@ -3649,7 +3653,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="15" hidden="1">
+    <row r="52" spans="1:11" ht="15">
       <c r="C52" s="8" t="s">
         <v>174</v>
       </c>
@@ -3675,7 +3679,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="15" hidden="1">
+    <row r="53" spans="1:11" ht="15">
       <c r="B53" t="s">
         <v>187</v>
       </c>
@@ -3704,7 +3708,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="15" hidden="1">
+    <row r="54" spans="1:11" ht="15">
       <c r="C54" s="8" t="s">
         <v>176</v>
       </c>
@@ -3730,14 +3734,14 @@
         <v>356</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="31" hidden="1" customHeight="1">
+    <row r="55" spans="1:11" ht="31" customHeight="1">
       <c r="C55" s="8" t="s">
         <v>177</v>
       </c>
       <c r="D55" s="36" t="s">
         <v>192</v>
       </c>
-      <c r="E55" s="39" t="s">
+      <c r="E55" s="38" t="s">
         <v>193</v>
       </c>
       <c r="F55" t="s">
@@ -3756,7 +3760,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="56" spans="1:11" ht="25" hidden="1">
+    <row r="56" spans="1:11" ht="25">
       <c r="B56" t="s">
         <v>212</v>
       </c>
@@ -3785,7 +3789,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="57" spans="1:11" ht="25" hidden="1">
+    <row r="57" spans="1:11" ht="25">
       <c r="C57" s="8" t="s">
         <v>179</v>
       </c>
@@ -3811,7 +3815,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="58" spans="1:11" ht="15" hidden="1">
+    <row r="58" spans="1:11" ht="15">
       <c r="C58" s="8" t="s">
         <v>218</v>
       </c>
@@ -3834,19 +3838,19 @@
         <v>356</v>
       </c>
     </row>
-    <row r="59" spans="1:11" ht="12" hidden="1">
+    <row r="59" spans="1:11" ht="12">
       <c r="C59" s="1"/>
       <c r="E59" s="33"/>
     </row>
-    <row r="60" spans="1:11" ht="12" hidden="1">
+    <row r="60" spans="1:11" ht="12">
       <c r="C60" s="1"/>
       <c r="E60" s="33"/>
     </row>
-    <row r="61" spans="1:11" ht="12" hidden="1">
+    <row r="61" spans="1:11" ht="12">
       <c r="C61" s="1"/>
       <c r="E61" s="33"/>
     </row>
-    <row r="62" spans="1:11" ht="25" hidden="1">
+    <row r="62" spans="1:11" ht="25">
       <c r="A62" s="15" t="s">
         <v>224</v>
       </c>
@@ -3875,7 +3879,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="63" spans="1:11" ht="37" hidden="1">
+    <row r="63" spans="1:11" ht="37">
       <c r="A63" s="21" t="s">
         <v>226</v>
       </c>
@@ -3901,7 +3905,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="64" spans="1:11" ht="37" hidden="1">
+    <row r="64" spans="1:11" ht="37">
       <c r="A64" s="21" t="s">
         <v>227</v>
       </c>
@@ -3927,7 +3931,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="65" spans="1:11" ht="15" hidden="1">
+    <row r="65" spans="1:11" ht="15">
       <c r="C65" s="8" t="s">
         <v>231</v>
       </c>
@@ -3950,7 +3954,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="66" spans="1:11" ht="49" hidden="1">
+    <row r="66" spans="1:11" ht="49">
       <c r="B66" t="s">
         <v>252</v>
       </c>
@@ -3979,14 +3983,14 @@
         <v>357</v>
       </c>
     </row>
-    <row r="67" spans="1:11" ht="24" hidden="1">
+    <row r="67" spans="1:11" ht="24">
       <c r="C67" s="8" t="s">
         <v>233</v>
       </c>
       <c r="D67" s="36" t="s">
         <v>365</v>
       </c>
-      <c r="E67" s="39" t="s">
+      <c r="E67" s="38" t="s">
         <v>255</v>
       </c>
       <c r="F67" t="s">
@@ -4009,10 +4013,10 @@
       <c r="C68" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="D68" s="41" t="s">
+      <c r="D68" s="36" t="s">
         <v>364</v>
       </c>
-      <c r="E68" s="39" t="s">
+      <c r="E68" s="38" t="s">
         <v>258</v>
       </c>
       <c r="F68" t="s">
@@ -4021,8 +4025,8 @@
       <c r="G68" t="s">
         <v>259</v>
       </c>
-      <c r="I68" s="19" t="s">
-        <v>346</v>
+      <c r="I68" s="17" t="s">
+        <v>342</v>
       </c>
       <c r="J68" t="s">
         <v>336</v>
@@ -4035,10 +4039,10 @@
       <c r="C69" s="8" t="s">
         <v>235</v>
       </c>
-      <c r="D69" s="37" t="s">
+      <c r="D69" s="39" t="s">
         <v>366</v>
       </c>
-      <c r="E69" s="39" t="s">
+      <c r="E69" s="38" t="s">
         <v>260</v>
       </c>
       <c r="F69" t="s">
@@ -4057,14 +4061,14 @@
         <v>356</v>
       </c>
     </row>
-    <row r="70" spans="1:11" ht="24" hidden="1">
+    <row r="70" spans="1:11" ht="24">
       <c r="C70" s="8" t="s">
         <v>236</v>
       </c>
       <c r="D70" s="36" t="s">
         <v>263</v>
       </c>
-      <c r="E70" s="39" t="s">
+      <c r="E70" s="38" t="s">
         <v>265</v>
       </c>
       <c r="F70" t="s">
@@ -4083,7 +4087,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="71" spans="1:11" ht="24" hidden="1">
+    <row r="71" spans="1:11" ht="24">
       <c r="B71" t="s">
         <v>267</v>
       </c>
@@ -4093,7 +4097,7 @@
       <c r="D71" s="36" t="s">
         <v>268</v>
       </c>
-      <c r="E71" s="39" t="s">
+      <c r="E71" s="38" t="s">
         <v>269</v>
       </c>
       <c r="F71" t="s">
@@ -4112,7 +4116,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="72" spans="1:11" ht="25" hidden="1">
+    <row r="72" spans="1:11" ht="25">
       <c r="C72" s="8" t="s">
         <v>238</v>
       </c>
@@ -4138,7 +4142,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="73" spans="1:11" ht="15" hidden="1">
+    <row r="73" spans="1:11" ht="15">
       <c r="C73" s="8" t="s">
         <v>239</v>
       </c>
@@ -4161,19 +4165,19 @@
         <v>356</v>
       </c>
     </row>
-    <row r="74" spans="1:11" ht="12" hidden="1">
+    <row r="74" spans="1:11" ht="12">
       <c r="C74" s="8"/>
       <c r="E74" s="33"/>
     </row>
-    <row r="75" spans="1:11" ht="12" hidden="1">
+    <row r="75" spans="1:11" ht="12">
       <c r="C75" s="1"/>
       <c r="E75" s="33"/>
     </row>
-    <row r="76" spans="1:11" ht="12" hidden="1">
+    <row r="76" spans="1:11" ht="12">
       <c r="C76" s="1"/>
       <c r="E76" s="33"/>
     </row>
-    <row r="77" spans="1:11" ht="15" hidden="1">
+    <row r="77" spans="1:11" ht="15">
       <c r="A77" s="15" t="s">
         <v>278</v>
       </c>
@@ -4209,10 +4213,10 @@
       <c r="C78" s="8" t="s">
         <v>282</v>
       </c>
-      <c r="D78" s="41" t="s">
+      <c r="D78" s="36" t="s">
         <v>295</v>
       </c>
-      <c r="E78" s="39" t="s">
+      <c r="E78" s="38" t="s">
         <v>296</v>
       </c>
       <c r="F78" t="s">
@@ -4221,8 +4225,8 @@
       <c r="G78" t="s">
         <v>298</v>
       </c>
-      <c r="I78" s="19" t="s">
-        <v>346</v>
+      <c r="I78" s="17" t="s">
+        <v>342</v>
       </c>
       <c r="J78" t="s">
         <v>336</v>
@@ -4231,7 +4235,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="79" spans="1:11" ht="25" hidden="1">
+    <row r="79" spans="1:11" ht="25">
       <c r="A79" s="21" t="s">
         <v>280</v>
       </c>
@@ -4260,7 +4264,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="80" spans="1:11" ht="25" hidden="1">
+    <row r="80" spans="1:11" ht="25">
       <c r="B80" t="s">
         <v>303</v>
       </c>
@@ -4289,7 +4293,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="81" spans="2:11" ht="25" hidden="1">
+    <row r="81" spans="2:11" ht="25">
       <c r="C81" s="8" t="s">
         <v>285</v>
       </c>
@@ -4322,7 +4326,7 @@
       <c r="D82" s="27" t="s">
         <v>311</v>
       </c>
-      <c r="E82" s="39" t="s">
+      <c r="E82" s="38" t="s">
         <v>312</v>
       </c>
       <c r="F82" t="s">
@@ -4341,7 +4345,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="83" spans="2:11" ht="25" hidden="1">
+    <row r="83" spans="2:11" ht="25">
       <c r="B83" t="s">
         <v>343</v>
       </c>
@@ -4370,7 +4374,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="84" spans="2:11" ht="37" hidden="1">
+    <row r="84" spans="2:11" ht="37">
       <c r="C84" s="8" t="s">
         <v>288</v>
       </c>
@@ -4396,7 +4400,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="85" spans="2:11" ht="25" hidden="1">
+    <row r="85" spans="2:11" ht="25">
       <c r="C85" s="8" t="s">
         <v>289</v>
       </c>
@@ -4413,14 +4417,14 @@
         <v>356</v>
       </c>
     </row>
-    <row r="86" spans="2:11" ht="36" hidden="1">
+    <row r="86" spans="2:11" ht="36">
       <c r="C86" s="8" t="s">
         <v>290</v>
       </c>
       <c r="D86" s="36" t="s">
         <v>320</v>
       </c>
-      <c r="E86" s="39" t="s">
+      <c r="E86" s="38" t="s">
         <v>321</v>
       </c>
       <c r="F86" t="s">
@@ -4439,7 +4443,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="87" spans="2:11" ht="25" hidden="1">
+    <row r="87" spans="2:11" ht="25">
       <c r="B87" t="s">
         <v>333</v>
       </c>
@@ -4468,7 +4472,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="88" spans="2:11" ht="25" hidden="1">
+    <row r="88" spans="2:11" ht="25">
       <c r="C88" s="8" t="s">
         <v>292</v>
       </c>
@@ -4494,7 +4498,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="89" spans="2:11" ht="25" hidden="1">
+    <row r="89" spans="2:11" ht="25">
       <c r="C89" s="8" t="s">
         <v>349</v>
       </c>
@@ -7255,18 +7259,7 @@
     <row r="1003" spans="3:3" ht="12"/>
     <row r="1004" spans="3:3" ht="12"/>
   </sheetData>
-  <autoFilter ref="A1:K89">
-    <filterColumn colId="8">
-      <filters>
-        <filter val="todo"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="10">
-      <filters>
-        <filter val="W"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:K89"/>
   <mergeCells count="1">
     <mergeCell ref="A5:A7"/>
   </mergeCells>

</xml_diff>

<commit_message>
Quiz "we love lambda"
</commit_message>
<xml_diff>
--- a/fl_course_outline_weeks.xlsx
+++ b/fl_course_outline_weeks.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="368">
   <si>
     <t>Week</t>
   </si>
@@ -1104,9 +1104,6 @@
     <t>J</t>
   </si>
   <si>
-    <t>I</t>
-  </si>
-  <si>
     <t>Tutorial 1.1: The Basics: Expressions, Functions and Equations</t>
   </si>
   <si>
@@ -1129,6 +1126,12 @@
   </si>
   <si>
     <t>Video: type inference</t>
+  </si>
+  <si>
+    <t>QA Done?</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -1208,7 +1211,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1245,18 +1248,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF03EFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1331,7 +1322,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="332">
+  <cellStyleXfs count="338">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1664,8 +1655,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1727,7 +1724,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1759,7 +1755,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1773,7 +1768,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="332">
+  <cellStyles count="338">
     <cellStyle name="Bad" xfId="150" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -1939,6 +1934,9 @@
     <cellStyle name="Followed Hyperlink" xfId="327" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="329" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="331" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="333" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="335" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="337" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="55" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -2104,6 +2102,9 @@
     <cellStyle name="Hyperlink" xfId="326" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="328" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="330" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="332" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="334" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="336" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="151" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -2372,7 +2373,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2382,10 +2383,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L1004"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="I68" sqref="I68"/>
+      <selection pane="bottomLeft" activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -2394,13 +2395,13 @@
     <col min="2" max="2" width="24" customWidth="1"/>
     <col min="3" max="3" width="7.6640625" customWidth="1"/>
     <col min="4" max="4" width="52" customWidth="1"/>
-    <col min="5" max="5" width="38.6640625" style="30" customWidth="1"/>
+    <col min="5" max="5" width="38.6640625" style="29" customWidth="1"/>
     <col min="6" max="6" width="39.83203125" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="33.6640625" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="42.5" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="89" customHeight="1">
+    <row r="1" spans="1:12" ht="89" customHeight="1">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -2413,7 +2414,7 @@
       <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="28" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="10" t="s">
@@ -2434,8 +2435,11 @@
       <c r="K1" s="12" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" ht="49" customHeight="1">
+      <c r="L1" s="12" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="49" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -2448,7 +2452,7 @@
       <c r="D2" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="27" t="s">
         <v>31</v>
       </c>
       <c r="F2" s="3" t="s">
@@ -2465,7 +2469,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="29" customHeight="1">
+    <row r="3" spans="1:12" ht="29" customHeight="1">
       <c r="A3" s="11" t="s">
         <v>55</v>
       </c>
@@ -2473,10 +2477,10 @@
       <c r="C3" s="6">
         <v>1.2</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="37" t="s">
+      <c r="E3" s="36" t="s">
         <v>32</v>
       </c>
       <c r="F3" s="3" t="s">
@@ -2495,8 +2499,11 @@
       <c r="K3" s="16" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" ht="15.75" customHeight="1">
+      <c r="L3" s="16" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="15.75" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -2507,7 +2514,7 @@
       <c r="D4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="28" t="s">
+      <c r="E4" s="27" t="s">
         <v>33</v>
       </c>
       <c r="F4" s="3" t="s">
@@ -2527,18 +2534,18 @@
         <v>356</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A5" s="41" t="s">
+    <row r="5" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A5" s="39" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="6">
         <v>1.4</v>
       </c>
-      <c r="D5" s="28" t="s">
-        <v>359</v>
-      </c>
-      <c r="E5" s="35" t="s">
+      <c r="D5" s="27" t="s">
+        <v>358</v>
+      </c>
+      <c r="E5" s="34" t="s">
         <v>34</v>
       </c>
       <c r="F5" s="3" t="s">
@@ -2558,8 +2565,8 @@
         <v>356</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A6" s="42"/>
+    <row r="6" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A6" s="40"/>
       <c r="B6" s="5"/>
       <c r="C6" s="7">
         <v>1.5</v>
@@ -2567,7 +2574,7 @@
       <c r="D6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="28" t="s">
+      <c r="E6" s="27" t="s">
         <v>35</v>
       </c>
       <c r="F6" s="3" t="s">
@@ -2587,18 +2594,18 @@
         <v>356</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="31" customHeight="1">
-      <c r="A7" s="43"/>
+    <row r="7" spans="1:12" ht="31" customHeight="1">
+      <c r="A7" s="41"/>
       <c r="B7" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="40" t="s">
+      <c r="D7" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="37" t="s">
+      <c r="E7" s="36" t="s">
         <v>36</v>
       </c>
       <c r="F7" s="3" t="s">
@@ -2618,7 +2625,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15.75" customHeight="1">
+    <row r="8" spans="1:12" ht="15.75" customHeight="1">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="8" t="s">
@@ -2627,7 +2634,7 @@
       <c r="D8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="28" t="s">
+      <c r="E8" s="27" t="s">
         <v>37</v>
       </c>
       <c r="F8" s="3" t="s">
@@ -2647,16 +2654,16 @@
         <v>356</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15.75" customHeight="1">
+    <row r="9" spans="1:12" ht="15.75" customHeight="1">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="8" t="s">
         <v>26</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>360</v>
-      </c>
-      <c r="E9" s="28" t="s">
+        <v>359</v>
+      </c>
+      <c r="E9" s="27" t="s">
         <v>38</v>
       </c>
       <c r="F9" s="3" t="s">
@@ -2676,7 +2683,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15.75" customHeight="1">
+    <row r="10" spans="1:12" ht="15.75" customHeight="1">
       <c r="A10" s="3"/>
       <c r="B10" s="5"/>
       <c r="C10" s="8" t="s">
@@ -2685,7 +2692,7 @@
       <c r="D10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="28" t="s">
+      <c r="E10" s="27" t="s">
         <v>35</v>
       </c>
       <c r="F10" s="3" t="s">
@@ -2705,7 +2712,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15.75" customHeight="1">
+    <row r="11" spans="1:12" ht="15.75" customHeight="1">
       <c r="A11" s="3"/>
       <c r="B11" s="3" t="s">
         <v>21</v>
@@ -2716,7 +2723,7 @@
       <c r="D11" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="28" t="s">
+      <c r="E11" s="27" t="s">
         <v>39</v>
       </c>
       <c r="F11" s="3" t="s">
@@ -2736,7 +2743,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="15.75" customHeight="1">
+    <row r="12" spans="1:12" ht="15.75" customHeight="1">
       <c r="A12" s="3"/>
       <c r="B12" s="5"/>
       <c r="C12" s="8" t="s">
@@ -2745,7 +2752,7 @@
       <c r="D12" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="28" t="s">
+      <c r="E12" s="27" t="s">
         <v>40</v>
       </c>
       <c r="F12" s="3" t="s">
@@ -2765,7 +2772,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="15.75" customHeight="1">
+    <row r="13" spans="1:12" ht="15.75" customHeight="1">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="8" t="s">
@@ -2774,7 +2781,7 @@
       <c r="D13" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E13" s="28" t="s">
+      <c r="E13" s="27" t="s">
         <v>41</v>
       </c>
       <c r="F13" s="3" t="s">
@@ -2791,32 +2798,32 @@
         <v>357</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="15.75" customHeight="1">
+    <row r="14" spans="1:12" ht="15.75" customHeight="1">
       <c r="A14" s="3"/>
       <c r="B14" s="5"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
-      <c r="E14" s="28"/>
+      <c r="E14" s="27"/>
       <c r="F14" s="5"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
     </row>
-    <row r="15" spans="1:11" ht="15.75" customHeight="1">
+    <row r="15" spans="1:12" ht="15.75" customHeight="1">
       <c r="A15" s="3"/>
       <c r="B15" s="5"/>
       <c r="C15" s="9"/>
       <c r="D15" s="3"/>
-      <c r="E15" s="28"/>
+      <c r="E15" s="27"/>
       <c r="F15" s="5"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
     </row>
-    <row r="16" spans="1:11" ht="15.75" customHeight="1">
+    <row r="16" spans="1:12" ht="15.75" customHeight="1">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="9"/>
       <c r="D16" s="3"/>
-      <c r="E16" s="28"/>
+      <c r="E16" s="27"/>
       <c r="F16" s="5"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
@@ -2826,7 +2833,7 @@
       <c r="B17" s="5"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
-      <c r="E17" s="28"/>
+      <c r="E17" s="27"/>
       <c r="F17" s="5"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
@@ -2844,7 +2851,7 @@
       <c r="D18" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="E18" s="28" t="s">
+      <c r="E18" s="27" t="s">
         <v>71</v>
       </c>
       <c r="F18" s="3" t="s">
@@ -2872,7 +2879,7 @@
       <c r="D19" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="E19" s="28" t="s">
+      <c r="E19" s="27" t="s">
         <v>73</v>
       </c>
       <c r="F19" s="3" t="s">
@@ -2903,7 +2910,7 @@
       <c r="D20" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="E20" s="28" t="s">
+      <c r="E20" s="27" t="s">
         <v>76</v>
       </c>
       <c r="F20" s="3" t="s">
@@ -2932,7 +2939,7 @@
       <c r="D21" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="E21" s="28" t="s">
+      <c r="E21" s="27" t="s">
         <v>80</v>
       </c>
       <c r="F21" s="3" t="s">
@@ -2961,7 +2968,7 @@
       <c r="D22" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="E22" s="28" t="s">
+      <c r="E22" s="27" t="s">
         <v>85</v>
       </c>
       <c r="F22" s="3" t="s">
@@ -2992,7 +2999,7 @@
       <c r="D23" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="E23" s="28" t="s">
+      <c r="E23" s="27" t="s">
         <v>90</v>
       </c>
       <c r="F23" s="3"/>
@@ -3017,7 +3024,7 @@
       <c r="D24" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="E24" s="28" t="s">
+      <c r="E24" s="27" t="s">
         <v>92</v>
       </c>
       <c r="F24" s="3"/>
@@ -3042,7 +3049,7 @@
       <c r="D25" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="E25" s="31" t="s">
+      <c r="E25" s="30" t="s">
         <v>94</v>
       </c>
       <c r="F25" s="5"/>
@@ -3069,7 +3076,7 @@
       <c r="D26" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="E26" s="31" t="s">
+      <c r="E26" s="30" t="s">
         <v>97</v>
       </c>
       <c r="F26" s="5"/>
@@ -3094,7 +3101,7 @@
       <c r="D27" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="E27" s="31" t="s">
+      <c r="E27" s="30" t="s">
         <v>101</v>
       </c>
       <c r="F27" s="5" t="s">
@@ -3119,7 +3126,7 @@
       <c r="D28" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="E28" s="32" t="s">
+      <c r="E28" s="31" t="s">
         <v>103</v>
       </c>
       <c r="I28" s="19" t="s">
@@ -3139,7 +3146,7 @@
       <c r="D29" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="E29" s="32" t="s">
+      <c r="E29" s="31" t="s">
         <v>104</v>
       </c>
       <c r="F29" s="14" t="s">
@@ -3162,7 +3169,7 @@
       <c r="D30" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="E30" s="32" t="s">
+      <c r="E30" s="31" t="s">
         <v>107</v>
       </c>
       <c r="F30" t="s">
@@ -3177,7 +3184,7 @@
     </row>
     <row r="31" spans="1:11" ht="15.75" customHeight="1">
       <c r="C31" s="8"/>
-      <c r="E31" s="33"/>
+      <c r="E31" s="32"/>
     </row>
     <row r="33" spans="1:12" ht="15.75" customHeight="1">
       <c r="A33" s="11" t="s">
@@ -3192,7 +3199,7 @@
       <c r="D33" t="s">
         <v>124</v>
       </c>
-      <c r="E33" s="33" t="s">
+      <c r="E33" s="32" t="s">
         <v>71</v>
       </c>
       <c r="F33" t="s">
@@ -3218,7 +3225,7 @@
       <c r="D34" t="s">
         <v>126</v>
       </c>
-      <c r="E34" s="33" t="s">
+      <c r="E34" s="32" t="s">
         <v>127</v>
       </c>
       <c r="F34" t="s">
@@ -3245,9 +3252,9 @@
         <v>113</v>
       </c>
       <c r="D35" t="s">
-        <v>361</v>
-      </c>
-      <c r="E35" s="33" t="s">
+        <v>360</v>
+      </c>
+      <c r="E35" s="32" t="s">
         <v>125</v>
       </c>
       <c r="F35" t="s">
@@ -3270,10 +3277,10 @@
       <c r="C36" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="D36" s="36" t="s">
-        <v>363</v>
-      </c>
-      <c r="E36" s="33" t="s">
+      <c r="D36" s="35" t="s">
+        <v>362</v>
+      </c>
+      <c r="E36" s="32" t="s">
         <v>129</v>
       </c>
       <c r="F36" t="s">
@@ -3297,9 +3304,9 @@
         <v>114</v>
       </c>
       <c r="D37" t="s">
-        <v>362</v>
-      </c>
-      <c r="E37" s="33" t="s">
+        <v>361</v>
+      </c>
+      <c r="E37" s="32" t="s">
         <v>128</v>
       </c>
       <c r="F37" t="s">
@@ -3317,18 +3324,18 @@
       <c r="K37" s="25" t="s">
         <v>356</v>
       </c>
-      <c r="L37" t="s">
-        <v>358</v>
+      <c r="L37" s="16" t="s">
+        <v>367</v>
       </c>
     </row>
     <row r="38" spans="1:12" ht="15.75" customHeight="1">
       <c r="C38" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="D38" s="36" t="s">
+      <c r="D38" s="35" t="s">
         <v>130</v>
       </c>
-      <c r="E38" s="33" t="s">
+      <c r="E38" s="32" t="s">
         <v>131</v>
       </c>
       <c r="F38" t="s">
@@ -3345,6 +3352,9 @@
       </c>
       <c r="K38" s="25" t="s">
         <v>356</v>
+      </c>
+      <c r="L38" s="16" t="s">
+        <v>367</v>
       </c>
     </row>
     <row r="39" spans="1:12" ht="15.75" customHeight="1">
@@ -3357,7 +3367,7 @@
       <c r="D39" s="24" t="s">
         <v>133</v>
       </c>
-      <c r="E39" s="33" t="s">
+      <c r="E39" s="32" t="s">
         <v>134</v>
       </c>
       <c r="F39" t="s">
@@ -3383,7 +3393,7 @@
       <c r="D40" t="s">
         <v>136</v>
       </c>
-      <c r="E40" s="33" t="s">
+      <c r="E40" s="32" t="s">
         <v>137</v>
       </c>
       <c r="F40" t="s">
@@ -3409,7 +3419,7 @@
       <c r="D41" s="24" t="s">
         <v>138</v>
       </c>
-      <c r="E41" s="33" t="s">
+      <c r="E41" s="32" t="s">
         <v>139</v>
       </c>
       <c r="F41" t="s">
@@ -3435,7 +3445,7 @@
       <c r="D42" t="s">
         <v>140</v>
       </c>
-      <c r="E42" s="33" t="s">
+      <c r="E42" s="32" t="s">
         <v>141</v>
       </c>
       <c r="F42" t="s">
@@ -3464,7 +3474,7 @@
       <c r="D43" s="24" t="s">
         <v>154</v>
       </c>
-      <c r="E43" s="32" t="s">
+      <c r="E43" s="31" t="s">
         <v>155</v>
       </c>
       <c r="F43" t="s">
@@ -3490,7 +3500,7 @@
       <c r="D44" t="s">
         <v>156</v>
       </c>
-      <c r="E44" s="34" t="s">
+      <c r="E44" s="33" t="s">
         <v>157</v>
       </c>
       <c r="F44" s="14" t="s">
@@ -3516,7 +3526,7 @@
       <c r="D45" t="s">
         <v>142</v>
       </c>
-      <c r="E45" s="32" t="s">
+      <c r="E45" s="31" t="s">
         <v>144</v>
       </c>
       <c r="F45" t="s">
@@ -3534,11 +3544,11 @@
     </row>
     <row r="46" spans="1:12" ht="15.75" customHeight="1">
       <c r="C46" s="1"/>
-      <c r="E46" s="33"/>
+      <c r="E46" s="32"/>
     </row>
     <row r="47" spans="1:12" ht="12">
       <c r="C47" s="1"/>
-      <c r="E47" s="33"/>
+      <c r="E47" s="32"/>
     </row>
     <row r="48" spans="1:12" ht="25">
       <c r="A48" s="11" t="s">
@@ -3553,7 +3563,7 @@
       <c r="D48" t="s">
         <v>344</v>
       </c>
-      <c r="E48" s="33" t="s">
+      <c r="E48" s="32" t="s">
         <v>71</v>
       </c>
       <c r="F48" t="s">
@@ -3569,7 +3579,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="15">
+    <row r="49" spans="1:12" ht="15">
       <c r="A49" t="s">
         <v>181</v>
       </c>
@@ -3579,7 +3589,7 @@
       <c r="D49" t="s">
         <v>197</v>
       </c>
-      <c r="E49" s="33" t="s">
+      <c r="E49" s="32" t="s">
         <v>198</v>
       </c>
       <c r="F49" t="s">
@@ -3598,7 +3608,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="25">
+    <row r="50" spans="1:12" ht="25">
       <c r="A50" t="s">
         <v>182</v>
       </c>
@@ -3608,7 +3618,7 @@
       <c r="D50" t="s">
         <v>201</v>
       </c>
-      <c r="E50" s="33" t="s">
+      <c r="E50" s="32" t="s">
         <v>202</v>
       </c>
       <c r="F50" t="s">
@@ -3627,14 +3637,14 @@
         <v>357</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="15">
+    <row r="51" spans="1:12" ht="15">
       <c r="C51" s="8" t="s">
         <v>173</v>
       </c>
       <c r="D51" s="24" t="s">
         <v>204</v>
       </c>
-      <c r="E51" s="33" t="s">
+      <c r="E51" s="32" t="s">
         <v>205</v>
       </c>
       <c r="F51" t="s">
@@ -3653,14 +3663,14 @@
         <v>357</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="15">
+    <row r="52" spans="1:12" ht="15">
       <c r="C52" s="8" t="s">
         <v>174</v>
       </c>
       <c r="D52" t="s">
         <v>208</v>
       </c>
-      <c r="E52" s="33" t="s">
+      <c r="E52" s="32" t="s">
         <v>209</v>
       </c>
       <c r="F52" t="s">
@@ -3679,7 +3689,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="15">
+    <row r="53" spans="1:12" ht="15">
       <c r="B53" t="s">
         <v>187</v>
       </c>
@@ -3689,7 +3699,7 @@
       <c r="D53" t="s">
         <v>183</v>
       </c>
-      <c r="E53" s="33" t="s">
+      <c r="E53" s="32" t="s">
         <v>184</v>
       </c>
       <c r="F53" t="s">
@@ -3707,15 +3717,18 @@
       <c r="K53" s="26" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="54" spans="1:11" ht="15">
+      <c r="L53" s="16" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" ht="15">
       <c r="C54" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="D54" s="36" t="s">
+      <c r="D54" s="35" t="s">
         <v>188</v>
       </c>
-      <c r="E54" s="33" t="s">
+      <c r="E54" s="32" t="s">
         <v>189</v>
       </c>
       <c r="F54" t="s">
@@ -3733,15 +3746,18 @@
       <c r="K54" s="26" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="55" spans="1:11" ht="31" customHeight="1">
+      <c r="L54" s="16" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" ht="31" customHeight="1">
       <c r="C55" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="D55" s="36" t="s">
+      <c r="D55" s="35" t="s">
         <v>192</v>
       </c>
-      <c r="E55" s="38" t="s">
+      <c r="E55" s="37" t="s">
         <v>193</v>
       </c>
       <c r="F55" t="s">
@@ -3759,8 +3775,11 @@
       <c r="K55" s="26" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="56" spans="1:11" ht="25">
+      <c r="L55" s="16" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" ht="25">
       <c r="B56" t="s">
         <v>212</v>
       </c>
@@ -3770,7 +3789,7 @@
       <c r="D56" s="24" t="s">
         <v>213</v>
       </c>
-      <c r="E56" s="33" t="s">
+      <c r="E56" s="32" t="s">
         <v>214</v>
       </c>
       <c r="F56" t="s">
@@ -3789,14 +3808,14 @@
         <v>357</v>
       </c>
     </row>
-    <row r="57" spans="1:11" ht="25">
+    <row r="57" spans="1:12" ht="25">
       <c r="C57" s="8" t="s">
         <v>179</v>
       </c>
       <c r="D57" t="s">
         <v>217</v>
       </c>
-      <c r="E57" s="33" t="s">
+      <c r="E57" s="32" t="s">
         <v>221</v>
       </c>
       <c r="F57" t="s">
@@ -3815,14 +3834,14 @@
         <v>357</v>
       </c>
     </row>
-    <row r="58" spans="1:11" ht="15">
+    <row r="58" spans="1:12" ht="15">
       <c r="C58" s="8" t="s">
         <v>218</v>
       </c>
       <c r="D58" t="s">
         <v>219</v>
       </c>
-      <c r="E58" s="33" t="s">
+      <c r="E58" s="32" t="s">
         <v>220</v>
       </c>
       <c r="F58" t="s">
@@ -3837,20 +3856,23 @@
       <c r="K58" s="26" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="59" spans="1:11" ht="12">
+      <c r="L58" s="16" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" ht="12">
       <c r="C59" s="1"/>
-      <c r="E59" s="33"/>
-    </row>
-    <row r="60" spans="1:11" ht="12">
+      <c r="E59" s="32"/>
+    </row>
+    <row r="60" spans="1:12" ht="12">
       <c r="C60" s="1"/>
-      <c r="E60" s="33"/>
-    </row>
-    <row r="61" spans="1:11" ht="12">
+      <c r="E60" s="32"/>
+    </row>
+    <row r="61" spans="1:12" ht="12">
       <c r="C61" s="1"/>
-      <c r="E61" s="33"/>
-    </row>
-    <row r="62" spans="1:11" ht="25">
+      <c r="E61" s="32"/>
+    </row>
+    <row r="62" spans="1:12" ht="25">
       <c r="A62" s="15" t="s">
         <v>224</v>
       </c>
@@ -3863,7 +3885,7 @@
       <c r="D62" t="s">
         <v>240</v>
       </c>
-      <c r="E62" s="33" t="s">
+      <c r="E62" s="32" t="s">
         <v>71</v>
       </c>
       <c r="F62" t="s">
@@ -3878,8 +3900,11 @@
       <c r="K62" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="63" spans="1:11" ht="37">
+      <c r="L62" s="16" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" ht="37">
       <c r="A63" s="21" t="s">
         <v>226</v>
       </c>
@@ -3889,7 +3914,7 @@
       <c r="D63" s="24" t="s">
         <v>241</v>
       </c>
-      <c r="E63" s="33" t="s">
+      <c r="E63" s="32" t="s">
         <v>242</v>
       </c>
       <c r="F63" t="s">
@@ -3905,7 +3930,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="64" spans="1:11" ht="37">
+    <row r="64" spans="1:12" ht="37">
       <c r="A64" s="21" t="s">
         <v>227</v>
       </c>
@@ -3915,7 +3940,7 @@
       <c r="D64" t="s">
         <v>244</v>
       </c>
-      <c r="E64" s="33" t="s">
+      <c r="E64" s="32" t="s">
         <v>245</v>
       </c>
       <c r="F64" t="s">
@@ -3931,14 +3956,14 @@
         <v>357</v>
       </c>
     </row>
-    <row r="65" spans="1:11" ht="15">
+    <row r="65" spans="1:12" ht="15">
       <c r="C65" s="8" t="s">
         <v>231</v>
       </c>
       <c r="D65" t="s">
         <v>247</v>
       </c>
-      <c r="E65" s="33" t="s">
+      <c r="E65" s="32" t="s">
         <v>248</v>
       </c>
       <c r="F65" t="s">
@@ -3954,7 +3979,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="66" spans="1:11" ht="49">
+    <row r="66" spans="1:12" ht="49">
       <c r="B66" t="s">
         <v>252</v>
       </c>
@@ -3964,7 +3989,7 @@
       <c r="D66" t="s">
         <v>250</v>
       </c>
-      <c r="E66" s="33" t="s">
+      <c r="E66" s="32" t="s">
         <v>251</v>
       </c>
       <c r="F66" t="s">
@@ -3983,14 +4008,14 @@
         <v>357</v>
       </c>
     </row>
-    <row r="67" spans="1:11" ht="24">
+    <row r="67" spans="1:12" ht="24">
       <c r="C67" s="8" t="s">
         <v>233</v>
       </c>
-      <c r="D67" s="36" t="s">
-        <v>365</v>
-      </c>
-      <c r="E67" s="38" t="s">
+      <c r="D67" s="35" t="s">
+        <v>364</v>
+      </c>
+      <c r="E67" s="37" t="s">
         <v>255</v>
       </c>
       <c r="F67" t="s">
@@ -4008,15 +4033,18 @@
       <c r="K67" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="68" spans="1:11" ht="36">
+      <c r="L67" s="16" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" ht="36">
       <c r="C68" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="D68" s="36" t="s">
-        <v>364</v>
-      </c>
-      <c r="E68" s="38" t="s">
+      <c r="D68" s="35" t="s">
+        <v>363</v>
+      </c>
+      <c r="E68" s="37" t="s">
         <v>258</v>
       </c>
       <c r="F68" t="s">
@@ -4034,15 +4062,18 @@
       <c r="K68" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="69" spans="1:11" ht="24">
+      <c r="L68" s="16" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" ht="24">
       <c r="C69" s="8" t="s">
         <v>235</v>
       </c>
-      <c r="D69" s="39" t="s">
-        <v>366</v>
-      </c>
-      <c r="E69" s="38" t="s">
+      <c r="D69" s="35" t="s">
+        <v>365</v>
+      </c>
+      <c r="E69" s="37" t="s">
         <v>260</v>
       </c>
       <c r="F69" t="s">
@@ -4051,8 +4082,8 @@
       <c r="G69" t="s">
         <v>262</v>
       </c>
-      <c r="I69" s="19" t="s">
-        <v>346</v>
+      <c r="I69" s="17" t="s">
+        <v>342</v>
       </c>
       <c r="J69" t="s">
         <v>336</v>
@@ -4060,15 +4091,18 @@
       <c r="K69" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="70" spans="1:11" ht="24">
+      <c r="L69" s="16" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" ht="24">
       <c r="C70" s="8" t="s">
         <v>236</v>
       </c>
-      <c r="D70" s="36" t="s">
+      <c r="D70" s="35" t="s">
         <v>263</v>
       </c>
-      <c r="E70" s="38" t="s">
+      <c r="E70" s="37" t="s">
         <v>265</v>
       </c>
       <c r="F70" t="s">
@@ -4086,18 +4120,21 @@
       <c r="K70" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="71" spans="1:11" ht="24">
+      <c r="L70" s="16" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" ht="24">
       <c r="B71" t="s">
         <v>267</v>
       </c>
       <c r="C71" s="8" t="s">
         <v>237</v>
       </c>
-      <c r="D71" s="36" t="s">
+      <c r="D71" s="35" t="s">
         <v>268</v>
       </c>
-      <c r="E71" s="38" t="s">
+      <c r="E71" s="37" t="s">
         <v>269</v>
       </c>
       <c r="F71" t="s">
@@ -4115,15 +4152,18 @@
       <c r="K71" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="72" spans="1:11" ht="25">
+      <c r="L71" s="16" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" ht="25">
       <c r="C72" s="8" t="s">
         <v>238</v>
       </c>
       <c r="D72" s="24" t="s">
         <v>272</v>
       </c>
-      <c r="E72" s="33" t="s">
+      <c r="E72" s="32" t="s">
         <v>273</v>
       </c>
       <c r="F72" t="s">
@@ -4142,14 +4182,14 @@
         <v>357</v>
       </c>
     </row>
-    <row r="73" spans="1:11" ht="15">
+    <row r="73" spans="1:12" ht="15">
       <c r="C73" s="8" t="s">
         <v>239</v>
       </c>
       <c r="D73" t="s">
         <v>276</v>
       </c>
-      <c r="E73" s="33" t="s">
+      <c r="E73" s="32" t="s">
         <v>277</v>
       </c>
       <c r="F73" t="s">
@@ -4164,20 +4204,23 @@
       <c r="K73" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="74" spans="1:11" ht="12">
+      <c r="L73" s="16" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" ht="12">
       <c r="C74" s="8"/>
-      <c r="E74" s="33"/>
-    </row>
-    <row r="75" spans="1:11" ht="12">
+      <c r="E74" s="32"/>
+    </row>
+    <row r="75" spans="1:12" ht="12">
       <c r="C75" s="1"/>
-      <c r="E75" s="33"/>
-    </row>
-    <row r="76" spans="1:11" ht="12">
+      <c r="E75" s="32"/>
+    </row>
+    <row r="76" spans="1:12" ht="12">
       <c r="C76" s="1"/>
-      <c r="E76" s="33"/>
-    </row>
-    <row r="77" spans="1:11" ht="15">
+      <c r="E76" s="32"/>
+    </row>
+    <row r="77" spans="1:12" ht="15">
       <c r="A77" s="15" t="s">
         <v>278</v>
       </c>
@@ -4190,7 +4233,7 @@
       <c r="D77" t="s">
         <v>294</v>
       </c>
-      <c r="E77" s="33" t="s">
+      <c r="E77" s="32" t="s">
         <v>71</v>
       </c>
       <c r="F77" t="s">
@@ -4205,18 +4248,21 @@
       <c r="K77" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="78" spans="1:11" ht="25">
+      <c r="L77" s="16" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" ht="25">
       <c r="A78" s="21" t="s">
         <v>279</v>
       </c>
       <c r="C78" s="8" t="s">
         <v>282</v>
       </c>
-      <c r="D78" s="36" t="s">
+      <c r="D78" s="35" t="s">
         <v>295</v>
       </c>
-      <c r="E78" s="38" t="s">
+      <c r="E78" s="37" t="s">
         <v>296</v>
       </c>
       <c r="F78" t="s">
@@ -4234,8 +4280,11 @@
       <c r="K78" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="79" spans="1:11" ht="25">
+      <c r="L78" s="16" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" ht="25">
       <c r="A79" s="21" t="s">
         <v>280</v>
       </c>
@@ -4245,7 +4294,7 @@
       <c r="D79" t="s">
         <v>299</v>
       </c>
-      <c r="E79" s="33" t="s">
+      <c r="E79" s="32" t="s">
         <v>300</v>
       </c>
       <c r="F79" t="s">
@@ -4263,8 +4312,11 @@
       <c r="K79" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="80" spans="1:11" ht="25">
+      <c r="L79" s="16" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" ht="25">
       <c r="B80" t="s">
         <v>303</v>
       </c>
@@ -4274,7 +4326,7 @@
       <c r="D80" t="s">
         <v>307</v>
       </c>
-      <c r="E80" s="33" t="s">
+      <c r="E80" s="32" t="s">
         <v>304</v>
       </c>
       <c r="F80" t="s">
@@ -4292,15 +4344,18 @@
       <c r="K80" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="81" spans="2:11" ht="25">
+      <c r="L80" s="16" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="81" spans="2:12" ht="25">
       <c r="C81" s="8" t="s">
         <v>285</v>
       </c>
       <c r="D81" s="24" t="s">
         <v>308</v>
       </c>
-      <c r="E81" s="33" t="s">
+      <c r="E81" s="32" t="s">
         <v>309</v>
       </c>
       <c r="F81" t="s">
@@ -4319,14 +4374,14 @@
         <v>357</v>
       </c>
     </row>
-    <row r="82" spans="2:11" ht="15">
+    <row r="82" spans="2:12" ht="15">
       <c r="C82" s="8" t="s">
         <v>286</v>
       </c>
-      <c r="D82" s="27" t="s">
+      <c r="D82" s="35" t="s">
         <v>311</v>
       </c>
-      <c r="E82" s="38" t="s">
+      <c r="E82" s="37" t="s">
         <v>312</v>
       </c>
       <c r="F82" t="s">
@@ -4335,8 +4390,8 @@
       <c r="G82" t="s">
         <v>314</v>
       </c>
-      <c r="I82" s="19" t="s">
-        <v>346</v>
+      <c r="I82" s="17" t="s">
+        <v>342</v>
       </c>
       <c r="J82" t="s">
         <v>337</v>
@@ -4344,8 +4399,11 @@
       <c r="K82" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="83" spans="2:11" ht="25">
+      <c r="L82" s="16" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="83" spans="2:12" ht="25">
       <c r="B83" t="s">
         <v>343</v>
       </c>
@@ -4355,7 +4413,7 @@
       <c r="D83" s="24" t="s">
         <v>348</v>
       </c>
-      <c r="E83" s="33" t="s">
+      <c r="E83" s="32" t="s">
         <v>317</v>
       </c>
       <c r="F83" t="s">
@@ -4374,14 +4432,14 @@
         <v>357</v>
       </c>
     </row>
-    <row r="84" spans="2:11" ht="37">
+    <row r="84" spans="2:12" ht="37">
       <c r="C84" s="8" t="s">
         <v>288</v>
       </c>
       <c r="D84" t="s">
         <v>351</v>
       </c>
-      <c r="E84" s="33" t="s">
+      <c r="E84" s="32" t="s">
         <v>352</v>
       </c>
       <c r="F84" t="s">
@@ -4399,15 +4457,18 @@
       <c r="K84" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="85" spans="2:11" ht="25">
+      <c r="L84" s="16" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="85" spans="2:12" ht="25">
       <c r="C85" s="8" t="s">
         <v>289</v>
       </c>
       <c r="D85" t="s">
         <v>350</v>
       </c>
-      <c r="E85" s="33" t="s">
+      <c r="E85" s="32" t="s">
         <v>353</v>
       </c>
       <c r="I85" s="18" t="s">
@@ -4416,15 +4477,18 @@
       <c r="K85" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="86" spans="2:11" ht="36">
+      <c r="L85" s="16" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="86" spans="2:12" ht="36">
       <c r="C86" s="8" t="s">
         <v>290</v>
       </c>
-      <c r="D86" s="36" t="s">
+      <c r="D86" s="35" t="s">
         <v>320</v>
       </c>
-      <c r="E86" s="38" t="s">
+      <c r="E86" s="37" t="s">
         <v>321</v>
       </c>
       <c r="F86" t="s">
@@ -4442,8 +4506,11 @@
       <c r="K86" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="87" spans="2:11" ht="25">
+      <c r="L86" s="16" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="87" spans="2:12" ht="25">
       <c r="B87" t="s">
         <v>333</v>
       </c>
@@ -4453,7 +4520,7 @@
       <c r="D87" s="24" t="s">
         <v>324</v>
       </c>
-      <c r="E87" s="33" t="s">
+      <c r="E87" s="32" t="s">
         <v>325</v>
       </c>
       <c r="F87" t="s">
@@ -4472,14 +4539,14 @@
         <v>355</v>
       </c>
     </row>
-    <row r="88" spans="2:11" ht="25">
+    <row r="88" spans="2:12" ht="25">
       <c r="C88" s="8" t="s">
         <v>292</v>
       </c>
       <c r="D88" t="s">
         <v>328</v>
       </c>
-      <c r="E88" s="33" t="s">
+      <c r="E88" s="32" t="s">
         <v>329</v>
       </c>
       <c r="F88" t="s">
@@ -4498,14 +4565,14 @@
         <v>357</v>
       </c>
     </row>
-    <row r="89" spans="2:11" ht="25">
+    <row r="89" spans="2:12" ht="25">
       <c r="C89" s="8" t="s">
         <v>349</v>
       </c>
       <c r="D89" t="s">
         <v>332</v>
       </c>
-      <c r="E89" s="33" t="s">
+      <c r="E89" s="32" t="s">
         <v>334</v>
       </c>
       <c r="F89" t="s">
@@ -4521,25 +4588,25 @@
         <v>355</v>
       </c>
     </row>
-    <row r="90" spans="2:11" ht="12">
+    <row r="90" spans="2:12" ht="12">
       <c r="C90" s="1"/>
     </row>
-    <row r="91" spans="2:11" ht="12">
+    <row r="91" spans="2:12" ht="12">
       <c r="C91" s="1"/>
     </row>
-    <row r="92" spans="2:11" ht="12">
+    <row r="92" spans="2:12" ht="12">
       <c r="C92" s="1"/>
     </row>
-    <row r="93" spans="2:11" ht="12">
+    <row r="93" spans="2:12" ht="12">
       <c r="C93" s="1"/>
     </row>
-    <row r="94" spans="2:11" ht="12">
+    <row r="94" spans="2:12" ht="12">
       <c r="C94" s="1"/>
     </row>
-    <row r="95" spans="2:11" ht="12">
+    <row r="95" spans="2:12" ht="12">
       <c r="C95" s="1"/>
     </row>
-    <row r="96" spans="2:11" ht="12">
+    <row r="96" spans="2:12" ht="12">
       <c r="C96" s="1"/>
     </row>
     <row r="97" spans="3:3" ht="12">

</xml_diff>

<commit_message>
Created an overview of current activities etc
added placeholders for tutorials; added a few pics; fixed some typos.
</commit_message>
<xml_diff>
--- a/fl_course_outline_weeks.xlsx
+++ b/fl_course_outline_weeks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27127"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="27260" tabRatio="500"/>
+    <workbookView xWindow="11960" yWindow="0" windowWidth="51200" windowHeight="27260" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="369">
   <si>
     <t>Week</t>
   </si>
@@ -1132,6 +1132,9 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>Haskell Basics: Expressions and Equations</t>
   </si>
 </sst>
 </file>
@@ -1322,7 +1325,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="338">
+  <cellStyleXfs count="342">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1475,6 +1478,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1768,7 +1775,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="338">
+  <cellStyles count="342">
     <cellStyle name="Bad" xfId="150" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -1937,6 +1944,8 @@
     <cellStyle name="Followed Hyperlink" xfId="333" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="335" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="337" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="339" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="341" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="55" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -2105,6 +2114,8 @@
     <cellStyle name="Hyperlink" xfId="332" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="334" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="336" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="338" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="340" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="151" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -2373,7 +2384,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2384,15 +2395,15 @@
   <dimension ref="A1:L1004"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="Q10" sqref="Q10"/>
+      <selection pane="bottomLeft" activeCell="I84" sqref="I84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="26.5" customWidth="1"/>
-    <col min="2" max="2" width="24" customWidth="1"/>
+    <col min="1" max="1" width="43.83203125" customWidth="1"/>
+    <col min="2" max="2" width="31.83203125" customWidth="1"/>
     <col min="3" max="3" width="7.6640625" customWidth="1"/>
     <col min="4" max="4" width="52" customWidth="1"/>
     <col min="5" max="5" width="38.6640625" style="29" customWidth="1"/>
@@ -2473,7 +2484,9 @@
       <c r="A3" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="B3" s="5"/>
+      <c r="B3" s="5" t="s">
+        <v>368</v>
+      </c>
       <c r="C3" s="6">
         <v>1.2</v>
       </c>
@@ -3550,7 +3563,7 @@
       <c r="C47" s="1"/>
       <c r="E47" s="32"/>
     </row>
-    <row r="48" spans="1:12" ht="25">
+    <row r="48" spans="1:12" ht="15">
       <c r="A48" s="11" t="s">
         <v>180</v>
       </c>
@@ -3872,7 +3885,7 @@
       <c r="C61" s="1"/>
       <c r="E61" s="32"/>
     </row>
-    <row r="62" spans="1:12" ht="25">
+    <row r="62" spans="1:12" ht="15">
       <c r="A62" s="15" t="s">
         <v>224</v>
       </c>
@@ -3904,7 +3917,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="63" spans="1:12" ht="37">
+    <row r="63" spans="1:12" ht="25">
       <c r="A63" s="21" t="s">
         <v>226</v>
       </c>
@@ -3930,7 +3943,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="64" spans="1:12" ht="37">
+    <row r="64" spans="1:12" ht="25">
       <c r="A64" s="21" t="s">
         <v>227</v>
       </c>
@@ -4448,8 +4461,8 @@
       <c r="G84" t="s">
         <v>319</v>
       </c>
-      <c r="I84" s="18" t="s">
-        <v>345</v>
+      <c r="I84" s="17" t="s">
+        <v>342</v>
       </c>
       <c r="J84" t="s">
         <v>338</v>
@@ -4471,8 +4484,8 @@
       <c r="E85" s="32" t="s">
         <v>353</v>
       </c>
-      <c r="I85" s="18" t="s">
-        <v>345</v>
+      <c r="I85" s="17" t="s">
+        <v>342</v>
       </c>
       <c r="K85" t="s">
         <v>356</v>

</xml_diff>

<commit_message>
updated status on Excel tracker
</commit_message>
<xml_diff>
--- a/fl_course_outline_weeks.xlsx
+++ b/fl_course_outline_weeks.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27127"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27226"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="50660" windowHeight="27100" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="25600" windowHeight="14880" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1325,7 +1325,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="394">
+  <cellStyleXfs count="396">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1478,6 +1478,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1827,7 +1829,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="394">
+  <cellStyles count="396">
     <cellStyle name="Bad" xfId="150" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -2024,6 +2026,7 @@
     <cellStyle name="Followed Hyperlink" xfId="389" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="391" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="393" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="395" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="55" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -2220,6 +2223,7 @@
     <cellStyle name="Hyperlink" xfId="388" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="390" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="392" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="394" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="151" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -2488,7 +2492,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2496,12 +2500,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:O1004"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="I11" sqref="I11"/>
+      <selection pane="bottomLeft" activeCell="I56" sqref="I56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -2555,18 +2560,18 @@
       </c>
       <c r="M1">
         <f>SUM(M2:M90)</f>
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N1">
         <f>SUM(N2:N90)</f>
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="O1">
         <f>SUM(O2:O90)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" ht="49" customHeight="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="49" hidden="1" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -2608,7 +2613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="29" customHeight="1">
+    <row r="3" spans="1:15" ht="29" hidden="1" customHeight="1">
       <c r="A3" s="11" t="s">
         <v>55</v>
       </c>
@@ -2656,7 +2661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="15.75" customHeight="1">
+    <row r="4" spans="1:15" ht="15.75" hidden="1" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -2699,7 +2704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="15.75" customHeight="1">
+    <row r="5" spans="1:15" ht="15.75" hidden="1" customHeight="1">
       <c r="A5" s="39" t="s">
         <v>12</v>
       </c>
@@ -2742,7 +2747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="15.75" customHeight="1">
+    <row r="6" spans="1:15" ht="15.75" hidden="1" customHeight="1">
       <c r="A6" s="40"/>
       <c r="B6" s="5"/>
       <c r="C6" s="7">
@@ -2783,7 +2788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="31" customHeight="1">
+    <row r="7" spans="1:15" ht="31" hidden="1" customHeight="1">
       <c r="A7" s="41"/>
       <c r="B7" s="5" t="s">
         <v>18</v>
@@ -2826,7 +2831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="15.75" customHeight="1">
+    <row r="8" spans="1:15" ht="15.75" hidden="1" customHeight="1">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="8" t="s">
@@ -2867,7 +2872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="15.75" customHeight="1">
+    <row r="9" spans="1:15" ht="15.75" hidden="1" customHeight="1">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="8" t="s">
@@ -2908,7 +2913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="15.75" customHeight="1">
+    <row r="10" spans="1:15" ht="15.75" hidden="1" customHeight="1">
       <c r="A10" s="3"/>
       <c r="B10" s="5"/>
       <c r="C10" s="8" t="s">
@@ -3071,7 +3076,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="15.75" customHeight="1">
+    <row r="14" spans="1:15" ht="15.75" hidden="1" customHeight="1">
       <c r="A14" s="3"/>
       <c r="B14" s="5"/>
       <c r="C14" s="3"/>
@@ -3093,7 +3098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="15.75" customHeight="1">
+    <row r="15" spans="1:15" ht="15.75" hidden="1" customHeight="1">
       <c r="A15" s="3"/>
       <c r="B15" s="5"/>
       <c r="C15" s="9"/>
@@ -3115,7 +3120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="15.75" customHeight="1">
+    <row r="16" spans="1:15" ht="15.75" hidden="1" customHeight="1">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="9"/>
@@ -3137,7 +3142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="15.75" customHeight="1">
+    <row r="17" spans="1:15" ht="15.75" hidden="1" customHeight="1">
       <c r="A17" s="3"/>
       <c r="B17" s="5"/>
       <c r="C17" s="3"/>
@@ -3386,8 +3391,8 @@
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
-      <c r="I23" s="19" t="s">
-        <v>346</v>
+      <c r="I23" s="18" t="s">
+        <v>345</v>
       </c>
       <c r="J23" s="16" t="s">
         <v>336</v>
@@ -3401,11 +3406,11 @@
       </c>
       <c r="N23">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O23">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:15" ht="15.75" customHeight="1">
@@ -3499,8 +3504,8 @@
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
-      <c r="I26" s="19" t="s">
-        <v>346</v>
+      <c r="I26" s="18" t="s">
+        <v>345</v>
       </c>
       <c r="J26" s="16" t="s">
         <v>337</v>
@@ -3514,11 +3519,11 @@
       </c>
       <c r="N26">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O26">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:15" ht="15.75" customHeight="1">
@@ -3659,7 +3664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="15.75" customHeight="1">
+    <row r="31" spans="1:15" ht="15.75" hidden="1" customHeight="1">
       <c r="C31" s="8"/>
       <c r="E31" s="32"/>
       <c r="M31">
@@ -3675,7 +3680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:15" ht="15.75" customHeight="1">
+    <row r="32" spans="1:15" ht="15.75" hidden="1" customHeight="1">
       <c r="M32">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3689,7 +3694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:15" ht="15.75" customHeight="1">
+    <row r="33" spans="1:15" ht="15.75" hidden="1" customHeight="1">
       <c r="A33" s="11" t="s">
         <v>347</v>
       </c>
@@ -3730,7 +3735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="15.75" customHeight="1">
+    <row r="34" spans="1:15" ht="15.75" hidden="1" customHeight="1">
       <c r="A34" t="s">
         <v>108</v>
       </c>
@@ -3771,7 +3776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:15" ht="15.75" customHeight="1">
+    <row r="35" spans="1:15" ht="15.75" hidden="1" customHeight="1">
       <c r="A35" t="s">
         <v>109</v>
       </c>
@@ -3812,7 +3817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:15" ht="15.75" customHeight="1">
+    <row r="36" spans="1:15" ht="15.75" hidden="1" customHeight="1">
       <c r="C36" s="8" t="s">
         <v>115</v>
       </c>
@@ -3850,7 +3855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:15" ht="15.75" customHeight="1">
+    <row r="37" spans="1:15" ht="15.75" hidden="1" customHeight="1">
       <c r="C37" s="8" t="s">
         <v>114</v>
       </c>
@@ -3891,7 +3896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:15" ht="15.75" customHeight="1">
+    <row r="38" spans="1:15" ht="15.75" hidden="1" customHeight="1">
       <c r="C38" s="8" t="s">
         <v>116</v>
       </c>
@@ -3951,8 +3956,8 @@
       <c r="G39" t="s">
         <v>165</v>
       </c>
-      <c r="I39" s="19" t="s">
-        <v>346</v>
+      <c r="I39" s="18" t="s">
+        <v>345</v>
       </c>
       <c r="J39" s="16" t="s">
         <v>336</v>
@@ -3966,11 +3971,11 @@
       </c>
       <c r="N39">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O39">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:15" ht="15.75" customHeight="1">
@@ -3989,8 +3994,8 @@
       <c r="G40" t="s">
         <v>166</v>
       </c>
-      <c r="I40" s="17" t="s">
-        <v>342</v>
+      <c r="I40" s="18" t="s">
+        <v>345</v>
       </c>
       <c r="J40" s="16" t="s">
         <v>340</v>
@@ -4000,7 +4005,7 @@
       </c>
       <c r="M40">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N40">
         <f t="shared" si="1"/>
@@ -4008,7 +4013,7 @@
       </c>
       <c r="O40">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:15" ht="15.75" customHeight="1">
@@ -4201,7 +4206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:15" ht="15.75" customHeight="1">
+    <row r="46" spans="1:15" ht="15.75" hidden="1" customHeight="1">
       <c r="C46" s="1"/>
       <c r="E46" s="32"/>
       <c r="M46">
@@ -4217,7 +4222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:15" ht="12">
+    <row r="47" spans="1:15" ht="12" hidden="1">
       <c r="C47" s="1"/>
       <c r="E47" s="32"/>
       <c r="M47">
@@ -4293,8 +4298,8 @@
       <c r="G49" t="s">
         <v>200</v>
       </c>
-      <c r="I49" s="19" t="s">
-        <v>346</v>
+      <c r="I49" s="18" t="s">
+        <v>345</v>
       </c>
       <c r="J49" s="16" t="s">
         <v>336</v>
@@ -4308,11 +4313,11 @@
       </c>
       <c r="N49">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O49">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:15" ht="25">
@@ -4334,8 +4339,8 @@
       <c r="G50" t="s">
         <v>203</v>
       </c>
-      <c r="I50" s="19" t="s">
-        <v>346</v>
+      <c r="I50" s="18" t="s">
+        <v>345</v>
       </c>
       <c r="J50" s="16" t="s">
         <v>336</v>
@@ -4349,11 +4354,11 @@
       </c>
       <c r="N50">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O50">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:15" ht="15">
@@ -4432,7 +4437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:15" ht="15">
+    <row r="53" spans="1:15" ht="15" hidden="1">
       <c r="B53" t="s">
         <v>187</v>
       </c>
@@ -4476,7 +4481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:15" ht="15">
+    <row r="54" spans="1:15" ht="15" hidden="1">
       <c r="C54" s="8" t="s">
         <v>176</v>
       </c>
@@ -4517,7 +4522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:15" ht="31" customHeight="1">
+    <row r="55" spans="1:15" ht="31" hidden="1" customHeight="1">
       <c r="C55" s="8" t="s">
         <v>177</v>
       </c>
@@ -4577,8 +4582,8 @@
       <c r="G56" t="s">
         <v>216</v>
       </c>
-      <c r="I56" s="19" t="s">
-        <v>346</v>
+      <c r="I56" s="18" t="s">
+        <v>345</v>
       </c>
       <c r="J56" s="16" t="s">
         <v>336</v>
@@ -4592,11 +4597,11 @@
       </c>
       <c r="N56">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O56">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:15" ht="25">
@@ -4615,8 +4620,8 @@
       <c r="G57" t="s">
         <v>223</v>
       </c>
-      <c r="I57" s="19" t="s">
-        <v>346</v>
+      <c r="I57" s="18" t="s">
+        <v>345</v>
       </c>
       <c r="J57" t="s">
         <v>337</v>
@@ -4630,14 +4635,14 @@
       </c>
       <c r="N57">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O57">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:15" ht="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" ht="15" hidden="1">
       <c r="C58" s="8" t="s">
         <v>218</v>
       </c>
@@ -4675,7 +4680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:15" ht="12">
+    <row r="59" spans="1:15" ht="12" hidden="1">
       <c r="C59" s="1"/>
       <c r="E59" s="32"/>
       <c r="M59">
@@ -4691,7 +4696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:15" ht="12">
+    <row r="60" spans="1:15" ht="12" hidden="1">
       <c r="C60" s="1"/>
       <c r="E60" s="32"/>
       <c r="M60">
@@ -4707,7 +4712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:15" ht="12">
+    <row r="61" spans="1:15" ht="12" hidden="1">
       <c r="C61" s="1"/>
       <c r="E61" s="32"/>
       <c r="M61">
@@ -4723,7 +4728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:15" ht="15">
+    <row r="62" spans="1:15" ht="15" hidden="1">
       <c r="A62" s="15" t="s">
         <v>224</v>
       </c>
@@ -4919,7 +4924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:15" ht="24">
+    <row r="67" spans="1:15" ht="24" hidden="1">
       <c r="C67" s="8" t="s">
         <v>233</v>
       </c>
@@ -4960,7 +4965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:15" ht="36">
+    <row r="68" spans="1:15" ht="36" hidden="1">
       <c r="C68" s="8" t="s">
         <v>234</v>
       </c>
@@ -5001,7 +5006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:15" ht="24">
+    <row r="69" spans="1:15" ht="24" hidden="1">
       <c r="C69" s="8" t="s">
         <v>235</v>
       </c>
@@ -5042,7 +5047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:15" ht="24">
+    <row r="70" spans="1:15" ht="24" hidden="1">
       <c r="C70" s="8" t="s">
         <v>236</v>
       </c>
@@ -5083,7 +5088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:15" ht="24">
+    <row r="71" spans="1:15" ht="24" hidden="1">
       <c r="B71" t="s">
         <v>267</v>
       </c>
@@ -5165,7 +5170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:15" ht="15">
+    <row r="73" spans="1:15" ht="15" hidden="1">
       <c r="C73" s="8" t="s">
         <v>239</v>
       </c>
@@ -5203,7 +5208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:15" ht="12">
+    <row r="74" spans="1:15" ht="12" hidden="1">
       <c r="C74" s="8"/>
       <c r="E74" s="32"/>
       <c r="M74">
@@ -5219,7 +5224,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:15" ht="12">
+    <row r="75" spans="1:15" ht="12" hidden="1">
       <c r="C75" s="1"/>
       <c r="E75" s="32"/>
       <c r="M75">
@@ -5235,7 +5240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:15" ht="12">
+    <row r="76" spans="1:15" ht="12" hidden="1">
       <c r="C76" s="1"/>
       <c r="E76" s="32"/>
       <c r="M76">
@@ -5251,7 +5256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:15" ht="15">
+    <row r="77" spans="1:15" ht="15" hidden="1">
       <c r="A77" s="15" t="s">
         <v>278</v>
       </c>
@@ -5295,7 +5300,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:15" ht="25">
+    <row r="78" spans="1:15" ht="25" hidden="1">
       <c r="A78" s="21" t="s">
         <v>279</v>
       </c>
@@ -5339,7 +5344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:15" ht="25">
+    <row r="79" spans="1:15" ht="25" hidden="1">
       <c r="A79" s="21" t="s">
         <v>280</v>
       </c>
@@ -5383,7 +5388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:15" ht="25">
+    <row r="80" spans="1:15" ht="25" hidden="1">
       <c r="B80" t="s">
         <v>303</v>
       </c>
@@ -5465,7 +5470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="2:15" ht="15">
+    <row r="82" spans="2:15" ht="15" hidden="1">
       <c r="C82" s="8" t="s">
         <v>286</v>
       </c>
@@ -5547,7 +5552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="2:15" ht="37">
+    <row r="84" spans="2:15" ht="37" hidden="1">
       <c r="C84" s="8" t="s">
         <v>288</v>
       </c>
@@ -5588,7 +5593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="2:15" ht="25">
+    <row r="85" spans="2:15" ht="25" hidden="1">
       <c r="C85" s="8" t="s">
         <v>289</v>
       </c>
@@ -5620,7 +5625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="2:15" ht="36">
+    <row r="86" spans="2:15" ht="36" hidden="1">
       <c r="C86" s="8" t="s">
         <v>290</v>
       </c>
@@ -5661,7 +5666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="2:15" ht="25">
+    <row r="87" spans="2:15" ht="25" hidden="1">
       <c r="B87" t="s">
         <v>333</v>
       </c>
@@ -5740,7 +5745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="2:15" ht="25">
+    <row r="89" spans="2:15" ht="25" hidden="1">
       <c r="C89" s="8" t="s">
         <v>349</v>
       </c>
@@ -8513,7 +8518,13 @@
     <row r="1003" spans="3:3" ht="12"/>
     <row r="1004" spans="3:3" ht="12"/>
   </sheetData>
-  <autoFilter ref="A1:K89"/>
+  <autoFilter ref="A1:K89">
+    <filterColumn colId="10">
+      <filters>
+        <filter val="J"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="1">
     <mergeCell ref="A5:A7"/>
   </mergeCells>

</xml_diff>

<commit_message>
updated FL spreadsheet tracker
</commit_message>
<xml_diff>
--- a/fl_course_outline_weeks.xlsx
+++ b/fl_course_outline_weeks.xlsx
@@ -2500,7 +2500,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2511,7 +2511,7 @@
   <dimension ref="A1:O1004"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
     </sheetView>

</xml_diff>

<commit_message>
updated status tracker spreadsheet
</commit_message>
<xml_diff>
--- a/fl_course_outline_weeks.xlsx
+++ b/fl_course_outline_weeks.xlsx
@@ -1325,7 +1325,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="400">
+  <cellStyleXfs count="402">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1478,6 +1478,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1833,7 +1835,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="400">
+  <cellStyles count="402">
     <cellStyle name="Bad" xfId="150" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -2033,6 +2035,7 @@
     <cellStyle name="Followed Hyperlink" xfId="395" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="397" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="399" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="401" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="55" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -2232,6 +2235,7 @@
     <cellStyle name="Hyperlink" xfId="394" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="396" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="398" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="400" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="151" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -2500,7 +2504,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2511,9 +2515,9 @@
   <dimension ref="A1:O1004"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
+      <selection pane="bottomLeft" activeCell="I44" sqref="I44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -2567,7 +2571,7 @@
       </c>
       <c r="M1">
         <f>SUM(M2:M90)</f>
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N1">
         <f>SUM(N2:N90)</f>
@@ -2575,7 +2579,7 @@
       </c>
       <c r="O1">
         <f>SUM(O2:O90)</f>
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="49" customHeight="1">
@@ -4156,8 +4160,8 @@
       <c r="G44" s="14" t="s">
         <v>159</v>
       </c>
-      <c r="I44" s="20" t="s">
-        <v>345</v>
+      <c r="I44" s="17" t="s">
+        <v>342</v>
       </c>
       <c r="J44" s="16" t="s">
         <v>338</v>
@@ -4167,7 +4171,7 @@
       </c>
       <c r="M44">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N44">
         <f t="shared" si="1"/>
@@ -4175,7 +4179,7 @@
       </c>
       <c r="O44">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:15" ht="15.75" customHeight="1">

</xml_diff>

<commit_message>
finished week 1 - updated tracker spreadsheet
</commit_message>
<xml_diff>
--- a/fl_course_outline_weeks.xlsx
+++ b/fl_course_outline_weeks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27226"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-20" windowWidth="33660" windowHeight="22420" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14880" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1325,7 +1325,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="402">
+  <cellStyleXfs count="406">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1478,6 +1478,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1835,7 +1839,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="402">
+  <cellStyles count="406">
     <cellStyle name="Bad" xfId="150" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -2036,6 +2040,8 @@
     <cellStyle name="Followed Hyperlink" xfId="397" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="399" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="401" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="403" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="405" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="55" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -2236,6 +2242,8 @@
     <cellStyle name="Hyperlink" xfId="396" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="398" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="400" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="402" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="404" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="151" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -2504,7 +2512,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2514,10 +2522,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O1004"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="I44" sqref="I44"/>
+      <selection pane="bottomLeft" activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -2571,7 +2579,7 @@
       </c>
       <c r="M1">
         <f>SUM(M2:M90)</f>
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="N1">
         <f>SUM(N2:N90)</f>
@@ -2579,7 +2587,7 @@
       </c>
       <c r="O1">
         <f>SUM(O2:O90)</f>
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="49" customHeight="1">
@@ -2986,8 +2994,8 @@
         <v>52</v>
       </c>
       <c r="H11" s="3"/>
-      <c r="I11" s="20" t="s">
-        <v>345</v>
+      <c r="I11" s="17" t="s">
+        <v>342</v>
       </c>
       <c r="J11" s="16" t="s">
         <v>338</v>
@@ -2997,7 +3005,7 @@
       </c>
       <c r="M11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N11">
         <f t="shared" si="1"/>
@@ -3005,7 +3013,7 @@
       </c>
       <c r="O11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="15.75" customHeight="1">
@@ -3027,8 +3035,8 @@
         <v>53</v>
       </c>
       <c r="H12" s="3"/>
-      <c r="I12" s="18" t="s">
-        <v>345</v>
+      <c r="I12" s="17" t="s">
+        <v>342</v>
       </c>
       <c r="J12" s="16" t="s">
         <v>339</v>
@@ -3038,7 +3046,7 @@
       </c>
       <c r="M12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N12">
         <f t="shared" si="1"/>
@@ -3046,7 +3054,7 @@
       </c>
       <c r="O12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="15.75" customHeight="1">
@@ -3068,15 +3076,15 @@
         <v>44</v>
       </c>
       <c r="H13" s="3"/>
-      <c r="I13" s="18" t="s">
-        <v>345</v>
+      <c r="I13" s="17" t="s">
+        <v>342</v>
       </c>
       <c r="K13" s="16" t="s">
         <v>357</v>
       </c>
       <c r="M13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N13">
         <f t="shared" si="1"/>
@@ -3084,7 +3092,7 @@
       </c>
       <c r="O13">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="15.75" customHeight="1">

</xml_diff>

<commit_message>
updated IO and Monads article
</commit_message>
<xml_diff>
--- a/fl_course_outline_weeks.xlsx
+++ b/fl_course_outline_weeks.xlsx
@@ -1325,7 +1325,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="408">
+  <cellStyleXfs count="412">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1478,6 +1478,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1841,7 +1845,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="408">
+  <cellStyles count="412">
     <cellStyle name="Bad" xfId="150" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -2045,6 +2049,8 @@
     <cellStyle name="Followed Hyperlink" xfId="403" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="405" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="407" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="409" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="411" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="55" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -2248,6 +2254,8 @@
     <cellStyle name="Hyperlink" xfId="402" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="404" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="406" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="408" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="410" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="151" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -2516,7 +2524,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2526,10 +2534,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O1004"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="E28" sqref="E28"/>
+      <selection pane="bottomLeft" activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -2583,7 +2591,7 @@
       </c>
       <c r="M1">
         <f>SUM(M2:M90)</f>
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="N1">
         <f>SUM(N2:N90)</f>
@@ -2591,7 +2599,7 @@
       </c>
       <c r="O1">
         <f>SUM(O2:O90)</f>
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="49" customHeight="1">
@@ -3414,8 +3422,8 @@
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
-      <c r="I23" s="18" t="s">
-        <v>345</v>
+      <c r="I23" s="17" t="s">
+        <v>342</v>
       </c>
       <c r="J23" s="16" t="s">
         <v>336</v>
@@ -3425,7 +3433,7 @@
       </c>
       <c r="M23">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N23">
         <f t="shared" si="1"/>
@@ -3433,7 +3441,7 @@
       </c>
       <c r="O23">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:15" ht="15.75" customHeight="1">
@@ -3451,8 +3459,8 @@
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
-      <c r="I24" s="17" t="s">
-        <v>342</v>
+      <c r="I24" s="18" t="s">
+        <v>345</v>
       </c>
       <c r="J24" s="16" t="s">
         <v>337</v>
@@ -3462,7 +3470,7 @@
       </c>
       <c r="M24">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N24">
         <f t="shared" si="1"/>
@@ -3470,7 +3478,7 @@
       </c>
       <c r="O24">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:15" ht="15.75" customHeight="1">
@@ -3488,8 +3496,8 @@
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
-      <c r="I25" s="18" t="s">
-        <v>345</v>
+      <c r="I25" s="17" t="s">
+        <v>342</v>
       </c>
       <c r="J25" s="16" t="s">
         <v>336</v>
@@ -3499,7 +3507,7 @@
       </c>
       <c r="M25">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N25">
         <f t="shared" si="1"/>
@@ -3507,7 +3515,7 @@
       </c>
       <c r="O25">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:15" ht="15.75" customHeight="1">

</xml_diff>

<commit_message>
update status tracker spreadsheet
</commit_message>
<xml_diff>
--- a/fl_course_outline_weeks.xlsx
+++ b/fl_course_outline_weeks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27322"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="9300" yWindow="480" windowWidth="37360" windowHeight="18960" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14880" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1338,7 +1338,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="450">
+  <cellStyleXfs count="452">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1491,6 +1491,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1896,7 +1898,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="450">
+  <cellStyles count="452">
     <cellStyle name="Bad" xfId="150" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -2121,6 +2123,7 @@
     <cellStyle name="Followed Hyperlink" xfId="445" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="447" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="449" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="451" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="55" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -2345,6 +2348,7 @@
     <cellStyle name="Hyperlink" xfId="444" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="446" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="448" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="450" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="151" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -2613,7 +2617,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2623,10 +2627,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O1005"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="I73" sqref="I73"/>
+      <selection pane="bottomLeft" activeCell="I51" sqref="I51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -2680,7 +2684,7 @@
       </c>
       <c r="M1">
         <f>SUM(M2:M91)</f>
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="N1">
         <f>SUM(N2:N91)</f>
@@ -2688,7 +2692,7 @@
       </c>
       <c r="O1">
         <f>SUM(O2:O91)</f>
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="49" customHeight="1">
@@ -4459,8 +4463,8 @@
       <c r="G50" t="s">
         <v>203</v>
       </c>
-      <c r="I50" s="18" t="s">
-        <v>344</v>
+      <c r="I50" s="17" t="s">
+        <v>341</v>
       </c>
       <c r="J50" s="16" t="s">
         <v>335</v>
@@ -4470,7 +4474,7 @@
       </c>
       <c r="M50">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N50">
         <f t="shared" si="1"/>
@@ -4478,7 +4482,7 @@
       </c>
       <c r="O50">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:15" ht="15">
@@ -4497,8 +4501,8 @@
       <c r="G51" t="s">
         <v>207</v>
       </c>
-      <c r="I51" s="20" t="s">
-        <v>344</v>
+      <c r="I51" s="17" t="s">
+        <v>341</v>
       </c>
       <c r="J51" s="16" t="s">
         <v>335</v>
@@ -4508,7 +4512,7 @@
       </c>
       <c r="M51">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N51">
         <f t="shared" si="1"/>
@@ -4516,7 +4520,7 @@
       </c>
       <c r="O51">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:15" ht="15">

</xml_diff>

<commit_message>
added infinity quiz (week 5)
</commit_message>
<xml_diff>
--- a/fl_course_outline_weeks.xlsx
+++ b/fl_course_outline_weeks.xlsx
@@ -1150,7 +1150,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1226,8 +1226,14 @@
       <sz val="8"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1265,6 +1271,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -1338,7 +1350,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="454">
+  <cellStyleXfs count="458">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1793,8 +1805,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1899,8 +1915,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="454">
+  <cellStyles count="458">
     <cellStyle name="Bad" xfId="150" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -2127,6 +2146,8 @@
     <cellStyle name="Followed Hyperlink" xfId="449" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="451" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="453" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="455" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="457" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="55" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -2353,6 +2374,8 @@
     <cellStyle name="Hyperlink" xfId="448" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="450" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="452" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="454" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="456" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="151" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -2632,9 +2655,9 @@
   <dimension ref="A1:O1005"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="I57" sqref="I57"/>
+      <selection pane="bottomLeft" activeCell="I58" sqref="I58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -2688,7 +2711,7 @@
       </c>
       <c r="M1">
         <f>SUM(M2:M91)</f>
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="N1">
         <f>SUM(N2:N91)</f>
@@ -2696,7 +2719,7 @@
       </c>
       <c r="O1">
         <f>SUM(O2:O91)</f>
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="49" customHeight="1">
@@ -4748,7 +4771,7 @@
       <c r="G57" t="s">
         <v>223</v>
       </c>
-      <c r="I57" s="17" t="s">
+      <c r="I57" s="42" t="s">
         <v>341</v>
       </c>
       <c r="J57" t="s">
@@ -4780,7 +4803,7 @@
       <c r="E58" s="32" t="s">
         <v>371</v>
       </c>
-      <c r="I58" s="17" t="s">
+      <c r="I58" s="42" t="s">
         <v>341</v>
       </c>
       <c r="J58" s="16" t="s">
@@ -4974,8 +4997,8 @@
       <c r="F65" t="s">
         <v>246</v>
       </c>
-      <c r="I65" s="18" t="s">
-        <v>344</v>
+      <c r="I65" s="17" t="s">
+        <v>341</v>
       </c>
       <c r="J65" t="s">
         <v>339</v>
@@ -4985,7 +5008,7 @@
       </c>
       <c r="M65">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N65">
         <f t="shared" si="1"/>
@@ -4993,7 +5016,7 @@
       </c>
       <c r="O65">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:15" ht="15">

</xml_diff>

<commit_message>
updated status tracker (nearly finished videos!)
</commit_message>
<xml_diff>
--- a/fl_course_outline_weeks.xlsx
+++ b/fl_course_outline_weeks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27322"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="0" windowWidth="25600" windowHeight="14880" tabRatio="500"/>
+    <workbookView xWindow="6940" yWindow="200" windowWidth="34520" windowHeight="19580" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1350,7 +1350,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="470">
+  <cellStyleXfs count="478">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1503,6 +1503,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1931,7 +1939,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="470">
+  <cellStyles count="478">
     <cellStyle name="Bad" xfId="150" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -2166,6 +2174,10 @@
     <cellStyle name="Followed Hyperlink" xfId="465" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="467" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="469" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="471" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="473" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="475" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="477" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="55" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -2400,6 +2412,10 @@
     <cellStyle name="Hyperlink" xfId="464" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="466" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="468" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="470" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="472" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="474" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="476" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="151" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -2668,7 +2684,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2678,10 +2694,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O1005"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="I73" sqref="I73"/>
+      <selection pane="bottomLeft" activeCell="I82" sqref="I82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -2735,15 +2751,15 @@
       </c>
       <c r="M1">
         <f>SUM(M2:M91)</f>
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="N1">
         <f>SUM(N2:N91)</f>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="O1">
         <f>SUM(O2:O91)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="49" customHeight="1">
@@ -3527,8 +3543,8 @@
         <v>54</v>
       </c>
       <c r="H22" s="3"/>
-      <c r="I22" s="19" t="s">
-        <v>345</v>
+      <c r="I22" s="17" t="s">
+        <v>341</v>
       </c>
       <c r="J22" s="16" t="s">
         <v>336</v>
@@ -3538,11 +3554,11 @@
       </c>
       <c r="M22">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N22">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O22">
         <f t="shared" si="2"/>
@@ -5643,8 +5659,8 @@
       <c r="G82" t="s">
         <v>301</v>
       </c>
-      <c r="I82" s="19" t="s">
-        <v>345</v>
+      <c r="I82" s="20" t="s">
+        <v>344</v>
       </c>
       <c r="J82" t="s">
         <v>335</v>
@@ -5658,11 +5674,11 @@
       </c>
       <c r="N82">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O82">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83" spans="2:15" ht="15">
@@ -5725,8 +5741,8 @@
       <c r="G84" t="s">
         <v>315</v>
       </c>
-      <c r="I84" s="19" t="s">
-        <v>345</v>
+      <c r="I84" s="20" t="s">
+        <v>344</v>
       </c>
       <c r="J84" t="s">
         <v>335</v>
@@ -5740,11 +5756,11 @@
       </c>
       <c r="N84">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O84">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="85" spans="2:15" ht="37">
@@ -5918,8 +5934,8 @@
       <c r="G89" t="s">
         <v>334</v>
       </c>
-      <c r="I89" s="19" t="s">
-        <v>345</v>
+      <c r="I89" s="17" t="s">
+        <v>341</v>
       </c>
       <c r="J89" t="s">
         <v>338</v>
@@ -5929,11 +5945,11 @@
       </c>
       <c r="M89">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N89">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O89">
         <f t="shared" si="5"/>

</xml_diff>

<commit_message>
updated status tracker spreadsheet - nearly all finished!
</commit_message>
<xml_diff>
--- a/fl_course_outline_weeks.xlsx
+++ b/fl_course_outline_weeks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27322"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6940" yWindow="200" windowWidth="34520" windowHeight="19580" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14880" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1350,7 +1350,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="482">
+  <cellStyleXfs count="484">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1503,6 +1503,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1943,7 +1945,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="482">
+  <cellStyles count="484">
     <cellStyle name="Bad" xfId="150" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -2184,6 +2186,7 @@
     <cellStyle name="Followed Hyperlink" xfId="477" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="479" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="481" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="483" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="55" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -2424,6 +2427,7 @@
     <cellStyle name="Hyperlink" xfId="476" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="478" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="480" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="482" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="151" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -2692,7 +2696,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2702,10 +2706,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O1005"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="I82" sqref="I82"/>
+      <selection pane="bottomLeft" activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -2759,7 +2763,7 @@
       </c>
       <c r="M1">
         <f>SUM(M2:M91)</f>
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="N1">
         <f>SUM(N2:N91)</f>
@@ -2767,7 +2771,7 @@
       </c>
       <c r="O1">
         <f>SUM(O2:O91)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="49" customHeight="1">
@@ -3510,8 +3514,8 @@
         <v>50</v>
       </c>
       <c r="H21" s="3"/>
-      <c r="I21" s="17" t="s">
-        <v>341</v>
+      <c r="I21" s="18" t="s">
+        <v>344</v>
       </c>
       <c r="J21" s="16" t="s">
         <v>336</v>
@@ -3521,7 +3525,7 @@
       </c>
       <c r="M21">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N21">
         <f t="shared" si="1"/>
@@ -3529,7 +3533,7 @@
       </c>
       <c r="O21">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:15" ht="15.75" customHeight="1">

</xml_diff>